<commit_message>
Update calendar dates for 2022
</commit_message>
<xml_diff>
--- a/data/calendar-dates.xlsx
+++ b/data/calendar-dates.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\deqhq1\WQ-Share\Harmful Algal Blooms Coordination Team\HAB_Shiny_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821C519A-B3DF-4F1D-BA18-F7C2C1E91872}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="calendar-dates" sheetId="1" r:id="rId1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -837,10 +838,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2193"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C2558"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -24970,6 +24973,4021 @@
         <v>44561</v>
       </c>
     </row>
+    <row r="2194" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2194">
+        <v>2022</v>
+      </c>
+      <c r="B2194">
+        <v>1</v>
+      </c>
+      <c r="C2194" s="1">
+        <v>44562</v>
+      </c>
+    </row>
+    <row r="2195" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2195">
+        <v>2022</v>
+      </c>
+      <c r="B2195">
+        <v>1</v>
+      </c>
+      <c r="C2195" s="1">
+        <v>44563</v>
+      </c>
+    </row>
+    <row r="2196" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2196">
+        <v>2022</v>
+      </c>
+      <c r="B2196">
+        <v>1</v>
+      </c>
+      <c r="C2196" s="1">
+        <v>44564</v>
+      </c>
+    </row>
+    <row r="2197" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2197">
+        <v>2022</v>
+      </c>
+      <c r="B2197">
+        <v>1</v>
+      </c>
+      <c r="C2197" s="1">
+        <v>44565</v>
+      </c>
+    </row>
+    <row r="2198" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2198">
+        <v>2022</v>
+      </c>
+      <c r="B2198">
+        <v>1</v>
+      </c>
+      <c r="C2198" s="1">
+        <v>44566</v>
+      </c>
+    </row>
+    <row r="2199" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2199">
+        <v>2022</v>
+      </c>
+      <c r="B2199">
+        <v>1</v>
+      </c>
+      <c r="C2199" s="1">
+        <v>44567</v>
+      </c>
+    </row>
+    <row r="2200" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2200">
+        <v>2022</v>
+      </c>
+      <c r="B2200">
+        <v>1</v>
+      </c>
+      <c r="C2200" s="1">
+        <v>44568</v>
+      </c>
+    </row>
+    <row r="2201" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2201">
+        <v>2022</v>
+      </c>
+      <c r="B2201">
+        <v>1</v>
+      </c>
+      <c r="C2201" s="1">
+        <v>44569</v>
+      </c>
+    </row>
+    <row r="2202" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2202">
+        <v>2022</v>
+      </c>
+      <c r="B2202">
+        <v>1</v>
+      </c>
+      <c r="C2202" s="1">
+        <v>44570</v>
+      </c>
+    </row>
+    <row r="2203" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2203">
+        <v>2022</v>
+      </c>
+      <c r="B2203">
+        <v>1</v>
+      </c>
+      <c r="C2203" s="1">
+        <v>44571</v>
+      </c>
+    </row>
+    <row r="2204" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2204">
+        <v>2022</v>
+      </c>
+      <c r="B2204">
+        <v>1</v>
+      </c>
+      <c r="C2204" s="1">
+        <v>44572</v>
+      </c>
+    </row>
+    <row r="2205" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2205">
+        <v>2022</v>
+      </c>
+      <c r="B2205">
+        <v>1</v>
+      </c>
+      <c r="C2205" s="1">
+        <v>44573</v>
+      </c>
+    </row>
+    <row r="2206" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2206">
+        <v>2022</v>
+      </c>
+      <c r="B2206">
+        <v>1</v>
+      </c>
+      <c r="C2206" s="1">
+        <v>44574</v>
+      </c>
+    </row>
+    <row r="2207" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2207">
+        <v>2022</v>
+      </c>
+      <c r="B2207">
+        <v>1</v>
+      </c>
+      <c r="C2207" s="1">
+        <v>44575</v>
+      </c>
+    </row>
+    <row r="2208" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2208">
+        <v>2022</v>
+      </c>
+      <c r="B2208">
+        <v>1</v>
+      </c>
+      <c r="C2208" s="1">
+        <v>44576</v>
+      </c>
+    </row>
+    <row r="2209" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2209">
+        <v>2022</v>
+      </c>
+      <c r="B2209">
+        <v>1</v>
+      </c>
+      <c r="C2209" s="1">
+        <v>44577</v>
+      </c>
+    </row>
+    <row r="2210" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2210">
+        <v>2022</v>
+      </c>
+      <c r="B2210">
+        <v>1</v>
+      </c>
+      <c r="C2210" s="1">
+        <v>44578</v>
+      </c>
+    </row>
+    <row r="2211" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2211">
+        <v>2022</v>
+      </c>
+      <c r="B2211">
+        <v>1</v>
+      </c>
+      <c r="C2211" s="1">
+        <v>44579</v>
+      </c>
+    </row>
+    <row r="2212" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2212">
+        <v>2022</v>
+      </c>
+      <c r="B2212">
+        <v>1</v>
+      </c>
+      <c r="C2212" s="1">
+        <v>44580</v>
+      </c>
+    </row>
+    <row r="2213" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2213">
+        <v>2022</v>
+      </c>
+      <c r="B2213">
+        <v>1</v>
+      </c>
+      <c r="C2213" s="1">
+        <v>44581</v>
+      </c>
+    </row>
+    <row r="2214" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2214">
+        <v>2022</v>
+      </c>
+      <c r="B2214">
+        <v>1</v>
+      </c>
+      <c r="C2214" s="1">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="2215" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2215">
+        <v>2022</v>
+      </c>
+      <c r="B2215">
+        <v>1</v>
+      </c>
+      <c r="C2215" s="1">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="2216" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2216">
+        <v>2022</v>
+      </c>
+      <c r="B2216">
+        <v>1</v>
+      </c>
+      <c r="C2216" s="1">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="2217" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2217">
+        <v>2022</v>
+      </c>
+      <c r="B2217">
+        <v>1</v>
+      </c>
+      <c r="C2217" s="1">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="2218" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2218">
+        <v>2022</v>
+      </c>
+      <c r="B2218">
+        <v>1</v>
+      </c>
+      <c r="C2218" s="1">
+        <v>44586</v>
+      </c>
+    </row>
+    <row r="2219" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2219">
+        <v>2022</v>
+      </c>
+      <c r="B2219">
+        <v>1</v>
+      </c>
+      <c r="C2219" s="1">
+        <v>44587</v>
+      </c>
+    </row>
+    <row r="2220" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2220">
+        <v>2022</v>
+      </c>
+      <c r="B2220">
+        <v>1</v>
+      </c>
+      <c r="C2220" s="1">
+        <v>44588</v>
+      </c>
+    </row>
+    <row r="2221" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2221">
+        <v>2022</v>
+      </c>
+      <c r="B2221">
+        <v>1</v>
+      </c>
+      <c r="C2221" s="1">
+        <v>44589</v>
+      </c>
+    </row>
+    <row r="2222" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2222">
+        <v>2022</v>
+      </c>
+      <c r="B2222">
+        <v>1</v>
+      </c>
+      <c r="C2222" s="1">
+        <v>44590</v>
+      </c>
+    </row>
+    <row r="2223" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2223">
+        <v>2022</v>
+      </c>
+      <c r="B2223">
+        <v>1</v>
+      </c>
+      <c r="C2223" s="1">
+        <v>44591</v>
+      </c>
+    </row>
+    <row r="2224" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2224">
+        <v>2022</v>
+      </c>
+      <c r="B2224">
+        <v>1</v>
+      </c>
+      <c r="C2224" s="1">
+        <v>44592</v>
+      </c>
+    </row>
+    <row r="2225" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2225">
+        <v>2022</v>
+      </c>
+      <c r="B2225">
+        <v>1</v>
+      </c>
+      <c r="C2225" s="1">
+        <v>44593</v>
+      </c>
+    </row>
+    <row r="2226" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2226">
+        <v>2022</v>
+      </c>
+      <c r="B2226">
+        <v>1</v>
+      </c>
+      <c r="C2226" s="1">
+        <v>44594</v>
+      </c>
+    </row>
+    <row r="2227" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2227">
+        <v>2022</v>
+      </c>
+      <c r="B2227">
+        <v>1</v>
+      </c>
+      <c r="C2227" s="1">
+        <v>44595</v>
+      </c>
+    </row>
+    <row r="2228" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2228">
+        <v>2022</v>
+      </c>
+      <c r="B2228">
+        <v>1</v>
+      </c>
+      <c r="C2228" s="1">
+        <v>44596</v>
+      </c>
+    </row>
+    <row r="2229" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2229">
+        <v>2022</v>
+      </c>
+      <c r="B2229">
+        <v>1</v>
+      </c>
+      <c r="C2229" s="1">
+        <v>44597</v>
+      </c>
+    </row>
+    <row r="2230" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2230">
+        <v>2022</v>
+      </c>
+      <c r="B2230">
+        <v>1</v>
+      </c>
+      <c r="C2230" s="1">
+        <v>44598</v>
+      </c>
+    </row>
+    <row r="2231" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2231">
+        <v>2022</v>
+      </c>
+      <c r="B2231">
+        <v>1</v>
+      </c>
+      <c r="C2231" s="1">
+        <v>44599</v>
+      </c>
+    </row>
+    <row r="2232" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2232">
+        <v>2022</v>
+      </c>
+      <c r="B2232">
+        <v>1</v>
+      </c>
+      <c r="C2232" s="1">
+        <v>44600</v>
+      </c>
+    </row>
+    <row r="2233" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2233">
+        <v>2022</v>
+      </c>
+      <c r="B2233">
+        <v>1</v>
+      </c>
+      <c r="C2233" s="1">
+        <v>44601</v>
+      </c>
+    </row>
+    <row r="2234" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2234">
+        <v>2022</v>
+      </c>
+      <c r="B2234">
+        <v>1</v>
+      </c>
+      <c r="C2234" s="1">
+        <v>44602</v>
+      </c>
+    </row>
+    <row r="2235" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2235">
+        <v>2022</v>
+      </c>
+      <c r="B2235">
+        <v>1</v>
+      </c>
+      <c r="C2235" s="1">
+        <v>44603</v>
+      </c>
+    </row>
+    <row r="2236" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2236">
+        <v>2022</v>
+      </c>
+      <c r="B2236">
+        <v>1</v>
+      </c>
+      <c r="C2236" s="1">
+        <v>44604</v>
+      </c>
+    </row>
+    <row r="2237" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2237">
+        <v>2022</v>
+      </c>
+      <c r="B2237">
+        <v>1</v>
+      </c>
+      <c r="C2237" s="1">
+        <v>44605</v>
+      </c>
+    </row>
+    <row r="2238" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2238">
+        <v>2022</v>
+      </c>
+      <c r="B2238">
+        <v>1</v>
+      </c>
+      <c r="C2238" s="1">
+        <v>44606</v>
+      </c>
+    </row>
+    <row r="2239" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2239">
+        <v>2022</v>
+      </c>
+      <c r="B2239">
+        <v>1</v>
+      </c>
+      <c r="C2239" s="1">
+        <v>44607</v>
+      </c>
+    </row>
+    <row r="2240" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2240">
+        <v>2022</v>
+      </c>
+      <c r="B2240">
+        <v>1</v>
+      </c>
+      <c r="C2240" s="1">
+        <v>44608</v>
+      </c>
+    </row>
+    <row r="2241" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2241">
+        <v>2022</v>
+      </c>
+      <c r="B2241">
+        <v>1</v>
+      </c>
+      <c r="C2241" s="1">
+        <v>44609</v>
+      </c>
+    </row>
+    <row r="2242" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2242">
+        <v>2022</v>
+      </c>
+      <c r="B2242">
+        <v>1</v>
+      </c>
+      <c r="C2242" s="1">
+        <v>44610</v>
+      </c>
+    </row>
+    <row r="2243" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2243">
+        <v>2022</v>
+      </c>
+      <c r="B2243">
+        <v>1</v>
+      </c>
+      <c r="C2243" s="1">
+        <v>44611</v>
+      </c>
+    </row>
+    <row r="2244" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2244">
+        <v>2022</v>
+      </c>
+      <c r="B2244">
+        <v>1</v>
+      </c>
+      <c r="C2244" s="1">
+        <v>44612</v>
+      </c>
+    </row>
+    <row r="2245" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2245">
+        <v>2022</v>
+      </c>
+      <c r="B2245">
+        <v>1</v>
+      </c>
+      <c r="C2245" s="1">
+        <v>44613</v>
+      </c>
+    </row>
+    <row r="2246" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2246">
+        <v>2022</v>
+      </c>
+      <c r="B2246">
+        <v>1</v>
+      </c>
+      <c r="C2246" s="1">
+        <v>44614</v>
+      </c>
+    </row>
+    <row r="2247" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2247">
+        <v>2022</v>
+      </c>
+      <c r="B2247">
+        <v>1</v>
+      </c>
+      <c r="C2247" s="1">
+        <v>44615</v>
+      </c>
+    </row>
+    <row r="2248" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2248">
+        <v>2022</v>
+      </c>
+      <c r="B2248">
+        <v>1</v>
+      </c>
+      <c r="C2248" s="1">
+        <v>44616</v>
+      </c>
+    </row>
+    <row r="2249" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2249">
+        <v>2022</v>
+      </c>
+      <c r="B2249">
+        <v>1</v>
+      </c>
+      <c r="C2249" s="1">
+        <v>44617</v>
+      </c>
+    </row>
+    <row r="2250" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2250">
+        <v>2022</v>
+      </c>
+      <c r="B2250">
+        <v>1</v>
+      </c>
+      <c r="C2250" s="1">
+        <v>44618</v>
+      </c>
+    </row>
+    <row r="2251" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2251">
+        <v>2022</v>
+      </c>
+      <c r="B2251">
+        <v>1</v>
+      </c>
+      <c r="C2251" s="1">
+        <v>44619</v>
+      </c>
+    </row>
+    <row r="2252" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2252">
+        <v>2022</v>
+      </c>
+      <c r="B2252">
+        <v>1</v>
+      </c>
+      <c r="C2252" s="1">
+        <v>44620</v>
+      </c>
+    </row>
+    <row r="2253" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2253">
+        <v>2022</v>
+      </c>
+      <c r="B2253">
+        <v>1</v>
+      </c>
+      <c r="C2253" s="1">
+        <v>44621</v>
+      </c>
+    </row>
+    <row r="2254" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2254">
+        <v>2022</v>
+      </c>
+      <c r="B2254">
+        <v>1</v>
+      </c>
+      <c r="C2254" s="1">
+        <v>44622</v>
+      </c>
+    </row>
+    <row r="2255" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2255">
+        <v>2022</v>
+      </c>
+      <c r="B2255">
+        <v>1</v>
+      </c>
+      <c r="C2255" s="1">
+        <v>44623</v>
+      </c>
+    </row>
+    <row r="2256" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2256">
+        <v>2022</v>
+      </c>
+      <c r="B2256">
+        <v>1</v>
+      </c>
+      <c r="C2256" s="1">
+        <v>44624</v>
+      </c>
+    </row>
+    <row r="2257" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2257">
+        <v>2022</v>
+      </c>
+      <c r="B2257">
+        <v>1</v>
+      </c>
+      <c r="C2257" s="1">
+        <v>44625</v>
+      </c>
+    </row>
+    <row r="2258" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2258">
+        <v>2022</v>
+      </c>
+      <c r="B2258">
+        <v>1</v>
+      </c>
+      <c r="C2258" s="1">
+        <v>44626</v>
+      </c>
+    </row>
+    <row r="2259" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2259">
+        <v>2022</v>
+      </c>
+      <c r="B2259">
+        <v>1</v>
+      </c>
+      <c r="C2259" s="1">
+        <v>44627</v>
+      </c>
+    </row>
+    <row r="2260" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2260">
+        <v>2022</v>
+      </c>
+      <c r="B2260">
+        <v>1</v>
+      </c>
+      <c r="C2260" s="1">
+        <v>44628</v>
+      </c>
+    </row>
+    <row r="2261" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2261">
+        <v>2022</v>
+      </c>
+      <c r="B2261">
+        <v>1</v>
+      </c>
+      <c r="C2261" s="1">
+        <v>44629</v>
+      </c>
+    </row>
+    <row r="2262" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2262">
+        <v>2022</v>
+      </c>
+      <c r="B2262">
+        <v>1</v>
+      </c>
+      <c r="C2262" s="1">
+        <v>44630</v>
+      </c>
+    </row>
+    <row r="2263" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2263">
+        <v>2022</v>
+      </c>
+      <c r="B2263">
+        <v>1</v>
+      </c>
+      <c r="C2263" s="1">
+        <v>44631</v>
+      </c>
+    </row>
+    <row r="2264" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2264">
+        <v>2022</v>
+      </c>
+      <c r="B2264">
+        <v>1</v>
+      </c>
+      <c r="C2264" s="1">
+        <v>44632</v>
+      </c>
+    </row>
+    <row r="2265" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2265">
+        <v>2022</v>
+      </c>
+      <c r="B2265">
+        <v>1</v>
+      </c>
+      <c r="C2265" s="1">
+        <v>44633</v>
+      </c>
+    </row>
+    <row r="2266" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2266">
+        <v>2022</v>
+      </c>
+      <c r="B2266">
+        <v>1</v>
+      </c>
+      <c r="C2266" s="1">
+        <v>44634</v>
+      </c>
+    </row>
+    <row r="2267" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2267">
+        <v>2022</v>
+      </c>
+      <c r="B2267">
+        <v>1</v>
+      </c>
+      <c r="C2267" s="1">
+        <v>44635</v>
+      </c>
+    </row>
+    <row r="2268" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2268">
+        <v>2022</v>
+      </c>
+      <c r="B2268">
+        <v>1</v>
+      </c>
+      <c r="C2268" s="1">
+        <v>44636</v>
+      </c>
+    </row>
+    <row r="2269" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2269">
+        <v>2022</v>
+      </c>
+      <c r="B2269">
+        <v>1</v>
+      </c>
+      <c r="C2269" s="1">
+        <v>44637</v>
+      </c>
+    </row>
+    <row r="2270" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2270">
+        <v>2022</v>
+      </c>
+      <c r="B2270">
+        <v>1</v>
+      </c>
+      <c r="C2270" s="1">
+        <v>44638</v>
+      </c>
+    </row>
+    <row r="2271" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2271">
+        <v>2022</v>
+      </c>
+      <c r="B2271">
+        <v>1</v>
+      </c>
+      <c r="C2271" s="1">
+        <v>44639</v>
+      </c>
+    </row>
+    <row r="2272" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2272">
+        <v>2022</v>
+      </c>
+      <c r="B2272">
+        <v>1</v>
+      </c>
+      <c r="C2272" s="1">
+        <v>44640</v>
+      </c>
+    </row>
+    <row r="2273" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2273">
+        <v>2022</v>
+      </c>
+      <c r="B2273">
+        <v>1</v>
+      </c>
+      <c r="C2273" s="1">
+        <v>44641</v>
+      </c>
+    </row>
+    <row r="2274" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2274">
+        <v>2022</v>
+      </c>
+      <c r="B2274">
+        <v>1</v>
+      </c>
+      <c r="C2274" s="1">
+        <v>44642</v>
+      </c>
+    </row>
+    <row r="2275" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2275">
+        <v>2022</v>
+      </c>
+      <c r="B2275">
+        <v>1</v>
+      </c>
+      <c r="C2275" s="1">
+        <v>44643</v>
+      </c>
+    </row>
+    <row r="2276" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2276">
+        <v>2022</v>
+      </c>
+      <c r="B2276">
+        <v>1</v>
+      </c>
+      <c r="C2276" s="1">
+        <v>44644</v>
+      </c>
+    </row>
+    <row r="2277" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2277">
+        <v>2022</v>
+      </c>
+      <c r="B2277">
+        <v>1</v>
+      </c>
+      <c r="C2277" s="1">
+        <v>44645</v>
+      </c>
+    </row>
+    <row r="2278" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2278">
+        <v>2022</v>
+      </c>
+      <c r="B2278">
+        <v>1</v>
+      </c>
+      <c r="C2278" s="1">
+        <v>44646</v>
+      </c>
+    </row>
+    <row r="2279" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2279">
+        <v>2022</v>
+      </c>
+      <c r="B2279">
+        <v>1</v>
+      </c>
+      <c r="C2279" s="1">
+        <v>44647</v>
+      </c>
+    </row>
+    <row r="2280" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2280">
+        <v>2022</v>
+      </c>
+      <c r="B2280">
+        <v>1</v>
+      </c>
+      <c r="C2280" s="1">
+        <v>44648</v>
+      </c>
+    </row>
+    <row r="2281" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2281">
+        <v>2022</v>
+      </c>
+      <c r="B2281">
+        <v>1</v>
+      </c>
+      <c r="C2281" s="1">
+        <v>44649</v>
+      </c>
+    </row>
+    <row r="2282" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2282">
+        <v>2022</v>
+      </c>
+      <c r="B2282">
+        <v>1</v>
+      </c>
+      <c r="C2282" s="1">
+        <v>44650</v>
+      </c>
+    </row>
+    <row r="2283" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2283">
+        <v>2022</v>
+      </c>
+      <c r="B2283">
+        <v>1</v>
+      </c>
+      <c r="C2283" s="1">
+        <v>44651</v>
+      </c>
+    </row>
+    <row r="2284" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2284">
+        <v>2022</v>
+      </c>
+      <c r="B2284">
+        <v>1</v>
+      </c>
+      <c r="C2284" s="1">
+        <v>44652</v>
+      </c>
+    </row>
+    <row r="2285" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2285">
+        <v>2022</v>
+      </c>
+      <c r="B2285">
+        <v>1</v>
+      </c>
+      <c r="C2285" s="1">
+        <v>44653</v>
+      </c>
+    </row>
+    <row r="2286" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2286">
+        <v>2022</v>
+      </c>
+      <c r="B2286">
+        <v>1</v>
+      </c>
+      <c r="C2286" s="1">
+        <v>44654</v>
+      </c>
+    </row>
+    <row r="2287" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2287">
+        <v>2022</v>
+      </c>
+      <c r="B2287">
+        <v>1</v>
+      </c>
+      <c r="C2287" s="1">
+        <v>44655</v>
+      </c>
+    </row>
+    <row r="2288" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2288">
+        <v>2022</v>
+      </c>
+      <c r="B2288">
+        <v>1</v>
+      </c>
+      <c r="C2288" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="2289" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2289">
+        <v>2022</v>
+      </c>
+      <c r="B2289">
+        <v>1</v>
+      </c>
+      <c r="C2289" s="1">
+        <v>44657</v>
+      </c>
+    </row>
+    <row r="2290" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2290">
+        <v>2022</v>
+      </c>
+      <c r="B2290">
+        <v>1</v>
+      </c>
+      <c r="C2290" s="1">
+        <v>44658</v>
+      </c>
+    </row>
+    <row r="2291" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2291">
+        <v>2022</v>
+      </c>
+      <c r="B2291">
+        <v>1</v>
+      </c>
+      <c r="C2291" s="1">
+        <v>44659</v>
+      </c>
+    </row>
+    <row r="2292" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2292">
+        <v>2022</v>
+      </c>
+      <c r="B2292">
+        <v>1</v>
+      </c>
+      <c r="C2292" s="1">
+        <v>44660</v>
+      </c>
+    </row>
+    <row r="2293" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2293">
+        <v>2022</v>
+      </c>
+      <c r="B2293">
+        <v>1</v>
+      </c>
+      <c r="C2293" s="1">
+        <v>44661</v>
+      </c>
+    </row>
+    <row r="2294" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2294">
+        <v>2022</v>
+      </c>
+      <c r="B2294">
+        <v>1</v>
+      </c>
+      <c r="C2294" s="1">
+        <v>44662</v>
+      </c>
+    </row>
+    <row r="2295" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2295">
+        <v>2022</v>
+      </c>
+      <c r="B2295">
+        <v>1</v>
+      </c>
+      <c r="C2295" s="1">
+        <v>44663</v>
+      </c>
+    </row>
+    <row r="2296" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2296">
+        <v>2022</v>
+      </c>
+      <c r="B2296">
+        <v>1</v>
+      </c>
+      <c r="C2296" s="1">
+        <v>44664</v>
+      </c>
+    </row>
+    <row r="2297" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2297">
+        <v>2022</v>
+      </c>
+      <c r="B2297">
+        <v>1</v>
+      </c>
+      <c r="C2297" s="1">
+        <v>44665</v>
+      </c>
+    </row>
+    <row r="2298" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2298">
+        <v>2022</v>
+      </c>
+      <c r="B2298">
+        <v>1</v>
+      </c>
+      <c r="C2298" s="1">
+        <v>44666</v>
+      </c>
+    </row>
+    <row r="2299" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2299">
+        <v>2022</v>
+      </c>
+      <c r="B2299">
+        <v>1</v>
+      </c>
+      <c r="C2299" s="1">
+        <v>44667</v>
+      </c>
+    </row>
+    <row r="2300" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2300">
+        <v>2022</v>
+      </c>
+      <c r="B2300">
+        <v>1</v>
+      </c>
+      <c r="C2300" s="1">
+        <v>44668</v>
+      </c>
+    </row>
+    <row r="2301" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2301">
+        <v>2022</v>
+      </c>
+      <c r="B2301">
+        <v>1</v>
+      </c>
+      <c r="C2301" s="1">
+        <v>44669</v>
+      </c>
+    </row>
+    <row r="2302" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2302">
+        <v>2022</v>
+      </c>
+      <c r="B2302">
+        <v>1</v>
+      </c>
+      <c r="C2302" s="1">
+        <v>44670</v>
+      </c>
+    </row>
+    <row r="2303" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2303">
+        <v>2022</v>
+      </c>
+      <c r="B2303">
+        <v>1</v>
+      </c>
+      <c r="C2303" s="1">
+        <v>44671</v>
+      </c>
+    </row>
+    <row r="2304" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2304">
+        <v>2022</v>
+      </c>
+      <c r="B2304">
+        <v>1</v>
+      </c>
+      <c r="C2304" s="1">
+        <v>44672</v>
+      </c>
+    </row>
+    <row r="2305" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2305">
+        <v>2022</v>
+      </c>
+      <c r="B2305">
+        <v>1</v>
+      </c>
+      <c r="C2305" s="1">
+        <v>44673</v>
+      </c>
+    </row>
+    <row r="2306" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2306">
+        <v>2022</v>
+      </c>
+      <c r="B2306">
+        <v>1</v>
+      </c>
+      <c r="C2306" s="1">
+        <v>44674</v>
+      </c>
+    </row>
+    <row r="2307" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2307">
+        <v>2022</v>
+      </c>
+      <c r="B2307">
+        <v>1</v>
+      </c>
+      <c r="C2307" s="1">
+        <v>44675</v>
+      </c>
+    </row>
+    <row r="2308" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2308">
+        <v>2022</v>
+      </c>
+      <c r="B2308">
+        <v>1</v>
+      </c>
+      <c r="C2308" s="1">
+        <v>44676</v>
+      </c>
+    </row>
+    <row r="2309" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2309">
+        <v>2022</v>
+      </c>
+      <c r="B2309">
+        <v>1</v>
+      </c>
+      <c r="C2309" s="1">
+        <v>44677</v>
+      </c>
+    </row>
+    <row r="2310" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2310">
+        <v>2022</v>
+      </c>
+      <c r="B2310">
+        <v>1</v>
+      </c>
+      <c r="C2310" s="1">
+        <v>44678</v>
+      </c>
+    </row>
+    <row r="2311" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2311">
+        <v>2022</v>
+      </c>
+      <c r="B2311">
+        <v>1</v>
+      </c>
+      <c r="C2311" s="1">
+        <v>44679</v>
+      </c>
+    </row>
+    <row r="2312" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2312">
+        <v>2022</v>
+      </c>
+      <c r="B2312">
+        <v>1</v>
+      </c>
+      <c r="C2312" s="1">
+        <v>44680</v>
+      </c>
+    </row>
+    <row r="2313" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2313">
+        <v>2022</v>
+      </c>
+      <c r="B2313">
+        <v>1</v>
+      </c>
+      <c r="C2313" s="1">
+        <v>44681</v>
+      </c>
+    </row>
+    <row r="2314" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2314">
+        <v>2022</v>
+      </c>
+      <c r="B2314">
+        <v>1</v>
+      </c>
+      <c r="C2314" s="1">
+        <v>44682</v>
+      </c>
+    </row>
+    <row r="2315" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2315">
+        <v>2022</v>
+      </c>
+      <c r="B2315">
+        <v>1</v>
+      </c>
+      <c r="C2315" s="1">
+        <v>44683</v>
+      </c>
+    </row>
+    <row r="2316" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2316">
+        <v>2022</v>
+      </c>
+      <c r="B2316">
+        <v>1</v>
+      </c>
+      <c r="C2316" s="1">
+        <v>44684</v>
+      </c>
+    </row>
+    <row r="2317" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2317">
+        <v>2022</v>
+      </c>
+      <c r="B2317">
+        <v>1</v>
+      </c>
+      <c r="C2317" s="1">
+        <v>44685</v>
+      </c>
+    </row>
+    <row r="2318" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2318">
+        <v>2022</v>
+      </c>
+      <c r="B2318">
+        <v>1</v>
+      </c>
+      <c r="C2318" s="1">
+        <v>44686</v>
+      </c>
+    </row>
+    <row r="2319" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2319">
+        <v>2022</v>
+      </c>
+      <c r="B2319">
+        <v>1</v>
+      </c>
+      <c r="C2319" s="1">
+        <v>44687</v>
+      </c>
+    </row>
+    <row r="2320" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2320">
+        <v>2022</v>
+      </c>
+      <c r="B2320">
+        <v>1</v>
+      </c>
+      <c r="C2320" s="1">
+        <v>44688</v>
+      </c>
+    </row>
+    <row r="2321" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2321">
+        <v>2022</v>
+      </c>
+      <c r="B2321">
+        <v>1</v>
+      </c>
+      <c r="C2321" s="1">
+        <v>44689</v>
+      </c>
+    </row>
+    <row r="2322" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2322">
+        <v>2022</v>
+      </c>
+      <c r="B2322">
+        <v>1</v>
+      </c>
+      <c r="C2322" s="1">
+        <v>44690</v>
+      </c>
+    </row>
+    <row r="2323" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2323">
+        <v>2022</v>
+      </c>
+      <c r="B2323">
+        <v>1</v>
+      </c>
+      <c r="C2323" s="1">
+        <v>44691</v>
+      </c>
+    </row>
+    <row r="2324" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2324">
+        <v>2022</v>
+      </c>
+      <c r="B2324">
+        <v>1</v>
+      </c>
+      <c r="C2324" s="1">
+        <v>44692</v>
+      </c>
+    </row>
+    <row r="2325" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2325">
+        <v>2022</v>
+      </c>
+      <c r="B2325">
+        <v>1</v>
+      </c>
+      <c r="C2325" s="1">
+        <v>44693</v>
+      </c>
+    </row>
+    <row r="2326" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2326">
+        <v>2022</v>
+      </c>
+      <c r="B2326">
+        <v>1</v>
+      </c>
+      <c r="C2326" s="1">
+        <v>44694</v>
+      </c>
+    </row>
+    <row r="2327" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2327">
+        <v>2022</v>
+      </c>
+      <c r="B2327">
+        <v>1</v>
+      </c>
+      <c r="C2327" s="1">
+        <v>44695</v>
+      </c>
+    </row>
+    <row r="2328" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2328">
+        <v>2022</v>
+      </c>
+      <c r="B2328">
+        <v>1</v>
+      </c>
+      <c r="C2328" s="1">
+        <v>44696</v>
+      </c>
+    </row>
+    <row r="2329" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2329">
+        <v>2022</v>
+      </c>
+      <c r="B2329">
+        <v>1</v>
+      </c>
+      <c r="C2329" s="1">
+        <v>44697</v>
+      </c>
+    </row>
+    <row r="2330" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2330">
+        <v>2022</v>
+      </c>
+      <c r="B2330">
+        <v>1</v>
+      </c>
+      <c r="C2330" s="1">
+        <v>44698</v>
+      </c>
+    </row>
+    <row r="2331" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2331">
+        <v>2022</v>
+      </c>
+      <c r="B2331">
+        <v>1</v>
+      </c>
+      <c r="C2331" s="1">
+        <v>44699</v>
+      </c>
+    </row>
+    <row r="2332" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2332">
+        <v>2022</v>
+      </c>
+      <c r="B2332">
+        <v>1</v>
+      </c>
+      <c r="C2332" s="1">
+        <v>44700</v>
+      </c>
+    </row>
+    <row r="2333" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2333">
+        <v>2022</v>
+      </c>
+      <c r="B2333">
+        <v>1</v>
+      </c>
+      <c r="C2333" s="1">
+        <v>44701</v>
+      </c>
+    </row>
+    <row r="2334" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2334">
+        <v>2022</v>
+      </c>
+      <c r="B2334">
+        <v>1</v>
+      </c>
+      <c r="C2334" s="1">
+        <v>44702</v>
+      </c>
+    </row>
+    <row r="2335" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2335">
+        <v>2022</v>
+      </c>
+      <c r="B2335">
+        <v>1</v>
+      </c>
+      <c r="C2335" s="1">
+        <v>44703</v>
+      </c>
+    </row>
+    <row r="2336" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2336">
+        <v>2022</v>
+      </c>
+      <c r="B2336">
+        <v>1</v>
+      </c>
+      <c r="C2336" s="1">
+        <v>44704</v>
+      </c>
+    </row>
+    <row r="2337" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2337">
+        <v>2022</v>
+      </c>
+      <c r="B2337">
+        <v>1</v>
+      </c>
+      <c r="C2337" s="1">
+        <v>44705</v>
+      </c>
+    </row>
+    <row r="2338" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2338">
+        <v>2022</v>
+      </c>
+      <c r="B2338">
+        <v>1</v>
+      </c>
+      <c r="C2338" s="1">
+        <v>44706</v>
+      </c>
+    </row>
+    <row r="2339" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2339">
+        <v>2022</v>
+      </c>
+      <c r="B2339">
+        <v>1</v>
+      </c>
+      <c r="C2339" s="1">
+        <v>44707</v>
+      </c>
+    </row>
+    <row r="2340" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2340">
+        <v>2022</v>
+      </c>
+      <c r="B2340">
+        <v>1</v>
+      </c>
+      <c r="C2340" s="1">
+        <v>44708</v>
+      </c>
+    </row>
+    <row r="2341" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2341">
+        <v>2022</v>
+      </c>
+      <c r="B2341">
+        <v>1</v>
+      </c>
+      <c r="C2341" s="1">
+        <v>44709</v>
+      </c>
+    </row>
+    <row r="2342" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2342">
+        <v>2022</v>
+      </c>
+      <c r="B2342">
+        <v>1</v>
+      </c>
+      <c r="C2342" s="1">
+        <v>44710</v>
+      </c>
+    </row>
+    <row r="2343" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2343">
+        <v>2022</v>
+      </c>
+      <c r="B2343">
+        <v>1</v>
+      </c>
+      <c r="C2343" s="1">
+        <v>44711</v>
+      </c>
+    </row>
+    <row r="2344" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2344">
+        <v>2022</v>
+      </c>
+      <c r="B2344">
+        <v>1</v>
+      </c>
+      <c r="C2344" s="1">
+        <v>44712</v>
+      </c>
+    </row>
+    <row r="2345" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2345">
+        <v>2022</v>
+      </c>
+      <c r="B2345">
+        <v>1</v>
+      </c>
+      <c r="C2345" s="1">
+        <v>44713</v>
+      </c>
+    </row>
+    <row r="2346" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2346">
+        <v>2022</v>
+      </c>
+      <c r="B2346">
+        <v>1</v>
+      </c>
+      <c r="C2346" s="1">
+        <v>44714</v>
+      </c>
+    </row>
+    <row r="2347" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2347">
+        <v>2022</v>
+      </c>
+      <c r="B2347">
+        <v>1</v>
+      </c>
+      <c r="C2347" s="1">
+        <v>44715</v>
+      </c>
+    </row>
+    <row r="2348" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2348">
+        <v>2022</v>
+      </c>
+      <c r="B2348">
+        <v>1</v>
+      </c>
+      <c r="C2348" s="1">
+        <v>44716</v>
+      </c>
+    </row>
+    <row r="2349" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2349">
+        <v>2022</v>
+      </c>
+      <c r="B2349">
+        <v>1</v>
+      </c>
+      <c r="C2349" s="1">
+        <v>44717</v>
+      </c>
+    </row>
+    <row r="2350" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2350">
+        <v>2022</v>
+      </c>
+      <c r="B2350">
+        <v>1</v>
+      </c>
+      <c r="C2350" s="1">
+        <v>44718</v>
+      </c>
+    </row>
+    <row r="2351" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2351">
+        <v>2022</v>
+      </c>
+      <c r="B2351">
+        <v>1</v>
+      </c>
+      <c r="C2351" s="1">
+        <v>44719</v>
+      </c>
+    </row>
+    <row r="2352" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2352">
+        <v>2022</v>
+      </c>
+      <c r="B2352">
+        <v>1</v>
+      </c>
+      <c r="C2352" s="1">
+        <v>44720</v>
+      </c>
+    </row>
+    <row r="2353" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2353">
+        <v>2022</v>
+      </c>
+      <c r="B2353">
+        <v>1</v>
+      </c>
+      <c r="C2353" s="1">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="2354" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2354">
+        <v>2022</v>
+      </c>
+      <c r="B2354">
+        <v>1</v>
+      </c>
+      <c r="C2354" s="1">
+        <v>44722</v>
+      </c>
+    </row>
+    <row r="2355" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2355">
+        <v>2022</v>
+      </c>
+      <c r="B2355">
+        <v>1</v>
+      </c>
+      <c r="C2355" s="1">
+        <v>44723</v>
+      </c>
+    </row>
+    <row r="2356" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2356">
+        <v>2022</v>
+      </c>
+      <c r="B2356">
+        <v>1</v>
+      </c>
+      <c r="C2356" s="1">
+        <v>44724</v>
+      </c>
+    </row>
+    <row r="2357" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2357">
+        <v>2022</v>
+      </c>
+      <c r="B2357">
+        <v>1</v>
+      </c>
+      <c r="C2357" s="1">
+        <v>44725</v>
+      </c>
+    </row>
+    <row r="2358" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2358">
+        <v>2022</v>
+      </c>
+      <c r="B2358">
+        <v>1</v>
+      </c>
+      <c r="C2358" s="1">
+        <v>44726</v>
+      </c>
+    </row>
+    <row r="2359" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2359">
+        <v>2022</v>
+      </c>
+      <c r="B2359">
+        <v>1</v>
+      </c>
+      <c r="C2359" s="1">
+        <v>44727</v>
+      </c>
+    </row>
+    <row r="2360" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2360">
+        <v>2022</v>
+      </c>
+      <c r="B2360">
+        <v>1</v>
+      </c>
+      <c r="C2360" s="1">
+        <v>44728</v>
+      </c>
+    </row>
+    <row r="2361" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2361">
+        <v>2022</v>
+      </c>
+      <c r="B2361">
+        <v>1</v>
+      </c>
+      <c r="C2361" s="1">
+        <v>44729</v>
+      </c>
+    </row>
+    <row r="2362" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2362">
+        <v>2022</v>
+      </c>
+      <c r="B2362">
+        <v>1</v>
+      </c>
+      <c r="C2362" s="1">
+        <v>44730</v>
+      </c>
+    </row>
+    <row r="2363" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2363">
+        <v>2022</v>
+      </c>
+      <c r="B2363">
+        <v>1</v>
+      </c>
+      <c r="C2363" s="1">
+        <v>44731</v>
+      </c>
+    </row>
+    <row r="2364" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2364">
+        <v>2022</v>
+      </c>
+      <c r="B2364">
+        <v>1</v>
+      </c>
+      <c r="C2364" s="1">
+        <v>44732</v>
+      </c>
+    </row>
+    <row r="2365" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2365">
+        <v>2022</v>
+      </c>
+      <c r="B2365">
+        <v>1</v>
+      </c>
+      <c r="C2365" s="1">
+        <v>44733</v>
+      </c>
+    </row>
+    <row r="2366" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2366">
+        <v>2022</v>
+      </c>
+      <c r="B2366">
+        <v>1</v>
+      </c>
+      <c r="C2366" s="1">
+        <v>44734</v>
+      </c>
+    </row>
+    <row r="2367" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2367">
+        <v>2022</v>
+      </c>
+      <c r="B2367">
+        <v>1</v>
+      </c>
+      <c r="C2367" s="1">
+        <v>44735</v>
+      </c>
+    </row>
+    <row r="2368" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2368">
+        <v>2022</v>
+      </c>
+      <c r="B2368">
+        <v>1</v>
+      </c>
+      <c r="C2368" s="1">
+        <v>44736</v>
+      </c>
+    </row>
+    <row r="2369" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2369">
+        <v>2022</v>
+      </c>
+      <c r="B2369">
+        <v>1</v>
+      </c>
+      <c r="C2369" s="1">
+        <v>44737</v>
+      </c>
+    </row>
+    <row r="2370" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2370">
+        <v>2022</v>
+      </c>
+      <c r="B2370">
+        <v>1</v>
+      </c>
+      <c r="C2370" s="1">
+        <v>44738</v>
+      </c>
+    </row>
+    <row r="2371" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2371">
+        <v>2022</v>
+      </c>
+      <c r="B2371">
+        <v>1</v>
+      </c>
+      <c r="C2371" s="1">
+        <v>44739</v>
+      </c>
+    </row>
+    <row r="2372" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2372">
+        <v>2022</v>
+      </c>
+      <c r="B2372">
+        <v>1</v>
+      </c>
+      <c r="C2372" s="1">
+        <v>44740</v>
+      </c>
+    </row>
+    <row r="2373" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2373">
+        <v>2022</v>
+      </c>
+      <c r="B2373">
+        <v>1</v>
+      </c>
+      <c r="C2373" s="1">
+        <v>44741</v>
+      </c>
+    </row>
+    <row r="2374" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2374">
+        <v>2022</v>
+      </c>
+      <c r="B2374">
+        <v>1</v>
+      </c>
+      <c r="C2374" s="1">
+        <v>44742</v>
+      </c>
+    </row>
+    <row r="2375" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2375">
+        <v>2022</v>
+      </c>
+      <c r="B2375">
+        <v>1</v>
+      </c>
+      <c r="C2375" s="1">
+        <v>44743</v>
+      </c>
+    </row>
+    <row r="2376" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2376">
+        <v>2022</v>
+      </c>
+      <c r="B2376">
+        <v>1</v>
+      </c>
+      <c r="C2376" s="1">
+        <v>44744</v>
+      </c>
+    </row>
+    <row r="2377" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2377">
+        <v>2022</v>
+      </c>
+      <c r="B2377">
+        <v>1</v>
+      </c>
+      <c r="C2377" s="1">
+        <v>44745</v>
+      </c>
+    </row>
+    <row r="2378" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2378">
+        <v>2022</v>
+      </c>
+      <c r="B2378">
+        <v>1</v>
+      </c>
+      <c r="C2378" s="1">
+        <v>44746</v>
+      </c>
+    </row>
+    <row r="2379" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2379">
+        <v>2022</v>
+      </c>
+      <c r="B2379">
+        <v>1</v>
+      </c>
+      <c r="C2379" s="1">
+        <v>44747</v>
+      </c>
+    </row>
+    <row r="2380" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2380">
+        <v>2022</v>
+      </c>
+      <c r="B2380">
+        <v>1</v>
+      </c>
+      <c r="C2380" s="1">
+        <v>44748</v>
+      </c>
+    </row>
+    <row r="2381" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2381">
+        <v>2022</v>
+      </c>
+      <c r="B2381">
+        <v>1</v>
+      </c>
+      <c r="C2381" s="1">
+        <v>44749</v>
+      </c>
+    </row>
+    <row r="2382" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2382">
+        <v>2022</v>
+      </c>
+      <c r="B2382">
+        <v>1</v>
+      </c>
+      <c r="C2382" s="1">
+        <v>44750</v>
+      </c>
+    </row>
+    <row r="2383" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2383">
+        <v>2022</v>
+      </c>
+      <c r="B2383">
+        <v>1</v>
+      </c>
+      <c r="C2383" s="1">
+        <v>44751</v>
+      </c>
+    </row>
+    <row r="2384" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2384">
+        <v>2022</v>
+      </c>
+      <c r="B2384">
+        <v>1</v>
+      </c>
+      <c r="C2384" s="1">
+        <v>44752</v>
+      </c>
+    </row>
+    <row r="2385" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2385">
+        <v>2022</v>
+      </c>
+      <c r="B2385">
+        <v>1</v>
+      </c>
+      <c r="C2385" s="1">
+        <v>44753</v>
+      </c>
+    </row>
+    <row r="2386" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2386">
+        <v>2022</v>
+      </c>
+      <c r="B2386">
+        <v>1</v>
+      </c>
+      <c r="C2386" s="1">
+        <v>44754</v>
+      </c>
+    </row>
+    <row r="2387" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2387">
+        <v>2022</v>
+      </c>
+      <c r="B2387">
+        <v>1</v>
+      </c>
+      <c r="C2387" s="1">
+        <v>44755</v>
+      </c>
+    </row>
+    <row r="2388" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2388">
+        <v>2022</v>
+      </c>
+      <c r="B2388">
+        <v>1</v>
+      </c>
+      <c r="C2388" s="1">
+        <v>44756</v>
+      </c>
+    </row>
+    <row r="2389" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2389">
+        <v>2022</v>
+      </c>
+      <c r="B2389">
+        <v>1</v>
+      </c>
+      <c r="C2389" s="1">
+        <v>44757</v>
+      </c>
+    </row>
+    <row r="2390" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2390">
+        <v>2022</v>
+      </c>
+      <c r="B2390">
+        <v>1</v>
+      </c>
+      <c r="C2390" s="1">
+        <v>44758</v>
+      </c>
+    </row>
+    <row r="2391" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2391">
+        <v>2022</v>
+      </c>
+      <c r="B2391">
+        <v>1</v>
+      </c>
+      <c r="C2391" s="1">
+        <v>44759</v>
+      </c>
+    </row>
+    <row r="2392" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2392">
+        <v>2022</v>
+      </c>
+      <c r="B2392">
+        <v>1</v>
+      </c>
+      <c r="C2392" s="1">
+        <v>44760</v>
+      </c>
+    </row>
+    <row r="2393" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2393">
+        <v>2022</v>
+      </c>
+      <c r="B2393">
+        <v>1</v>
+      </c>
+      <c r="C2393" s="1">
+        <v>44761</v>
+      </c>
+    </row>
+    <row r="2394" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2394">
+        <v>2022</v>
+      </c>
+      <c r="B2394">
+        <v>1</v>
+      </c>
+      <c r="C2394" s="1">
+        <v>44762</v>
+      </c>
+    </row>
+    <row r="2395" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2395">
+        <v>2022</v>
+      </c>
+      <c r="B2395">
+        <v>1</v>
+      </c>
+      <c r="C2395" s="1">
+        <v>44763</v>
+      </c>
+    </row>
+    <row r="2396" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2396">
+        <v>2022</v>
+      </c>
+      <c r="B2396">
+        <v>1</v>
+      </c>
+      <c r="C2396" s="1">
+        <v>44764</v>
+      </c>
+    </row>
+    <row r="2397" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2397">
+        <v>2022</v>
+      </c>
+      <c r="B2397">
+        <v>1</v>
+      </c>
+      <c r="C2397" s="1">
+        <v>44765</v>
+      </c>
+    </row>
+    <row r="2398" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2398">
+        <v>2022</v>
+      </c>
+      <c r="B2398">
+        <v>1</v>
+      </c>
+      <c r="C2398" s="1">
+        <v>44766</v>
+      </c>
+    </row>
+    <row r="2399" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2399">
+        <v>2022</v>
+      </c>
+      <c r="B2399">
+        <v>1</v>
+      </c>
+      <c r="C2399" s="1">
+        <v>44767</v>
+      </c>
+    </row>
+    <row r="2400" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2400">
+        <v>2022</v>
+      </c>
+      <c r="B2400">
+        <v>1</v>
+      </c>
+      <c r="C2400" s="1">
+        <v>44768</v>
+      </c>
+    </row>
+    <row r="2401" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2401">
+        <v>2022</v>
+      </c>
+      <c r="B2401">
+        <v>1</v>
+      </c>
+      <c r="C2401" s="1">
+        <v>44769</v>
+      </c>
+    </row>
+    <row r="2402" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2402">
+        <v>2022</v>
+      </c>
+      <c r="B2402">
+        <v>1</v>
+      </c>
+      <c r="C2402" s="1">
+        <v>44770</v>
+      </c>
+    </row>
+    <row r="2403" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2403">
+        <v>2022</v>
+      </c>
+      <c r="B2403">
+        <v>1</v>
+      </c>
+      <c r="C2403" s="1">
+        <v>44771</v>
+      </c>
+    </row>
+    <row r="2404" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2404">
+        <v>2022</v>
+      </c>
+      <c r="B2404">
+        <v>1</v>
+      </c>
+      <c r="C2404" s="1">
+        <v>44772</v>
+      </c>
+    </row>
+    <row r="2405" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2405">
+        <v>2022</v>
+      </c>
+      <c r="B2405">
+        <v>1</v>
+      </c>
+      <c r="C2405" s="1">
+        <v>44773</v>
+      </c>
+    </row>
+    <row r="2406" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2406">
+        <v>2022</v>
+      </c>
+      <c r="B2406">
+        <v>1</v>
+      </c>
+      <c r="C2406" s="1">
+        <v>44774</v>
+      </c>
+    </row>
+    <row r="2407" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2407">
+        <v>2022</v>
+      </c>
+      <c r="B2407">
+        <v>1</v>
+      </c>
+      <c r="C2407" s="1">
+        <v>44775</v>
+      </c>
+    </row>
+    <row r="2408" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2408">
+        <v>2022</v>
+      </c>
+      <c r="B2408">
+        <v>1</v>
+      </c>
+      <c r="C2408" s="1">
+        <v>44776</v>
+      </c>
+    </row>
+    <row r="2409" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2409">
+        <v>2022</v>
+      </c>
+      <c r="B2409">
+        <v>1</v>
+      </c>
+      <c r="C2409" s="1">
+        <v>44777</v>
+      </c>
+    </row>
+    <row r="2410" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2410">
+        <v>2022</v>
+      </c>
+      <c r="B2410">
+        <v>1</v>
+      </c>
+      <c r="C2410" s="1">
+        <v>44778</v>
+      </c>
+    </row>
+    <row r="2411" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2411">
+        <v>2022</v>
+      </c>
+      <c r="B2411">
+        <v>1</v>
+      </c>
+      <c r="C2411" s="1">
+        <v>44779</v>
+      </c>
+    </row>
+    <row r="2412" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2412">
+        <v>2022</v>
+      </c>
+      <c r="B2412">
+        <v>1</v>
+      </c>
+      <c r="C2412" s="1">
+        <v>44780</v>
+      </c>
+    </row>
+    <row r="2413" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2413">
+        <v>2022</v>
+      </c>
+      <c r="B2413">
+        <v>1</v>
+      </c>
+      <c r="C2413" s="1">
+        <v>44781</v>
+      </c>
+    </row>
+    <row r="2414" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2414">
+        <v>2022</v>
+      </c>
+      <c r="B2414">
+        <v>1</v>
+      </c>
+      <c r="C2414" s="1">
+        <v>44782</v>
+      </c>
+    </row>
+    <row r="2415" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2415">
+        <v>2022</v>
+      </c>
+      <c r="B2415">
+        <v>1</v>
+      </c>
+      <c r="C2415" s="1">
+        <v>44783</v>
+      </c>
+    </row>
+    <row r="2416" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2416">
+        <v>2022</v>
+      </c>
+      <c r="B2416">
+        <v>1</v>
+      </c>
+      <c r="C2416" s="1">
+        <v>44784</v>
+      </c>
+    </row>
+    <row r="2417" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2417">
+        <v>2022</v>
+      </c>
+      <c r="B2417">
+        <v>1</v>
+      </c>
+      <c r="C2417" s="1">
+        <v>44785</v>
+      </c>
+    </row>
+    <row r="2418" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2418">
+        <v>2022</v>
+      </c>
+      <c r="B2418">
+        <v>1</v>
+      </c>
+      <c r="C2418" s="1">
+        <v>44786</v>
+      </c>
+    </row>
+    <row r="2419" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2419">
+        <v>2022</v>
+      </c>
+      <c r="B2419">
+        <v>1</v>
+      </c>
+      <c r="C2419" s="1">
+        <v>44787</v>
+      </c>
+    </row>
+    <row r="2420" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2420">
+        <v>2022</v>
+      </c>
+      <c r="B2420">
+        <v>1</v>
+      </c>
+      <c r="C2420" s="1">
+        <v>44788</v>
+      </c>
+    </row>
+    <row r="2421" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2421">
+        <v>2022</v>
+      </c>
+      <c r="B2421">
+        <v>1</v>
+      </c>
+      <c r="C2421" s="1">
+        <v>44789</v>
+      </c>
+    </row>
+    <row r="2422" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2422">
+        <v>2022</v>
+      </c>
+      <c r="B2422">
+        <v>1</v>
+      </c>
+      <c r="C2422" s="1">
+        <v>44790</v>
+      </c>
+    </row>
+    <row r="2423" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2423">
+        <v>2022</v>
+      </c>
+      <c r="B2423">
+        <v>1</v>
+      </c>
+      <c r="C2423" s="1">
+        <v>44791</v>
+      </c>
+    </row>
+    <row r="2424" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2424">
+        <v>2022</v>
+      </c>
+      <c r="B2424">
+        <v>1</v>
+      </c>
+      <c r="C2424" s="1">
+        <v>44792</v>
+      </c>
+    </row>
+    <row r="2425" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2425">
+        <v>2022</v>
+      </c>
+      <c r="B2425">
+        <v>1</v>
+      </c>
+      <c r="C2425" s="1">
+        <v>44793</v>
+      </c>
+    </row>
+    <row r="2426" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2426">
+        <v>2022</v>
+      </c>
+      <c r="B2426">
+        <v>1</v>
+      </c>
+      <c r="C2426" s="1">
+        <v>44794</v>
+      </c>
+    </row>
+    <row r="2427" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2427">
+        <v>2022</v>
+      </c>
+      <c r="B2427">
+        <v>1</v>
+      </c>
+      <c r="C2427" s="1">
+        <v>44795</v>
+      </c>
+    </row>
+    <row r="2428" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2428">
+        <v>2022</v>
+      </c>
+      <c r="B2428">
+        <v>1</v>
+      </c>
+      <c r="C2428" s="1">
+        <v>44796</v>
+      </c>
+    </row>
+    <row r="2429" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2429">
+        <v>2022</v>
+      </c>
+      <c r="B2429">
+        <v>1</v>
+      </c>
+      <c r="C2429" s="1">
+        <v>44797</v>
+      </c>
+    </row>
+    <row r="2430" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2430">
+        <v>2022</v>
+      </c>
+      <c r="B2430">
+        <v>1</v>
+      </c>
+      <c r="C2430" s="1">
+        <v>44798</v>
+      </c>
+    </row>
+    <row r="2431" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2431">
+        <v>2022</v>
+      </c>
+      <c r="B2431">
+        <v>1</v>
+      </c>
+      <c r="C2431" s="1">
+        <v>44799</v>
+      </c>
+    </row>
+    <row r="2432" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2432">
+        <v>2022</v>
+      </c>
+      <c r="B2432">
+        <v>1</v>
+      </c>
+      <c r="C2432" s="1">
+        <v>44800</v>
+      </c>
+    </row>
+    <row r="2433" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2433">
+        <v>2022</v>
+      </c>
+      <c r="B2433">
+        <v>1</v>
+      </c>
+      <c r="C2433" s="1">
+        <v>44801</v>
+      </c>
+    </row>
+    <row r="2434" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2434">
+        <v>2022</v>
+      </c>
+      <c r="B2434">
+        <v>1</v>
+      </c>
+      <c r="C2434" s="1">
+        <v>44802</v>
+      </c>
+    </row>
+    <row r="2435" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2435">
+        <v>2022</v>
+      </c>
+      <c r="B2435">
+        <v>1</v>
+      </c>
+      <c r="C2435" s="1">
+        <v>44803</v>
+      </c>
+    </row>
+    <row r="2436" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2436">
+        <v>2022</v>
+      </c>
+      <c r="B2436">
+        <v>1</v>
+      </c>
+      <c r="C2436" s="1">
+        <v>44804</v>
+      </c>
+    </row>
+    <row r="2437" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2437">
+        <v>2022</v>
+      </c>
+      <c r="B2437">
+        <v>1</v>
+      </c>
+      <c r="C2437" s="1">
+        <v>44805</v>
+      </c>
+    </row>
+    <row r="2438" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2438">
+        <v>2022</v>
+      </c>
+      <c r="B2438">
+        <v>1</v>
+      </c>
+      <c r="C2438" s="1">
+        <v>44806</v>
+      </c>
+    </row>
+    <row r="2439" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2439">
+        <v>2022</v>
+      </c>
+      <c r="B2439">
+        <v>1</v>
+      </c>
+      <c r="C2439" s="1">
+        <v>44807</v>
+      </c>
+    </row>
+    <row r="2440" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2440">
+        <v>2022</v>
+      </c>
+      <c r="B2440">
+        <v>1</v>
+      </c>
+      <c r="C2440" s="1">
+        <v>44808</v>
+      </c>
+    </row>
+    <row r="2441" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2441">
+        <v>2022</v>
+      </c>
+      <c r="B2441">
+        <v>1</v>
+      </c>
+      <c r="C2441" s="1">
+        <v>44809</v>
+      </c>
+    </row>
+    <row r="2442" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2442">
+        <v>2022</v>
+      </c>
+      <c r="B2442">
+        <v>1</v>
+      </c>
+      <c r="C2442" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="2443" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2443">
+        <v>2022</v>
+      </c>
+      <c r="B2443">
+        <v>1</v>
+      </c>
+      <c r="C2443" s="1">
+        <v>44811</v>
+      </c>
+    </row>
+    <row r="2444" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2444">
+        <v>2022</v>
+      </c>
+      <c r="B2444">
+        <v>1</v>
+      </c>
+      <c r="C2444" s="1">
+        <v>44812</v>
+      </c>
+    </row>
+    <row r="2445" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2445">
+        <v>2022</v>
+      </c>
+      <c r="B2445">
+        <v>1</v>
+      </c>
+      <c r="C2445" s="1">
+        <v>44813</v>
+      </c>
+    </row>
+    <row r="2446" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2446">
+        <v>2022</v>
+      </c>
+      <c r="B2446">
+        <v>1</v>
+      </c>
+      <c r="C2446" s="1">
+        <v>44814</v>
+      </c>
+    </row>
+    <row r="2447" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2447">
+        <v>2022</v>
+      </c>
+      <c r="B2447">
+        <v>1</v>
+      </c>
+      <c r="C2447" s="1">
+        <v>44815</v>
+      </c>
+    </row>
+    <row r="2448" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2448">
+        <v>2022</v>
+      </c>
+      <c r="B2448">
+        <v>1</v>
+      </c>
+      <c r="C2448" s="1">
+        <v>44816</v>
+      </c>
+    </row>
+    <row r="2449" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2449">
+        <v>2022</v>
+      </c>
+      <c r="B2449">
+        <v>1</v>
+      </c>
+      <c r="C2449" s="1">
+        <v>44817</v>
+      </c>
+    </row>
+    <row r="2450" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2450">
+        <v>2022</v>
+      </c>
+      <c r="B2450">
+        <v>1</v>
+      </c>
+      <c r="C2450" s="1">
+        <v>44818</v>
+      </c>
+    </row>
+    <row r="2451" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2451">
+        <v>2022</v>
+      </c>
+      <c r="B2451">
+        <v>1</v>
+      </c>
+      <c r="C2451" s="1">
+        <v>44819</v>
+      </c>
+    </row>
+    <row r="2452" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2452">
+        <v>2022</v>
+      </c>
+      <c r="B2452">
+        <v>1</v>
+      </c>
+      <c r="C2452" s="1">
+        <v>44820</v>
+      </c>
+    </row>
+    <row r="2453" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2453">
+        <v>2022</v>
+      </c>
+      <c r="B2453">
+        <v>1</v>
+      </c>
+      <c r="C2453" s="1">
+        <v>44821</v>
+      </c>
+    </row>
+    <row r="2454" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2454">
+        <v>2022</v>
+      </c>
+      <c r="B2454">
+        <v>1</v>
+      </c>
+      <c r="C2454" s="1">
+        <v>44822</v>
+      </c>
+    </row>
+    <row r="2455" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2455">
+        <v>2022</v>
+      </c>
+      <c r="B2455">
+        <v>1</v>
+      </c>
+      <c r="C2455" s="1">
+        <v>44823</v>
+      </c>
+    </row>
+    <row r="2456" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2456">
+        <v>2022</v>
+      </c>
+      <c r="B2456">
+        <v>1</v>
+      </c>
+      <c r="C2456" s="1">
+        <v>44824</v>
+      </c>
+    </row>
+    <row r="2457" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2457">
+        <v>2022</v>
+      </c>
+      <c r="B2457">
+        <v>1</v>
+      </c>
+      <c r="C2457" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="2458" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2458">
+        <v>2022</v>
+      </c>
+      <c r="B2458">
+        <v>1</v>
+      </c>
+      <c r="C2458" s="1">
+        <v>44826</v>
+      </c>
+    </row>
+    <row r="2459" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2459">
+        <v>2022</v>
+      </c>
+      <c r="B2459">
+        <v>1</v>
+      </c>
+      <c r="C2459" s="1">
+        <v>44827</v>
+      </c>
+    </row>
+    <row r="2460" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2460">
+        <v>2022</v>
+      </c>
+      <c r="B2460">
+        <v>1</v>
+      </c>
+      <c r="C2460" s="1">
+        <v>44828</v>
+      </c>
+    </row>
+    <row r="2461" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2461">
+        <v>2022</v>
+      </c>
+      <c r="B2461">
+        <v>1</v>
+      </c>
+      <c r="C2461" s="1">
+        <v>44829</v>
+      </c>
+    </row>
+    <row r="2462" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2462">
+        <v>2022</v>
+      </c>
+      <c r="B2462">
+        <v>1</v>
+      </c>
+      <c r="C2462" s="1">
+        <v>44830</v>
+      </c>
+    </row>
+    <row r="2463" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2463">
+        <v>2022</v>
+      </c>
+      <c r="B2463">
+        <v>1</v>
+      </c>
+      <c r="C2463" s="1">
+        <v>44831</v>
+      </c>
+    </row>
+    <row r="2464" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2464">
+        <v>2022</v>
+      </c>
+      <c r="B2464">
+        <v>1</v>
+      </c>
+      <c r="C2464" s="1">
+        <v>44832</v>
+      </c>
+    </row>
+    <row r="2465" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2465">
+        <v>2022</v>
+      </c>
+      <c r="B2465">
+        <v>1</v>
+      </c>
+      <c r="C2465" s="1">
+        <v>44833</v>
+      </c>
+    </row>
+    <row r="2466" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2466">
+        <v>2022</v>
+      </c>
+      <c r="B2466">
+        <v>1</v>
+      </c>
+      <c r="C2466" s="1">
+        <v>44834</v>
+      </c>
+    </row>
+    <row r="2467" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2467">
+        <v>2022</v>
+      </c>
+      <c r="B2467">
+        <v>1</v>
+      </c>
+      <c r="C2467" s="1">
+        <v>44835</v>
+      </c>
+    </row>
+    <row r="2468" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2468">
+        <v>2022</v>
+      </c>
+      <c r="B2468">
+        <v>1</v>
+      </c>
+      <c r="C2468" s="1">
+        <v>44836</v>
+      </c>
+    </row>
+    <row r="2469" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2469">
+        <v>2022</v>
+      </c>
+      <c r="B2469">
+        <v>1</v>
+      </c>
+      <c r="C2469" s="1">
+        <v>44837</v>
+      </c>
+    </row>
+    <row r="2470" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2470">
+        <v>2022</v>
+      </c>
+      <c r="B2470">
+        <v>1</v>
+      </c>
+      <c r="C2470" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="2471" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2471">
+        <v>2022</v>
+      </c>
+      <c r="B2471">
+        <v>1</v>
+      </c>
+      <c r="C2471" s="1">
+        <v>44839</v>
+      </c>
+    </row>
+    <row r="2472" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2472">
+        <v>2022</v>
+      </c>
+      <c r="B2472">
+        <v>1</v>
+      </c>
+      <c r="C2472" s="1">
+        <v>44840</v>
+      </c>
+    </row>
+    <row r="2473" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2473">
+        <v>2022</v>
+      </c>
+      <c r="B2473">
+        <v>1</v>
+      </c>
+      <c r="C2473" s="1">
+        <v>44841</v>
+      </c>
+    </row>
+    <row r="2474" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2474">
+        <v>2022</v>
+      </c>
+      <c r="B2474">
+        <v>1</v>
+      </c>
+      <c r="C2474" s="1">
+        <v>44842</v>
+      </c>
+    </row>
+    <row r="2475" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2475">
+        <v>2022</v>
+      </c>
+      <c r="B2475">
+        <v>1</v>
+      </c>
+      <c r="C2475" s="1">
+        <v>44843</v>
+      </c>
+    </row>
+    <row r="2476" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2476">
+        <v>2022</v>
+      </c>
+      <c r="B2476">
+        <v>1</v>
+      </c>
+      <c r="C2476" s="1">
+        <v>44844</v>
+      </c>
+    </row>
+    <row r="2477" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2477">
+        <v>2022</v>
+      </c>
+      <c r="B2477">
+        <v>1</v>
+      </c>
+      <c r="C2477" s="1">
+        <v>44845</v>
+      </c>
+    </row>
+    <row r="2478" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2478">
+        <v>2022</v>
+      </c>
+      <c r="B2478">
+        <v>1</v>
+      </c>
+      <c r="C2478" s="1">
+        <v>44846</v>
+      </c>
+    </row>
+    <row r="2479" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2479">
+        <v>2022</v>
+      </c>
+      <c r="B2479">
+        <v>1</v>
+      </c>
+      <c r="C2479" s="1">
+        <v>44847</v>
+      </c>
+    </row>
+    <row r="2480" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2480">
+        <v>2022</v>
+      </c>
+      <c r="B2480">
+        <v>1</v>
+      </c>
+      <c r="C2480" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="2481" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2481">
+        <v>2022</v>
+      </c>
+      <c r="B2481">
+        <v>1</v>
+      </c>
+      <c r="C2481" s="1">
+        <v>44849</v>
+      </c>
+    </row>
+    <row r="2482" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2482">
+        <v>2022</v>
+      </c>
+      <c r="B2482">
+        <v>1</v>
+      </c>
+      <c r="C2482" s="1">
+        <v>44850</v>
+      </c>
+    </row>
+    <row r="2483" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2483">
+        <v>2022</v>
+      </c>
+      <c r="B2483">
+        <v>1</v>
+      </c>
+      <c r="C2483" s="1">
+        <v>44851</v>
+      </c>
+    </row>
+    <row r="2484" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2484">
+        <v>2022</v>
+      </c>
+      <c r="B2484">
+        <v>1</v>
+      </c>
+      <c r="C2484" s="1">
+        <v>44852</v>
+      </c>
+    </row>
+    <row r="2485" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2485">
+        <v>2022</v>
+      </c>
+      <c r="B2485">
+        <v>1</v>
+      </c>
+      <c r="C2485" s="1">
+        <v>44853</v>
+      </c>
+    </row>
+    <row r="2486" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2486">
+        <v>2022</v>
+      </c>
+      <c r="B2486">
+        <v>1</v>
+      </c>
+      <c r="C2486" s="1">
+        <v>44854</v>
+      </c>
+    </row>
+    <row r="2487" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2487">
+        <v>2022</v>
+      </c>
+      <c r="B2487">
+        <v>1</v>
+      </c>
+      <c r="C2487" s="1">
+        <v>44855</v>
+      </c>
+    </row>
+    <row r="2488" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2488">
+        <v>2022</v>
+      </c>
+      <c r="B2488">
+        <v>1</v>
+      </c>
+      <c r="C2488" s="1">
+        <v>44856</v>
+      </c>
+    </row>
+    <row r="2489" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2489">
+        <v>2022</v>
+      </c>
+      <c r="B2489">
+        <v>1</v>
+      </c>
+      <c r="C2489" s="1">
+        <v>44857</v>
+      </c>
+    </row>
+    <row r="2490" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2490">
+        <v>2022</v>
+      </c>
+      <c r="B2490">
+        <v>1</v>
+      </c>
+      <c r="C2490" s="1">
+        <v>44858</v>
+      </c>
+    </row>
+    <row r="2491" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2491">
+        <v>2022</v>
+      </c>
+      <c r="B2491">
+        <v>1</v>
+      </c>
+      <c r="C2491" s="1">
+        <v>44859</v>
+      </c>
+    </row>
+    <row r="2492" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2492">
+        <v>2022</v>
+      </c>
+      <c r="B2492">
+        <v>1</v>
+      </c>
+      <c r="C2492" s="1">
+        <v>44860</v>
+      </c>
+    </row>
+    <row r="2493" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2493">
+        <v>2022</v>
+      </c>
+      <c r="B2493">
+        <v>1</v>
+      </c>
+      <c r="C2493" s="1">
+        <v>44861</v>
+      </c>
+    </row>
+    <row r="2494" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2494">
+        <v>2022</v>
+      </c>
+      <c r="B2494">
+        <v>1</v>
+      </c>
+      <c r="C2494" s="1">
+        <v>44862</v>
+      </c>
+    </row>
+    <row r="2495" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2495">
+        <v>2022</v>
+      </c>
+      <c r="B2495">
+        <v>1</v>
+      </c>
+      <c r="C2495" s="1">
+        <v>44863</v>
+      </c>
+    </row>
+    <row r="2496" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2496">
+        <v>2022</v>
+      </c>
+      <c r="B2496">
+        <v>1</v>
+      </c>
+      <c r="C2496" s="1">
+        <v>44864</v>
+      </c>
+    </row>
+    <row r="2497" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2497">
+        <v>2022</v>
+      </c>
+      <c r="B2497">
+        <v>1</v>
+      </c>
+      <c r="C2497" s="1">
+        <v>44865</v>
+      </c>
+    </row>
+    <row r="2498" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2498">
+        <v>2022</v>
+      </c>
+      <c r="B2498">
+        <v>1</v>
+      </c>
+      <c r="C2498" s="1">
+        <v>44866</v>
+      </c>
+    </row>
+    <row r="2499" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2499">
+        <v>2022</v>
+      </c>
+      <c r="B2499">
+        <v>1</v>
+      </c>
+      <c r="C2499" s="1">
+        <v>44867</v>
+      </c>
+    </row>
+    <row r="2500" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2500">
+        <v>2022</v>
+      </c>
+      <c r="B2500">
+        <v>1</v>
+      </c>
+      <c r="C2500" s="1">
+        <v>44868</v>
+      </c>
+    </row>
+    <row r="2501" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2501">
+        <v>2022</v>
+      </c>
+      <c r="B2501">
+        <v>1</v>
+      </c>
+      <c r="C2501" s="1">
+        <v>44869</v>
+      </c>
+    </row>
+    <row r="2502" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2502">
+        <v>2022</v>
+      </c>
+      <c r="B2502">
+        <v>1</v>
+      </c>
+      <c r="C2502" s="1">
+        <v>44870</v>
+      </c>
+    </row>
+    <row r="2503" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2503">
+        <v>2022</v>
+      </c>
+      <c r="B2503">
+        <v>1</v>
+      </c>
+      <c r="C2503" s="1">
+        <v>44871</v>
+      </c>
+    </row>
+    <row r="2504" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2504">
+        <v>2022</v>
+      </c>
+      <c r="B2504">
+        <v>1</v>
+      </c>
+      <c r="C2504" s="1">
+        <v>44872</v>
+      </c>
+    </row>
+    <row r="2505" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2505">
+        <v>2022</v>
+      </c>
+      <c r="B2505">
+        <v>1</v>
+      </c>
+      <c r="C2505" s="1">
+        <v>44873</v>
+      </c>
+    </row>
+    <row r="2506" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2506">
+        <v>2022</v>
+      </c>
+      <c r="B2506">
+        <v>1</v>
+      </c>
+      <c r="C2506" s="1">
+        <v>44874</v>
+      </c>
+    </row>
+    <row r="2507" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2507">
+        <v>2022</v>
+      </c>
+      <c r="B2507">
+        <v>1</v>
+      </c>
+      <c r="C2507" s="1">
+        <v>44875</v>
+      </c>
+    </row>
+    <row r="2508" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2508">
+        <v>2022</v>
+      </c>
+      <c r="B2508">
+        <v>1</v>
+      </c>
+      <c r="C2508" s="1">
+        <v>44876</v>
+      </c>
+    </row>
+    <row r="2509" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2509">
+        <v>2022</v>
+      </c>
+      <c r="B2509">
+        <v>1</v>
+      </c>
+      <c r="C2509" s="1">
+        <v>44877</v>
+      </c>
+    </row>
+    <row r="2510" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2510">
+        <v>2022</v>
+      </c>
+      <c r="B2510">
+        <v>1</v>
+      </c>
+      <c r="C2510" s="1">
+        <v>44878</v>
+      </c>
+    </row>
+    <row r="2511" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2511">
+        <v>2022</v>
+      </c>
+      <c r="B2511">
+        <v>1</v>
+      </c>
+      <c r="C2511" s="1">
+        <v>44879</v>
+      </c>
+    </row>
+    <row r="2512" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2512">
+        <v>2022</v>
+      </c>
+      <c r="B2512">
+        <v>1</v>
+      </c>
+      <c r="C2512" s="1">
+        <v>44880</v>
+      </c>
+    </row>
+    <row r="2513" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2513">
+        <v>2022</v>
+      </c>
+      <c r="B2513">
+        <v>1</v>
+      </c>
+      <c r="C2513" s="1">
+        <v>44881</v>
+      </c>
+    </row>
+    <row r="2514" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2514">
+        <v>2022</v>
+      </c>
+      <c r="B2514">
+        <v>1</v>
+      </c>
+      <c r="C2514" s="1">
+        <v>44882</v>
+      </c>
+    </row>
+    <row r="2515" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2515">
+        <v>2022</v>
+      </c>
+      <c r="B2515">
+        <v>1</v>
+      </c>
+      <c r="C2515" s="1">
+        <v>44883</v>
+      </c>
+    </row>
+    <row r="2516" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2516">
+        <v>2022</v>
+      </c>
+      <c r="B2516">
+        <v>1</v>
+      </c>
+      <c r="C2516" s="1">
+        <v>44884</v>
+      </c>
+    </row>
+    <row r="2517" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2517">
+        <v>2022</v>
+      </c>
+      <c r="B2517">
+        <v>1</v>
+      </c>
+      <c r="C2517" s="1">
+        <v>44885</v>
+      </c>
+    </row>
+    <row r="2518" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2518">
+        <v>2022</v>
+      </c>
+      <c r="B2518">
+        <v>1</v>
+      </c>
+      <c r="C2518" s="1">
+        <v>44886</v>
+      </c>
+    </row>
+    <row r="2519" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2519">
+        <v>2022</v>
+      </c>
+      <c r="B2519">
+        <v>1</v>
+      </c>
+      <c r="C2519" s="1">
+        <v>44887</v>
+      </c>
+    </row>
+    <row r="2520" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2520">
+        <v>2022</v>
+      </c>
+      <c r="B2520">
+        <v>1</v>
+      </c>
+      <c r="C2520" s="1">
+        <v>44888</v>
+      </c>
+    </row>
+    <row r="2521" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2521">
+        <v>2022</v>
+      </c>
+      <c r="B2521">
+        <v>1</v>
+      </c>
+      <c r="C2521" s="1">
+        <v>44889</v>
+      </c>
+    </row>
+    <row r="2522" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2522">
+        <v>2022</v>
+      </c>
+      <c r="B2522">
+        <v>1</v>
+      </c>
+      <c r="C2522" s="1">
+        <v>44890</v>
+      </c>
+    </row>
+    <row r="2523" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2523">
+        <v>2022</v>
+      </c>
+      <c r="B2523">
+        <v>1</v>
+      </c>
+      <c r="C2523" s="1">
+        <v>44891</v>
+      </c>
+    </row>
+    <row r="2524" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2524">
+        <v>2022</v>
+      </c>
+      <c r="B2524">
+        <v>1</v>
+      </c>
+      <c r="C2524" s="1">
+        <v>44892</v>
+      </c>
+    </row>
+    <row r="2525" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2525">
+        <v>2022</v>
+      </c>
+      <c r="B2525">
+        <v>1</v>
+      </c>
+      <c r="C2525" s="1">
+        <v>44893</v>
+      </c>
+    </row>
+    <row r="2526" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2526">
+        <v>2022</v>
+      </c>
+      <c r="B2526">
+        <v>1</v>
+      </c>
+      <c r="C2526" s="1">
+        <v>44894</v>
+      </c>
+    </row>
+    <row r="2527" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2527">
+        <v>2022</v>
+      </c>
+      <c r="B2527">
+        <v>1</v>
+      </c>
+      <c r="C2527" s="1">
+        <v>44895</v>
+      </c>
+    </row>
+    <row r="2528" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2528">
+        <v>2022</v>
+      </c>
+      <c r="B2528">
+        <v>1</v>
+      </c>
+      <c r="C2528" s="1">
+        <v>44896</v>
+      </c>
+    </row>
+    <row r="2529" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2529">
+        <v>2022</v>
+      </c>
+      <c r="B2529">
+        <v>1</v>
+      </c>
+      <c r="C2529" s="1">
+        <v>44897</v>
+      </c>
+    </row>
+    <row r="2530" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2530">
+        <v>2022</v>
+      </c>
+      <c r="B2530">
+        <v>1</v>
+      </c>
+      <c r="C2530" s="1">
+        <v>44898</v>
+      </c>
+    </row>
+    <row r="2531" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2531">
+        <v>2022</v>
+      </c>
+      <c r="B2531">
+        <v>1</v>
+      </c>
+      <c r="C2531" s="1">
+        <v>44899</v>
+      </c>
+    </row>
+    <row r="2532" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2532">
+        <v>2022</v>
+      </c>
+      <c r="B2532">
+        <v>1</v>
+      </c>
+      <c r="C2532" s="1">
+        <v>44900</v>
+      </c>
+    </row>
+    <row r="2533" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2533">
+        <v>2022</v>
+      </c>
+      <c r="B2533">
+        <v>1</v>
+      </c>
+      <c r="C2533" s="1">
+        <v>44901</v>
+      </c>
+    </row>
+    <row r="2534" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2534">
+        <v>2022</v>
+      </c>
+      <c r="B2534">
+        <v>1</v>
+      </c>
+      <c r="C2534" s="1">
+        <v>44902</v>
+      </c>
+    </row>
+    <row r="2535" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2535">
+        <v>2022</v>
+      </c>
+      <c r="B2535">
+        <v>1</v>
+      </c>
+      <c r="C2535" s="1">
+        <v>44903</v>
+      </c>
+    </row>
+    <row r="2536" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2536">
+        <v>2022</v>
+      </c>
+      <c r="B2536">
+        <v>1</v>
+      </c>
+      <c r="C2536" s="1">
+        <v>44904</v>
+      </c>
+    </row>
+    <row r="2537" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2537">
+        <v>2022</v>
+      </c>
+      <c r="B2537">
+        <v>1</v>
+      </c>
+      <c r="C2537" s="1">
+        <v>44905</v>
+      </c>
+    </row>
+    <row r="2538" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2538">
+        <v>2022</v>
+      </c>
+      <c r="B2538">
+        <v>1</v>
+      </c>
+      <c r="C2538" s="1">
+        <v>44906</v>
+      </c>
+    </row>
+    <row r="2539" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2539">
+        <v>2022</v>
+      </c>
+      <c r="B2539">
+        <v>1</v>
+      </c>
+      <c r="C2539" s="1">
+        <v>44907</v>
+      </c>
+    </row>
+    <row r="2540" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2540">
+        <v>2022</v>
+      </c>
+      <c r="B2540">
+        <v>1</v>
+      </c>
+      <c r="C2540" s="1">
+        <v>44908</v>
+      </c>
+    </row>
+    <row r="2541" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2541">
+        <v>2022</v>
+      </c>
+      <c r="B2541">
+        <v>1</v>
+      </c>
+      <c r="C2541" s="1">
+        <v>44909</v>
+      </c>
+    </row>
+    <row r="2542" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2542">
+        <v>2022</v>
+      </c>
+      <c r="B2542">
+        <v>1</v>
+      </c>
+      <c r="C2542" s="1">
+        <v>44910</v>
+      </c>
+    </row>
+    <row r="2543" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2543">
+        <v>2022</v>
+      </c>
+      <c r="B2543">
+        <v>1</v>
+      </c>
+      <c r="C2543" s="1">
+        <v>44911</v>
+      </c>
+    </row>
+    <row r="2544" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2544">
+        <v>2022</v>
+      </c>
+      <c r="B2544">
+        <v>1</v>
+      </c>
+      <c r="C2544" s="1">
+        <v>44912</v>
+      </c>
+    </row>
+    <row r="2545" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2545">
+        <v>2022</v>
+      </c>
+      <c r="B2545">
+        <v>1</v>
+      </c>
+      <c r="C2545" s="1">
+        <v>44913</v>
+      </c>
+    </row>
+    <row r="2546" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2546">
+        <v>2022</v>
+      </c>
+      <c r="B2546">
+        <v>1</v>
+      </c>
+      <c r="C2546" s="1">
+        <v>44914</v>
+      </c>
+    </row>
+    <row r="2547" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2547">
+        <v>2022</v>
+      </c>
+      <c r="B2547">
+        <v>1</v>
+      </c>
+      <c r="C2547" s="1">
+        <v>44915</v>
+      </c>
+    </row>
+    <row r="2548" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2548">
+        <v>2022</v>
+      </c>
+      <c r="B2548">
+        <v>1</v>
+      </c>
+      <c r="C2548" s="1">
+        <v>44916</v>
+      </c>
+    </row>
+    <row r="2549" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2549">
+        <v>2022</v>
+      </c>
+      <c r="B2549">
+        <v>1</v>
+      </c>
+      <c r="C2549" s="1">
+        <v>44917</v>
+      </c>
+    </row>
+    <row r="2550" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2550">
+        <v>2022</v>
+      </c>
+      <c r="B2550">
+        <v>1</v>
+      </c>
+      <c r="C2550" s="1">
+        <v>44918</v>
+      </c>
+    </row>
+    <row r="2551" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2551">
+        <v>2022</v>
+      </c>
+      <c r="B2551">
+        <v>1</v>
+      </c>
+      <c r="C2551" s="1">
+        <v>44919</v>
+      </c>
+    </row>
+    <row r="2552" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2552">
+        <v>2022</v>
+      </c>
+      <c r="B2552">
+        <v>1</v>
+      </c>
+      <c r="C2552" s="1">
+        <v>44920</v>
+      </c>
+    </row>
+    <row r="2553" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2553">
+        <v>2022</v>
+      </c>
+      <c r="B2553">
+        <v>1</v>
+      </c>
+      <c r="C2553" s="1">
+        <v>44921</v>
+      </c>
+    </row>
+    <row r="2554" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2554">
+        <v>2022</v>
+      </c>
+      <c r="B2554">
+        <v>1</v>
+      </c>
+      <c r="C2554" s="1">
+        <v>44922</v>
+      </c>
+    </row>
+    <row r="2555" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2555">
+        <v>2022</v>
+      </c>
+      <c r="B2555">
+        <v>1</v>
+      </c>
+      <c r="C2555" s="1">
+        <v>44923</v>
+      </c>
+    </row>
+    <row r="2556" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2556">
+        <v>2022</v>
+      </c>
+      <c r="B2556">
+        <v>1</v>
+      </c>
+      <c r="C2556" s="1">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="2557" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2557">
+        <v>2022</v>
+      </c>
+      <c r="B2557">
+        <v>1</v>
+      </c>
+      <c r="C2557" s="1">
+        <v>44925</v>
+      </c>
+    </row>
+    <row r="2558" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2558">
+        <v>2022</v>
+      </c>
+      <c r="B2558">
+        <v>1</v>
+      </c>
+      <c r="C2558" s="1">
+        <v>44926</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Data updated till 1/6/2022
</commit_message>
<xml_diff>
--- a/data/calendar-dates.xlsx
+++ b/data/calendar-dates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\deqhq1\WQ-Share\Harmful Algal Blooms Coordination Team\HAB_Shiny_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821C519A-B3DF-4F1D-BA18-F7C2C1E91872}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEF6BB3-03E4-463B-A479-B8E01D7457E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -841,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2558"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A1821" workbookViewId="0">
+      <selection activeCell="B2194" sqref="B2194:B2558"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24989,7 +24989,7 @@
         <v>2022</v>
       </c>
       <c r="B2195">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2195" s="1">
         <v>44563</v>
@@ -25000,7 +25000,7 @@
         <v>2022</v>
       </c>
       <c r="B2196">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2196" s="1">
         <v>44564</v>
@@ -25011,7 +25011,7 @@
         <v>2022</v>
       </c>
       <c r="B2197">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2197" s="1">
         <v>44565</v>
@@ -25022,7 +25022,7 @@
         <v>2022</v>
       </c>
       <c r="B2198">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2198" s="1">
         <v>44566</v>
@@ -25033,7 +25033,7 @@
         <v>2022</v>
       </c>
       <c r="B2199">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C2199" s="1">
         <v>44567</v>
@@ -25044,7 +25044,7 @@
         <v>2022</v>
       </c>
       <c r="B2200">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C2200" s="1">
         <v>44568</v>
@@ -25055,7 +25055,7 @@
         <v>2022</v>
       </c>
       <c r="B2201">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C2201" s="1">
         <v>44569</v>
@@ -25066,7 +25066,7 @@
         <v>2022</v>
       </c>
       <c r="B2202">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C2202" s="1">
         <v>44570</v>
@@ -25077,7 +25077,7 @@
         <v>2022</v>
       </c>
       <c r="B2203">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C2203" s="1">
         <v>44571</v>
@@ -25088,7 +25088,7 @@
         <v>2022</v>
       </c>
       <c r="B2204">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C2204" s="1">
         <v>44572</v>
@@ -25099,7 +25099,7 @@
         <v>2022</v>
       </c>
       <c r="B2205">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C2205" s="1">
         <v>44573</v>
@@ -25110,7 +25110,7 @@
         <v>2022</v>
       </c>
       <c r="B2206">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C2206" s="1">
         <v>44574</v>
@@ -25121,7 +25121,7 @@
         <v>2022</v>
       </c>
       <c r="B2207">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C2207" s="1">
         <v>44575</v>
@@ -25132,7 +25132,7 @@
         <v>2022</v>
       </c>
       <c r="B2208">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C2208" s="1">
         <v>44576</v>
@@ -25143,7 +25143,7 @@
         <v>2022</v>
       </c>
       <c r="B2209">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C2209" s="1">
         <v>44577</v>
@@ -25154,7 +25154,7 @@
         <v>2022</v>
       </c>
       <c r="B2210">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C2210" s="1">
         <v>44578</v>
@@ -25165,7 +25165,7 @@
         <v>2022</v>
       </c>
       <c r="B2211">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C2211" s="1">
         <v>44579</v>
@@ -25176,7 +25176,7 @@
         <v>2022</v>
       </c>
       <c r="B2212">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C2212" s="1">
         <v>44580</v>
@@ -25187,7 +25187,7 @@
         <v>2022</v>
       </c>
       <c r="B2213">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C2213" s="1">
         <v>44581</v>
@@ -25198,7 +25198,7 @@
         <v>2022</v>
       </c>
       <c r="B2214">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C2214" s="1">
         <v>44582</v>
@@ -25209,7 +25209,7 @@
         <v>2022</v>
       </c>
       <c r="B2215">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C2215" s="1">
         <v>44583</v>
@@ -25220,7 +25220,7 @@
         <v>2022</v>
       </c>
       <c r="B2216">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C2216" s="1">
         <v>44584</v>
@@ -25231,7 +25231,7 @@
         <v>2022</v>
       </c>
       <c r="B2217">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C2217" s="1">
         <v>44585</v>
@@ -25242,7 +25242,7 @@
         <v>2022</v>
       </c>
       <c r="B2218">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C2218" s="1">
         <v>44586</v>
@@ -25253,7 +25253,7 @@
         <v>2022</v>
       </c>
       <c r="B2219">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C2219" s="1">
         <v>44587</v>
@@ -25264,7 +25264,7 @@
         <v>2022</v>
       </c>
       <c r="B2220">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C2220" s="1">
         <v>44588</v>
@@ -25275,7 +25275,7 @@
         <v>2022</v>
       </c>
       <c r="B2221">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C2221" s="1">
         <v>44589</v>
@@ -25286,7 +25286,7 @@
         <v>2022</v>
       </c>
       <c r="B2222">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C2222" s="1">
         <v>44590</v>
@@ -25297,7 +25297,7 @@
         <v>2022</v>
       </c>
       <c r="B2223">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C2223" s="1">
         <v>44591</v>
@@ -25308,7 +25308,7 @@
         <v>2022</v>
       </c>
       <c r="B2224">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C2224" s="1">
         <v>44592</v>
@@ -25319,7 +25319,7 @@
         <v>2022</v>
       </c>
       <c r="B2225">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="C2225" s="1">
         <v>44593</v>
@@ -25330,7 +25330,7 @@
         <v>2022</v>
       </c>
       <c r="B2226">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="C2226" s="1">
         <v>44594</v>
@@ -25341,7 +25341,7 @@
         <v>2022</v>
       </c>
       <c r="B2227">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C2227" s="1">
         <v>44595</v>
@@ -25352,7 +25352,7 @@
         <v>2022</v>
       </c>
       <c r="B2228">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="C2228" s="1">
         <v>44596</v>
@@ -25363,7 +25363,7 @@
         <v>2022</v>
       </c>
       <c r="B2229">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C2229" s="1">
         <v>44597</v>
@@ -25374,7 +25374,7 @@
         <v>2022</v>
       </c>
       <c r="B2230">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="C2230" s="1">
         <v>44598</v>
@@ -25385,7 +25385,7 @@
         <v>2022</v>
       </c>
       <c r="B2231">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C2231" s="1">
         <v>44599</v>
@@ -25396,7 +25396,7 @@
         <v>2022</v>
       </c>
       <c r="B2232">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="C2232" s="1">
         <v>44600</v>
@@ -25407,7 +25407,7 @@
         <v>2022</v>
       </c>
       <c r="B2233">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="C2233" s="1">
         <v>44601</v>
@@ -25418,7 +25418,7 @@
         <v>2022</v>
       </c>
       <c r="B2234">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="C2234" s="1">
         <v>44602</v>
@@ -25429,7 +25429,7 @@
         <v>2022</v>
       </c>
       <c r="B2235">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="C2235" s="1">
         <v>44603</v>
@@ -25440,7 +25440,7 @@
         <v>2022</v>
       </c>
       <c r="B2236">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="C2236" s="1">
         <v>44604</v>
@@ -25451,7 +25451,7 @@
         <v>2022</v>
       </c>
       <c r="B2237">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="C2237" s="1">
         <v>44605</v>
@@ -25462,7 +25462,7 @@
         <v>2022</v>
       </c>
       <c r="B2238">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C2238" s="1">
         <v>44606</v>
@@ -25473,7 +25473,7 @@
         <v>2022</v>
       </c>
       <c r="B2239">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="C2239" s="1">
         <v>44607</v>
@@ -25484,7 +25484,7 @@
         <v>2022</v>
       </c>
       <c r="B2240">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C2240" s="1">
         <v>44608</v>
@@ -25495,7 +25495,7 @@
         <v>2022</v>
       </c>
       <c r="B2241">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="C2241" s="1">
         <v>44609</v>
@@ -25506,7 +25506,7 @@
         <v>2022</v>
       </c>
       <c r="B2242">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="C2242" s="1">
         <v>44610</v>
@@ -25517,7 +25517,7 @@
         <v>2022</v>
       </c>
       <c r="B2243">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C2243" s="1">
         <v>44611</v>
@@ -25528,7 +25528,7 @@
         <v>2022</v>
       </c>
       <c r="B2244">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="C2244" s="1">
         <v>44612</v>
@@ -25539,7 +25539,7 @@
         <v>2022</v>
       </c>
       <c r="B2245">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="C2245" s="1">
         <v>44613</v>
@@ -25550,7 +25550,7 @@
         <v>2022</v>
       </c>
       <c r="B2246">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C2246" s="1">
         <v>44614</v>
@@ -25561,7 +25561,7 @@
         <v>2022</v>
       </c>
       <c r="B2247">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="C2247" s="1">
         <v>44615</v>
@@ -25572,7 +25572,7 @@
         <v>2022</v>
       </c>
       <c r="B2248">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="C2248" s="1">
         <v>44616</v>
@@ -25583,7 +25583,7 @@
         <v>2022</v>
       </c>
       <c r="B2249">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="C2249" s="1">
         <v>44617</v>
@@ -25594,7 +25594,7 @@
         <v>2022</v>
       </c>
       <c r="B2250">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C2250" s="1">
         <v>44618</v>
@@ -25605,7 +25605,7 @@
         <v>2022</v>
       </c>
       <c r="B2251">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="C2251" s="1">
         <v>44619</v>
@@ -25616,7 +25616,7 @@
         <v>2022</v>
       </c>
       <c r="B2252">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="C2252" s="1">
         <v>44620</v>
@@ -25627,7 +25627,7 @@
         <v>2022</v>
       </c>
       <c r="B2253">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="C2253" s="1">
         <v>44621</v>
@@ -25638,7 +25638,7 @@
         <v>2022</v>
       </c>
       <c r="B2254">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="C2254" s="1">
         <v>44622</v>
@@ -25649,7 +25649,7 @@
         <v>2022</v>
       </c>
       <c r="B2255">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="C2255" s="1">
         <v>44623</v>
@@ -25660,7 +25660,7 @@
         <v>2022</v>
       </c>
       <c r="B2256">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="C2256" s="1">
         <v>44624</v>
@@ -25671,7 +25671,7 @@
         <v>2022</v>
       </c>
       <c r="B2257">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="C2257" s="1">
         <v>44625</v>
@@ -25682,7 +25682,7 @@
         <v>2022</v>
       </c>
       <c r="B2258">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="C2258" s="1">
         <v>44626</v>
@@ -25693,7 +25693,7 @@
         <v>2022</v>
       </c>
       <c r="B2259">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="C2259" s="1">
         <v>44627</v>
@@ -25704,7 +25704,7 @@
         <v>2022</v>
       </c>
       <c r="B2260">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="C2260" s="1">
         <v>44628</v>
@@ -25715,7 +25715,7 @@
         <v>2022</v>
       </c>
       <c r="B2261">
-        <v>1</v>
+        <v>68</v>
       </c>
       <c r="C2261" s="1">
         <v>44629</v>
@@ -25726,7 +25726,7 @@
         <v>2022</v>
       </c>
       <c r="B2262">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="C2262" s="1">
         <v>44630</v>
@@ -25737,7 +25737,7 @@
         <v>2022</v>
       </c>
       <c r="B2263">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="C2263" s="1">
         <v>44631</v>
@@ -25748,7 +25748,7 @@
         <v>2022</v>
       </c>
       <c r="B2264">
-        <v>1</v>
+        <v>71</v>
       </c>
       <c r="C2264" s="1">
         <v>44632</v>
@@ -25759,7 +25759,7 @@
         <v>2022</v>
       </c>
       <c r="B2265">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="C2265" s="1">
         <v>44633</v>
@@ -25770,7 +25770,7 @@
         <v>2022</v>
       </c>
       <c r="B2266">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="C2266" s="1">
         <v>44634</v>
@@ -25781,7 +25781,7 @@
         <v>2022</v>
       </c>
       <c r="B2267">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="C2267" s="1">
         <v>44635</v>
@@ -25792,7 +25792,7 @@
         <v>2022</v>
       </c>
       <c r="B2268">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="C2268" s="1">
         <v>44636</v>
@@ -25803,7 +25803,7 @@
         <v>2022</v>
       </c>
       <c r="B2269">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="C2269" s="1">
         <v>44637</v>
@@ -25814,7 +25814,7 @@
         <v>2022</v>
       </c>
       <c r="B2270">
-        <v>1</v>
+        <v>77</v>
       </c>
       <c r="C2270" s="1">
         <v>44638</v>
@@ -25825,7 +25825,7 @@
         <v>2022</v>
       </c>
       <c r="B2271">
-        <v>1</v>
+        <v>78</v>
       </c>
       <c r="C2271" s="1">
         <v>44639</v>
@@ -25836,7 +25836,7 @@
         <v>2022</v>
       </c>
       <c r="B2272">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C2272" s="1">
         <v>44640</v>
@@ -25847,7 +25847,7 @@
         <v>2022</v>
       </c>
       <c r="B2273">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="C2273" s="1">
         <v>44641</v>
@@ -25858,7 +25858,7 @@
         <v>2022</v>
       </c>
       <c r="B2274">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="C2274" s="1">
         <v>44642</v>
@@ -25869,7 +25869,7 @@
         <v>2022</v>
       </c>
       <c r="B2275">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C2275" s="1">
         <v>44643</v>
@@ -25880,7 +25880,7 @@
         <v>2022</v>
       </c>
       <c r="B2276">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="C2276" s="1">
         <v>44644</v>
@@ -25891,7 +25891,7 @@
         <v>2022</v>
       </c>
       <c r="B2277">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="C2277" s="1">
         <v>44645</v>
@@ -25902,7 +25902,7 @@
         <v>2022</v>
       </c>
       <c r="B2278">
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="C2278" s="1">
         <v>44646</v>
@@ -25913,7 +25913,7 @@
         <v>2022</v>
       </c>
       <c r="B2279">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="C2279" s="1">
         <v>44647</v>
@@ -25924,7 +25924,7 @@
         <v>2022</v>
       </c>
       <c r="B2280">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C2280" s="1">
         <v>44648</v>
@@ -25935,7 +25935,7 @@
         <v>2022</v>
       </c>
       <c r="B2281">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="C2281" s="1">
         <v>44649</v>
@@ -25946,7 +25946,7 @@
         <v>2022</v>
       </c>
       <c r="B2282">
-        <v>1</v>
+        <v>89</v>
       </c>
       <c r="C2282" s="1">
         <v>44650</v>
@@ -25957,7 +25957,7 @@
         <v>2022</v>
       </c>
       <c r="B2283">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="C2283" s="1">
         <v>44651</v>
@@ -25968,7 +25968,7 @@
         <v>2022</v>
       </c>
       <c r="B2284">
-        <v>1</v>
+        <v>91</v>
       </c>
       <c r="C2284" s="1">
         <v>44652</v>
@@ -25979,7 +25979,7 @@
         <v>2022</v>
       </c>
       <c r="B2285">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="C2285" s="1">
         <v>44653</v>
@@ -25990,7 +25990,7 @@
         <v>2022</v>
       </c>
       <c r="B2286">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="C2286" s="1">
         <v>44654</v>
@@ -26001,7 +26001,7 @@
         <v>2022</v>
       </c>
       <c r="B2287">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="C2287" s="1">
         <v>44655</v>
@@ -26012,7 +26012,7 @@
         <v>2022</v>
       </c>
       <c r="B2288">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="C2288" s="1">
         <v>44656</v>
@@ -26023,7 +26023,7 @@
         <v>2022</v>
       </c>
       <c r="B2289">
-        <v>1</v>
+        <v>96</v>
       </c>
       <c r="C2289" s="1">
         <v>44657</v>
@@ -26034,7 +26034,7 @@
         <v>2022</v>
       </c>
       <c r="B2290">
-        <v>1</v>
+        <v>97</v>
       </c>
       <c r="C2290" s="1">
         <v>44658</v>
@@ -26045,7 +26045,7 @@
         <v>2022</v>
       </c>
       <c r="B2291">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="C2291" s="1">
         <v>44659</v>
@@ -26056,7 +26056,7 @@
         <v>2022</v>
       </c>
       <c r="B2292">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="C2292" s="1">
         <v>44660</v>
@@ -26067,7 +26067,7 @@
         <v>2022</v>
       </c>
       <c r="B2293">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C2293" s="1">
         <v>44661</v>
@@ -26078,7 +26078,7 @@
         <v>2022</v>
       </c>
       <c r="B2294">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C2294" s="1">
         <v>44662</v>
@@ -26089,7 +26089,7 @@
         <v>2022</v>
       </c>
       <c r="B2295">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C2295" s="1">
         <v>44663</v>
@@ -26100,7 +26100,7 @@
         <v>2022</v>
       </c>
       <c r="B2296">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="C2296" s="1">
         <v>44664</v>
@@ -26111,7 +26111,7 @@
         <v>2022</v>
       </c>
       <c r="B2297">
-        <v>1</v>
+        <v>104</v>
       </c>
       <c r="C2297" s="1">
         <v>44665</v>
@@ -26122,7 +26122,7 @@
         <v>2022</v>
       </c>
       <c r="B2298">
-        <v>1</v>
+        <v>105</v>
       </c>
       <c r="C2298" s="1">
         <v>44666</v>
@@ -26133,7 +26133,7 @@
         <v>2022</v>
       </c>
       <c r="B2299">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="C2299" s="1">
         <v>44667</v>
@@ -26144,7 +26144,7 @@
         <v>2022</v>
       </c>
       <c r="B2300">
-        <v>1</v>
+        <v>107</v>
       </c>
       <c r="C2300" s="1">
         <v>44668</v>
@@ -26155,7 +26155,7 @@
         <v>2022</v>
       </c>
       <c r="B2301">
-        <v>1</v>
+        <v>108</v>
       </c>
       <c r="C2301" s="1">
         <v>44669</v>
@@ -26166,7 +26166,7 @@
         <v>2022</v>
       </c>
       <c r="B2302">
-        <v>1</v>
+        <v>109</v>
       </c>
       <c r="C2302" s="1">
         <v>44670</v>
@@ -26177,7 +26177,7 @@
         <v>2022</v>
       </c>
       <c r="B2303">
-        <v>1</v>
+        <v>110</v>
       </c>
       <c r="C2303" s="1">
         <v>44671</v>
@@ -26188,7 +26188,7 @@
         <v>2022</v>
       </c>
       <c r="B2304">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="C2304" s="1">
         <v>44672</v>
@@ -26199,7 +26199,7 @@
         <v>2022</v>
       </c>
       <c r="B2305">
-        <v>1</v>
+        <v>112</v>
       </c>
       <c r="C2305" s="1">
         <v>44673</v>
@@ -26210,7 +26210,7 @@
         <v>2022</v>
       </c>
       <c r="B2306">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="C2306" s="1">
         <v>44674</v>
@@ -26221,7 +26221,7 @@
         <v>2022</v>
       </c>
       <c r="B2307">
-        <v>1</v>
+        <v>114</v>
       </c>
       <c r="C2307" s="1">
         <v>44675</v>
@@ -26232,7 +26232,7 @@
         <v>2022</v>
       </c>
       <c r="B2308">
-        <v>1</v>
+        <v>115</v>
       </c>
       <c r="C2308" s="1">
         <v>44676</v>
@@ -26243,7 +26243,7 @@
         <v>2022</v>
       </c>
       <c r="B2309">
-        <v>1</v>
+        <v>116</v>
       </c>
       <c r="C2309" s="1">
         <v>44677</v>
@@ -26254,7 +26254,7 @@
         <v>2022</v>
       </c>
       <c r="B2310">
-        <v>1</v>
+        <v>117</v>
       </c>
       <c r="C2310" s="1">
         <v>44678</v>
@@ -26265,7 +26265,7 @@
         <v>2022</v>
       </c>
       <c r="B2311">
-        <v>1</v>
+        <v>118</v>
       </c>
       <c r="C2311" s="1">
         <v>44679</v>
@@ -26276,7 +26276,7 @@
         <v>2022</v>
       </c>
       <c r="B2312">
-        <v>1</v>
+        <v>119</v>
       </c>
       <c r="C2312" s="1">
         <v>44680</v>
@@ -26287,7 +26287,7 @@
         <v>2022</v>
       </c>
       <c r="B2313">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="C2313" s="1">
         <v>44681</v>
@@ -26298,7 +26298,7 @@
         <v>2022</v>
       </c>
       <c r="B2314">
-        <v>1</v>
+        <v>121</v>
       </c>
       <c r="C2314" s="1">
         <v>44682</v>
@@ -26309,7 +26309,7 @@
         <v>2022</v>
       </c>
       <c r="B2315">
-        <v>1</v>
+        <v>122</v>
       </c>
       <c r="C2315" s="1">
         <v>44683</v>
@@ -26320,7 +26320,7 @@
         <v>2022</v>
       </c>
       <c r="B2316">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="C2316" s="1">
         <v>44684</v>
@@ -26331,7 +26331,7 @@
         <v>2022</v>
       </c>
       <c r="B2317">
-        <v>1</v>
+        <v>124</v>
       </c>
       <c r="C2317" s="1">
         <v>44685</v>
@@ -26342,7 +26342,7 @@
         <v>2022</v>
       </c>
       <c r="B2318">
-        <v>1</v>
+        <v>125</v>
       </c>
       <c r="C2318" s="1">
         <v>44686</v>
@@ -26353,7 +26353,7 @@
         <v>2022</v>
       </c>
       <c r="B2319">
-        <v>1</v>
+        <v>126</v>
       </c>
       <c r="C2319" s="1">
         <v>44687</v>
@@ -26364,7 +26364,7 @@
         <v>2022</v>
       </c>
       <c r="B2320">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C2320" s="1">
         <v>44688</v>
@@ -26375,7 +26375,7 @@
         <v>2022</v>
       </c>
       <c r="B2321">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="C2321" s="1">
         <v>44689</v>
@@ -26386,7 +26386,7 @@
         <v>2022</v>
       </c>
       <c r="B2322">
-        <v>1</v>
+        <v>129</v>
       </c>
       <c r="C2322" s="1">
         <v>44690</v>
@@ -26397,7 +26397,7 @@
         <v>2022</v>
       </c>
       <c r="B2323">
-        <v>1</v>
+        <v>130</v>
       </c>
       <c r="C2323" s="1">
         <v>44691</v>
@@ -26408,7 +26408,7 @@
         <v>2022</v>
       </c>
       <c r="B2324">
-        <v>1</v>
+        <v>131</v>
       </c>
       <c r="C2324" s="1">
         <v>44692</v>
@@ -26419,7 +26419,7 @@
         <v>2022</v>
       </c>
       <c r="B2325">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="C2325" s="1">
         <v>44693</v>
@@ -26430,7 +26430,7 @@
         <v>2022</v>
       </c>
       <c r="B2326">
-        <v>1</v>
+        <v>133</v>
       </c>
       <c r="C2326" s="1">
         <v>44694</v>
@@ -26441,7 +26441,7 @@
         <v>2022</v>
       </c>
       <c r="B2327">
-        <v>1</v>
+        <v>134</v>
       </c>
       <c r="C2327" s="1">
         <v>44695</v>
@@ -26452,7 +26452,7 @@
         <v>2022</v>
       </c>
       <c r="B2328">
-        <v>1</v>
+        <v>135</v>
       </c>
       <c r="C2328" s="1">
         <v>44696</v>
@@ -26463,7 +26463,7 @@
         <v>2022</v>
       </c>
       <c r="B2329">
-        <v>1</v>
+        <v>136</v>
       </c>
       <c r="C2329" s="1">
         <v>44697</v>
@@ -26474,7 +26474,7 @@
         <v>2022</v>
       </c>
       <c r="B2330">
-        <v>1</v>
+        <v>137</v>
       </c>
       <c r="C2330" s="1">
         <v>44698</v>
@@ -26485,7 +26485,7 @@
         <v>2022</v>
       </c>
       <c r="B2331">
-        <v>1</v>
+        <v>138</v>
       </c>
       <c r="C2331" s="1">
         <v>44699</v>
@@ -26496,7 +26496,7 @@
         <v>2022</v>
       </c>
       <c r="B2332">
-        <v>1</v>
+        <v>139</v>
       </c>
       <c r="C2332" s="1">
         <v>44700</v>
@@ -26507,7 +26507,7 @@
         <v>2022</v>
       </c>
       <c r="B2333">
-        <v>1</v>
+        <v>140</v>
       </c>
       <c r="C2333" s="1">
         <v>44701</v>
@@ -26518,7 +26518,7 @@
         <v>2022</v>
       </c>
       <c r="B2334">
-        <v>1</v>
+        <v>141</v>
       </c>
       <c r="C2334" s="1">
         <v>44702</v>
@@ -26529,7 +26529,7 @@
         <v>2022</v>
       </c>
       <c r="B2335">
-        <v>1</v>
+        <v>142</v>
       </c>
       <c r="C2335" s="1">
         <v>44703</v>
@@ -26540,7 +26540,7 @@
         <v>2022</v>
       </c>
       <c r="B2336">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="C2336" s="1">
         <v>44704</v>
@@ -26551,7 +26551,7 @@
         <v>2022</v>
       </c>
       <c r="B2337">
-        <v>1</v>
+        <v>144</v>
       </c>
       <c r="C2337" s="1">
         <v>44705</v>
@@ -26562,7 +26562,7 @@
         <v>2022</v>
       </c>
       <c r="B2338">
-        <v>1</v>
+        <v>145</v>
       </c>
       <c r="C2338" s="1">
         <v>44706</v>
@@ -26573,7 +26573,7 @@
         <v>2022</v>
       </c>
       <c r="B2339">
-        <v>1</v>
+        <v>146</v>
       </c>
       <c r="C2339" s="1">
         <v>44707</v>
@@ -26584,7 +26584,7 @@
         <v>2022</v>
       </c>
       <c r="B2340">
-        <v>1</v>
+        <v>147</v>
       </c>
       <c r="C2340" s="1">
         <v>44708</v>
@@ -26595,7 +26595,7 @@
         <v>2022</v>
       </c>
       <c r="B2341">
-        <v>1</v>
+        <v>148</v>
       </c>
       <c r="C2341" s="1">
         <v>44709</v>
@@ -26606,7 +26606,7 @@
         <v>2022</v>
       </c>
       <c r="B2342">
-        <v>1</v>
+        <v>149</v>
       </c>
       <c r="C2342" s="1">
         <v>44710</v>
@@ -26617,7 +26617,7 @@
         <v>2022</v>
       </c>
       <c r="B2343">
-        <v>1</v>
+        <v>150</v>
       </c>
       <c r="C2343" s="1">
         <v>44711</v>
@@ -26628,7 +26628,7 @@
         <v>2022</v>
       </c>
       <c r="B2344">
-        <v>1</v>
+        <v>151</v>
       </c>
       <c r="C2344" s="1">
         <v>44712</v>
@@ -26639,7 +26639,7 @@
         <v>2022</v>
       </c>
       <c r="B2345">
-        <v>1</v>
+        <v>152</v>
       </c>
       <c r="C2345" s="1">
         <v>44713</v>
@@ -26650,7 +26650,7 @@
         <v>2022</v>
       </c>
       <c r="B2346">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="C2346" s="1">
         <v>44714</v>
@@ -26661,7 +26661,7 @@
         <v>2022</v>
       </c>
       <c r="B2347">
-        <v>1</v>
+        <v>154</v>
       </c>
       <c r="C2347" s="1">
         <v>44715</v>
@@ -26672,7 +26672,7 @@
         <v>2022</v>
       </c>
       <c r="B2348">
-        <v>1</v>
+        <v>155</v>
       </c>
       <c r="C2348" s="1">
         <v>44716</v>
@@ -26683,7 +26683,7 @@
         <v>2022</v>
       </c>
       <c r="B2349">
-        <v>1</v>
+        <v>156</v>
       </c>
       <c r="C2349" s="1">
         <v>44717</v>
@@ -26694,7 +26694,7 @@
         <v>2022</v>
       </c>
       <c r="B2350">
-        <v>1</v>
+        <v>157</v>
       </c>
       <c r="C2350" s="1">
         <v>44718</v>
@@ -26705,7 +26705,7 @@
         <v>2022</v>
       </c>
       <c r="B2351">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c r="C2351" s="1">
         <v>44719</v>
@@ -26716,7 +26716,7 @@
         <v>2022</v>
       </c>
       <c r="B2352">
-        <v>1</v>
+        <v>159</v>
       </c>
       <c r="C2352" s="1">
         <v>44720</v>
@@ -26727,7 +26727,7 @@
         <v>2022</v>
       </c>
       <c r="B2353">
-        <v>1</v>
+        <v>160</v>
       </c>
       <c r="C2353" s="1">
         <v>44721</v>
@@ -26738,7 +26738,7 @@
         <v>2022</v>
       </c>
       <c r="B2354">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="C2354" s="1">
         <v>44722</v>
@@ -26749,7 +26749,7 @@
         <v>2022</v>
       </c>
       <c r="B2355">
-        <v>1</v>
+        <v>162</v>
       </c>
       <c r="C2355" s="1">
         <v>44723</v>
@@ -26760,7 +26760,7 @@
         <v>2022</v>
       </c>
       <c r="B2356">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="C2356" s="1">
         <v>44724</v>
@@ -26771,7 +26771,7 @@
         <v>2022</v>
       </c>
       <c r="B2357">
-        <v>1</v>
+        <v>164</v>
       </c>
       <c r="C2357" s="1">
         <v>44725</v>
@@ -26782,7 +26782,7 @@
         <v>2022</v>
       </c>
       <c r="B2358">
-        <v>1</v>
+        <v>165</v>
       </c>
       <c r="C2358" s="1">
         <v>44726</v>
@@ -26793,7 +26793,7 @@
         <v>2022</v>
       </c>
       <c r="B2359">
-        <v>1</v>
+        <v>166</v>
       </c>
       <c r="C2359" s="1">
         <v>44727</v>
@@ -26804,7 +26804,7 @@
         <v>2022</v>
       </c>
       <c r="B2360">
-        <v>1</v>
+        <v>167</v>
       </c>
       <c r="C2360" s="1">
         <v>44728</v>
@@ -26815,7 +26815,7 @@
         <v>2022</v>
       </c>
       <c r="B2361">
-        <v>1</v>
+        <v>168</v>
       </c>
       <c r="C2361" s="1">
         <v>44729</v>
@@ -26826,7 +26826,7 @@
         <v>2022</v>
       </c>
       <c r="B2362">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="C2362" s="1">
         <v>44730</v>
@@ -26837,7 +26837,7 @@
         <v>2022</v>
       </c>
       <c r="B2363">
-        <v>1</v>
+        <v>170</v>
       </c>
       <c r="C2363" s="1">
         <v>44731</v>
@@ -26848,7 +26848,7 @@
         <v>2022</v>
       </c>
       <c r="B2364">
-        <v>1</v>
+        <v>171</v>
       </c>
       <c r="C2364" s="1">
         <v>44732</v>
@@ -26859,7 +26859,7 @@
         <v>2022</v>
       </c>
       <c r="B2365">
-        <v>1</v>
+        <v>172</v>
       </c>
       <c r="C2365" s="1">
         <v>44733</v>
@@ -26870,7 +26870,7 @@
         <v>2022</v>
       </c>
       <c r="B2366">
-        <v>1</v>
+        <v>173</v>
       </c>
       <c r="C2366" s="1">
         <v>44734</v>
@@ -26881,7 +26881,7 @@
         <v>2022</v>
       </c>
       <c r="B2367">
-        <v>1</v>
+        <v>174</v>
       </c>
       <c r="C2367" s="1">
         <v>44735</v>
@@ -26892,7 +26892,7 @@
         <v>2022</v>
       </c>
       <c r="B2368">
-        <v>1</v>
+        <v>175</v>
       </c>
       <c r="C2368" s="1">
         <v>44736</v>
@@ -26903,7 +26903,7 @@
         <v>2022</v>
       </c>
       <c r="B2369">
-        <v>1</v>
+        <v>176</v>
       </c>
       <c r="C2369" s="1">
         <v>44737</v>
@@ -26914,7 +26914,7 @@
         <v>2022</v>
       </c>
       <c r="B2370">
-        <v>1</v>
+        <v>177</v>
       </c>
       <c r="C2370" s="1">
         <v>44738</v>
@@ -26925,7 +26925,7 @@
         <v>2022</v>
       </c>
       <c r="B2371">
-        <v>1</v>
+        <v>178</v>
       </c>
       <c r="C2371" s="1">
         <v>44739</v>
@@ -26936,7 +26936,7 @@
         <v>2022</v>
       </c>
       <c r="B2372">
-        <v>1</v>
+        <v>179</v>
       </c>
       <c r="C2372" s="1">
         <v>44740</v>
@@ -26947,7 +26947,7 @@
         <v>2022</v>
       </c>
       <c r="B2373">
-        <v>1</v>
+        <v>180</v>
       </c>
       <c r="C2373" s="1">
         <v>44741</v>
@@ -26958,7 +26958,7 @@
         <v>2022</v>
       </c>
       <c r="B2374">
-        <v>1</v>
+        <v>181</v>
       </c>
       <c r="C2374" s="1">
         <v>44742</v>
@@ -26969,7 +26969,7 @@
         <v>2022</v>
       </c>
       <c r="B2375">
-        <v>1</v>
+        <v>182</v>
       </c>
       <c r="C2375" s="1">
         <v>44743</v>
@@ -26980,7 +26980,7 @@
         <v>2022</v>
       </c>
       <c r="B2376">
-        <v>1</v>
+        <v>183</v>
       </c>
       <c r="C2376" s="1">
         <v>44744</v>
@@ -26991,7 +26991,7 @@
         <v>2022</v>
       </c>
       <c r="B2377">
-        <v>1</v>
+        <v>184</v>
       </c>
       <c r="C2377" s="1">
         <v>44745</v>
@@ -27002,7 +27002,7 @@
         <v>2022</v>
       </c>
       <c r="B2378">
-        <v>1</v>
+        <v>185</v>
       </c>
       <c r="C2378" s="1">
         <v>44746</v>
@@ -27013,7 +27013,7 @@
         <v>2022</v>
       </c>
       <c r="B2379">
-        <v>1</v>
+        <v>186</v>
       </c>
       <c r="C2379" s="1">
         <v>44747</v>
@@ -27024,7 +27024,7 @@
         <v>2022</v>
       </c>
       <c r="B2380">
-        <v>1</v>
+        <v>187</v>
       </c>
       <c r="C2380" s="1">
         <v>44748</v>
@@ -27035,7 +27035,7 @@
         <v>2022</v>
       </c>
       <c r="B2381">
-        <v>1</v>
+        <v>188</v>
       </c>
       <c r="C2381" s="1">
         <v>44749</v>
@@ -27046,7 +27046,7 @@
         <v>2022</v>
       </c>
       <c r="B2382">
-        <v>1</v>
+        <v>189</v>
       </c>
       <c r="C2382" s="1">
         <v>44750</v>
@@ -27057,7 +27057,7 @@
         <v>2022</v>
       </c>
       <c r="B2383">
-        <v>1</v>
+        <v>190</v>
       </c>
       <c r="C2383" s="1">
         <v>44751</v>
@@ -27068,7 +27068,7 @@
         <v>2022</v>
       </c>
       <c r="B2384">
-        <v>1</v>
+        <v>191</v>
       </c>
       <c r="C2384" s="1">
         <v>44752</v>
@@ -27079,7 +27079,7 @@
         <v>2022</v>
       </c>
       <c r="B2385">
-        <v>1</v>
+        <v>192</v>
       </c>
       <c r="C2385" s="1">
         <v>44753</v>
@@ -27090,7 +27090,7 @@
         <v>2022</v>
       </c>
       <c r="B2386">
-        <v>1</v>
+        <v>193</v>
       </c>
       <c r="C2386" s="1">
         <v>44754</v>
@@ -27101,7 +27101,7 @@
         <v>2022</v>
       </c>
       <c r="B2387">
-        <v>1</v>
+        <v>194</v>
       </c>
       <c r="C2387" s="1">
         <v>44755</v>
@@ -27112,7 +27112,7 @@
         <v>2022</v>
       </c>
       <c r="B2388">
-        <v>1</v>
+        <v>195</v>
       </c>
       <c r="C2388" s="1">
         <v>44756</v>
@@ -27123,7 +27123,7 @@
         <v>2022</v>
       </c>
       <c r="B2389">
-        <v>1</v>
+        <v>196</v>
       </c>
       <c r="C2389" s="1">
         <v>44757</v>
@@ -27134,7 +27134,7 @@
         <v>2022</v>
       </c>
       <c r="B2390">
-        <v>1</v>
+        <v>197</v>
       </c>
       <c r="C2390" s="1">
         <v>44758</v>
@@ -27145,7 +27145,7 @@
         <v>2022</v>
       </c>
       <c r="B2391">
-        <v>1</v>
+        <v>198</v>
       </c>
       <c r="C2391" s="1">
         <v>44759</v>
@@ -27156,7 +27156,7 @@
         <v>2022</v>
       </c>
       <c r="B2392">
-        <v>1</v>
+        <v>199</v>
       </c>
       <c r="C2392" s="1">
         <v>44760</v>
@@ -27167,7 +27167,7 @@
         <v>2022</v>
       </c>
       <c r="B2393">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="C2393" s="1">
         <v>44761</v>
@@ -27178,7 +27178,7 @@
         <v>2022</v>
       </c>
       <c r="B2394">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="C2394" s="1">
         <v>44762</v>
@@ -27189,7 +27189,7 @@
         <v>2022</v>
       </c>
       <c r="B2395">
-        <v>1</v>
+        <v>202</v>
       </c>
       <c r="C2395" s="1">
         <v>44763</v>
@@ -27200,7 +27200,7 @@
         <v>2022</v>
       </c>
       <c r="B2396">
-        <v>1</v>
+        <v>203</v>
       </c>
       <c r="C2396" s="1">
         <v>44764</v>
@@ -27211,7 +27211,7 @@
         <v>2022</v>
       </c>
       <c r="B2397">
-        <v>1</v>
+        <v>204</v>
       </c>
       <c r="C2397" s="1">
         <v>44765</v>
@@ -27222,7 +27222,7 @@
         <v>2022</v>
       </c>
       <c r="B2398">
-        <v>1</v>
+        <v>205</v>
       </c>
       <c r="C2398" s="1">
         <v>44766</v>
@@ -27233,7 +27233,7 @@
         <v>2022</v>
       </c>
       <c r="B2399">
-        <v>1</v>
+        <v>206</v>
       </c>
       <c r="C2399" s="1">
         <v>44767</v>
@@ -27244,7 +27244,7 @@
         <v>2022</v>
       </c>
       <c r="B2400">
-        <v>1</v>
+        <v>207</v>
       </c>
       <c r="C2400" s="1">
         <v>44768</v>
@@ -27255,7 +27255,7 @@
         <v>2022</v>
       </c>
       <c r="B2401">
-        <v>1</v>
+        <v>208</v>
       </c>
       <c r="C2401" s="1">
         <v>44769</v>
@@ -27266,7 +27266,7 @@
         <v>2022</v>
       </c>
       <c r="B2402">
-        <v>1</v>
+        <v>209</v>
       </c>
       <c r="C2402" s="1">
         <v>44770</v>
@@ -27277,7 +27277,7 @@
         <v>2022</v>
       </c>
       <c r="B2403">
-        <v>1</v>
+        <v>210</v>
       </c>
       <c r="C2403" s="1">
         <v>44771</v>
@@ -27288,7 +27288,7 @@
         <v>2022</v>
       </c>
       <c r="B2404">
-        <v>1</v>
+        <v>211</v>
       </c>
       <c r="C2404" s="1">
         <v>44772</v>
@@ -27299,7 +27299,7 @@
         <v>2022</v>
       </c>
       <c r="B2405">
-        <v>1</v>
+        <v>212</v>
       </c>
       <c r="C2405" s="1">
         <v>44773</v>
@@ -27310,7 +27310,7 @@
         <v>2022</v>
       </c>
       <c r="B2406">
-        <v>1</v>
+        <v>213</v>
       </c>
       <c r="C2406" s="1">
         <v>44774</v>
@@ -27321,7 +27321,7 @@
         <v>2022</v>
       </c>
       <c r="B2407">
-        <v>1</v>
+        <v>214</v>
       </c>
       <c r="C2407" s="1">
         <v>44775</v>
@@ -27332,7 +27332,7 @@
         <v>2022</v>
       </c>
       <c r="B2408">
-        <v>1</v>
+        <v>215</v>
       </c>
       <c r="C2408" s="1">
         <v>44776</v>
@@ -27343,7 +27343,7 @@
         <v>2022</v>
       </c>
       <c r="B2409">
-        <v>1</v>
+        <v>216</v>
       </c>
       <c r="C2409" s="1">
         <v>44777</v>
@@ -27354,7 +27354,7 @@
         <v>2022</v>
       </c>
       <c r="B2410">
-        <v>1</v>
+        <v>217</v>
       </c>
       <c r="C2410" s="1">
         <v>44778</v>
@@ -27365,7 +27365,7 @@
         <v>2022</v>
       </c>
       <c r="B2411">
-        <v>1</v>
+        <v>218</v>
       </c>
       <c r="C2411" s="1">
         <v>44779</v>
@@ -27376,7 +27376,7 @@
         <v>2022</v>
       </c>
       <c r="B2412">
-        <v>1</v>
+        <v>219</v>
       </c>
       <c r="C2412" s="1">
         <v>44780</v>
@@ -27387,7 +27387,7 @@
         <v>2022</v>
       </c>
       <c r="B2413">
-        <v>1</v>
+        <v>220</v>
       </c>
       <c r="C2413" s="1">
         <v>44781</v>
@@ -27398,7 +27398,7 @@
         <v>2022</v>
       </c>
       <c r="B2414">
-        <v>1</v>
+        <v>221</v>
       </c>
       <c r="C2414" s="1">
         <v>44782</v>
@@ -27409,7 +27409,7 @@
         <v>2022</v>
       </c>
       <c r="B2415">
-        <v>1</v>
+        <v>222</v>
       </c>
       <c r="C2415" s="1">
         <v>44783</v>
@@ -27420,7 +27420,7 @@
         <v>2022</v>
       </c>
       <c r="B2416">
-        <v>1</v>
+        <v>223</v>
       </c>
       <c r="C2416" s="1">
         <v>44784</v>
@@ -27431,7 +27431,7 @@
         <v>2022</v>
       </c>
       <c r="B2417">
-        <v>1</v>
+        <v>224</v>
       </c>
       <c r="C2417" s="1">
         <v>44785</v>
@@ -27442,7 +27442,7 @@
         <v>2022</v>
       </c>
       <c r="B2418">
-        <v>1</v>
+        <v>225</v>
       </c>
       <c r="C2418" s="1">
         <v>44786</v>
@@ -27453,7 +27453,7 @@
         <v>2022</v>
       </c>
       <c r="B2419">
-        <v>1</v>
+        <v>226</v>
       </c>
       <c r="C2419" s="1">
         <v>44787</v>
@@ -27464,7 +27464,7 @@
         <v>2022</v>
       </c>
       <c r="B2420">
-        <v>1</v>
+        <v>227</v>
       </c>
       <c r="C2420" s="1">
         <v>44788</v>
@@ -27475,7 +27475,7 @@
         <v>2022</v>
       </c>
       <c r="B2421">
-        <v>1</v>
+        <v>228</v>
       </c>
       <c r="C2421" s="1">
         <v>44789</v>
@@ -27486,7 +27486,7 @@
         <v>2022</v>
       </c>
       <c r="B2422">
-        <v>1</v>
+        <v>229</v>
       </c>
       <c r="C2422" s="1">
         <v>44790</v>
@@ -27497,7 +27497,7 @@
         <v>2022</v>
       </c>
       <c r="B2423">
-        <v>1</v>
+        <v>230</v>
       </c>
       <c r="C2423" s="1">
         <v>44791</v>
@@ -27508,7 +27508,7 @@
         <v>2022</v>
       </c>
       <c r="B2424">
-        <v>1</v>
+        <v>231</v>
       </c>
       <c r="C2424" s="1">
         <v>44792</v>
@@ -27519,7 +27519,7 @@
         <v>2022</v>
       </c>
       <c r="B2425">
-        <v>1</v>
+        <v>232</v>
       </c>
       <c r="C2425" s="1">
         <v>44793</v>
@@ -27530,7 +27530,7 @@
         <v>2022</v>
       </c>
       <c r="B2426">
-        <v>1</v>
+        <v>233</v>
       </c>
       <c r="C2426" s="1">
         <v>44794</v>
@@ -27541,7 +27541,7 @@
         <v>2022</v>
       </c>
       <c r="B2427">
-        <v>1</v>
+        <v>234</v>
       </c>
       <c r="C2427" s="1">
         <v>44795</v>
@@ -27552,7 +27552,7 @@
         <v>2022</v>
       </c>
       <c r="B2428">
-        <v>1</v>
+        <v>235</v>
       </c>
       <c r="C2428" s="1">
         <v>44796</v>
@@ -27563,7 +27563,7 @@
         <v>2022</v>
       </c>
       <c r="B2429">
-        <v>1</v>
+        <v>236</v>
       </c>
       <c r="C2429" s="1">
         <v>44797</v>
@@ -27574,7 +27574,7 @@
         <v>2022</v>
       </c>
       <c r="B2430">
-        <v>1</v>
+        <v>237</v>
       </c>
       <c r="C2430" s="1">
         <v>44798</v>
@@ -27585,7 +27585,7 @@
         <v>2022</v>
       </c>
       <c r="B2431">
-        <v>1</v>
+        <v>238</v>
       </c>
       <c r="C2431" s="1">
         <v>44799</v>
@@ -27596,7 +27596,7 @@
         <v>2022</v>
       </c>
       <c r="B2432">
-        <v>1</v>
+        <v>239</v>
       </c>
       <c r="C2432" s="1">
         <v>44800</v>
@@ -27607,7 +27607,7 @@
         <v>2022</v>
       </c>
       <c r="B2433">
-        <v>1</v>
+        <v>240</v>
       </c>
       <c r="C2433" s="1">
         <v>44801</v>
@@ -27618,7 +27618,7 @@
         <v>2022</v>
       </c>
       <c r="B2434">
-        <v>1</v>
+        <v>241</v>
       </c>
       <c r="C2434" s="1">
         <v>44802</v>
@@ -27629,7 +27629,7 @@
         <v>2022</v>
       </c>
       <c r="B2435">
-        <v>1</v>
+        <v>242</v>
       </c>
       <c r="C2435" s="1">
         <v>44803</v>
@@ -27640,7 +27640,7 @@
         <v>2022</v>
       </c>
       <c r="B2436">
-        <v>1</v>
+        <v>243</v>
       </c>
       <c r="C2436" s="1">
         <v>44804</v>
@@ -27651,7 +27651,7 @@
         <v>2022</v>
       </c>
       <c r="B2437">
-        <v>1</v>
+        <v>244</v>
       </c>
       <c r="C2437" s="1">
         <v>44805</v>
@@ -27662,7 +27662,7 @@
         <v>2022</v>
       </c>
       <c r="B2438">
-        <v>1</v>
+        <v>245</v>
       </c>
       <c r="C2438" s="1">
         <v>44806</v>
@@ -27673,7 +27673,7 @@
         <v>2022</v>
       </c>
       <c r="B2439">
-        <v>1</v>
+        <v>246</v>
       </c>
       <c r="C2439" s="1">
         <v>44807</v>
@@ -27684,7 +27684,7 @@
         <v>2022</v>
       </c>
       <c r="B2440">
-        <v>1</v>
+        <v>247</v>
       </c>
       <c r="C2440" s="1">
         <v>44808</v>
@@ -27695,7 +27695,7 @@
         <v>2022</v>
       </c>
       <c r="B2441">
-        <v>1</v>
+        <v>248</v>
       </c>
       <c r="C2441" s="1">
         <v>44809</v>
@@ -27706,7 +27706,7 @@
         <v>2022</v>
       </c>
       <c r="B2442">
-        <v>1</v>
+        <v>249</v>
       </c>
       <c r="C2442" s="1">
         <v>44810</v>
@@ -27717,7 +27717,7 @@
         <v>2022</v>
       </c>
       <c r="B2443">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="C2443" s="1">
         <v>44811</v>
@@ -27728,7 +27728,7 @@
         <v>2022</v>
       </c>
       <c r="B2444">
-        <v>1</v>
+        <v>251</v>
       </c>
       <c r="C2444" s="1">
         <v>44812</v>
@@ -27739,7 +27739,7 @@
         <v>2022</v>
       </c>
       <c r="B2445">
-        <v>1</v>
+        <v>252</v>
       </c>
       <c r="C2445" s="1">
         <v>44813</v>
@@ -27750,7 +27750,7 @@
         <v>2022</v>
       </c>
       <c r="B2446">
-        <v>1</v>
+        <v>253</v>
       </c>
       <c r="C2446" s="1">
         <v>44814</v>
@@ -27761,7 +27761,7 @@
         <v>2022</v>
       </c>
       <c r="B2447">
-        <v>1</v>
+        <v>254</v>
       </c>
       <c r="C2447" s="1">
         <v>44815</v>
@@ -27772,7 +27772,7 @@
         <v>2022</v>
       </c>
       <c r="B2448">
-        <v>1</v>
+        <v>255</v>
       </c>
       <c r="C2448" s="1">
         <v>44816</v>
@@ -27783,7 +27783,7 @@
         <v>2022</v>
       </c>
       <c r="B2449">
-        <v>1</v>
+        <v>256</v>
       </c>
       <c r="C2449" s="1">
         <v>44817</v>
@@ -27794,7 +27794,7 @@
         <v>2022</v>
       </c>
       <c r="B2450">
-        <v>1</v>
+        <v>257</v>
       </c>
       <c r="C2450" s="1">
         <v>44818</v>
@@ -27805,7 +27805,7 @@
         <v>2022</v>
       </c>
       <c r="B2451">
-        <v>1</v>
+        <v>258</v>
       </c>
       <c r="C2451" s="1">
         <v>44819</v>
@@ -27816,7 +27816,7 @@
         <v>2022</v>
       </c>
       <c r="B2452">
-        <v>1</v>
+        <v>259</v>
       </c>
       <c r="C2452" s="1">
         <v>44820</v>
@@ -27827,7 +27827,7 @@
         <v>2022</v>
       </c>
       <c r="B2453">
-        <v>1</v>
+        <v>260</v>
       </c>
       <c r="C2453" s="1">
         <v>44821</v>
@@ -27838,7 +27838,7 @@
         <v>2022</v>
       </c>
       <c r="B2454">
-        <v>1</v>
+        <v>261</v>
       </c>
       <c r="C2454" s="1">
         <v>44822</v>
@@ -27849,7 +27849,7 @@
         <v>2022</v>
       </c>
       <c r="B2455">
-        <v>1</v>
+        <v>262</v>
       </c>
       <c r="C2455" s="1">
         <v>44823</v>
@@ -27860,7 +27860,7 @@
         <v>2022</v>
       </c>
       <c r="B2456">
-        <v>1</v>
+        <v>263</v>
       </c>
       <c r="C2456" s="1">
         <v>44824</v>
@@ -27871,7 +27871,7 @@
         <v>2022</v>
       </c>
       <c r="B2457">
-        <v>1</v>
+        <v>264</v>
       </c>
       <c r="C2457" s="1">
         <v>44825</v>
@@ -27882,7 +27882,7 @@
         <v>2022</v>
       </c>
       <c r="B2458">
-        <v>1</v>
+        <v>265</v>
       </c>
       <c r="C2458" s="1">
         <v>44826</v>
@@ -27893,7 +27893,7 @@
         <v>2022</v>
       </c>
       <c r="B2459">
-        <v>1</v>
+        <v>266</v>
       </c>
       <c r="C2459" s="1">
         <v>44827</v>
@@ -27904,7 +27904,7 @@
         <v>2022</v>
       </c>
       <c r="B2460">
-        <v>1</v>
+        <v>267</v>
       </c>
       <c r="C2460" s="1">
         <v>44828</v>
@@ -27915,7 +27915,7 @@
         <v>2022</v>
       </c>
       <c r="B2461">
-        <v>1</v>
+        <v>268</v>
       </c>
       <c r="C2461" s="1">
         <v>44829</v>
@@ -27926,7 +27926,7 @@
         <v>2022</v>
       </c>
       <c r="B2462">
-        <v>1</v>
+        <v>269</v>
       </c>
       <c r="C2462" s="1">
         <v>44830</v>
@@ -27937,7 +27937,7 @@
         <v>2022</v>
       </c>
       <c r="B2463">
-        <v>1</v>
+        <v>270</v>
       </c>
       <c r="C2463" s="1">
         <v>44831</v>
@@ -27948,7 +27948,7 @@
         <v>2022</v>
       </c>
       <c r="B2464">
-        <v>1</v>
+        <v>271</v>
       </c>
       <c r="C2464" s="1">
         <v>44832</v>
@@ -27959,7 +27959,7 @@
         <v>2022</v>
       </c>
       <c r="B2465">
-        <v>1</v>
+        <v>272</v>
       </c>
       <c r="C2465" s="1">
         <v>44833</v>
@@ -27970,7 +27970,7 @@
         <v>2022</v>
       </c>
       <c r="B2466">
-        <v>1</v>
+        <v>273</v>
       </c>
       <c r="C2466" s="1">
         <v>44834</v>
@@ -27981,7 +27981,7 @@
         <v>2022</v>
       </c>
       <c r="B2467">
-        <v>1</v>
+        <v>274</v>
       </c>
       <c r="C2467" s="1">
         <v>44835</v>
@@ -27992,7 +27992,7 @@
         <v>2022</v>
       </c>
       <c r="B2468">
-        <v>1</v>
+        <v>275</v>
       </c>
       <c r="C2468" s="1">
         <v>44836</v>
@@ -28003,7 +28003,7 @@
         <v>2022</v>
       </c>
       <c r="B2469">
-        <v>1</v>
+        <v>276</v>
       </c>
       <c r="C2469" s="1">
         <v>44837</v>
@@ -28014,7 +28014,7 @@
         <v>2022</v>
       </c>
       <c r="B2470">
-        <v>1</v>
+        <v>277</v>
       </c>
       <c r="C2470" s="1">
         <v>44838</v>
@@ -28025,7 +28025,7 @@
         <v>2022</v>
       </c>
       <c r="B2471">
-        <v>1</v>
+        <v>278</v>
       </c>
       <c r="C2471" s="1">
         <v>44839</v>
@@ -28036,7 +28036,7 @@
         <v>2022</v>
       </c>
       <c r="B2472">
-        <v>1</v>
+        <v>279</v>
       </c>
       <c r="C2472" s="1">
         <v>44840</v>
@@ -28047,7 +28047,7 @@
         <v>2022</v>
       </c>
       <c r="B2473">
-        <v>1</v>
+        <v>280</v>
       </c>
       <c r="C2473" s="1">
         <v>44841</v>
@@ -28058,7 +28058,7 @@
         <v>2022</v>
       </c>
       <c r="B2474">
-        <v>1</v>
+        <v>281</v>
       </c>
       <c r="C2474" s="1">
         <v>44842</v>
@@ -28069,7 +28069,7 @@
         <v>2022</v>
       </c>
       <c r="B2475">
-        <v>1</v>
+        <v>282</v>
       </c>
       <c r="C2475" s="1">
         <v>44843</v>
@@ -28080,7 +28080,7 @@
         <v>2022</v>
       </c>
       <c r="B2476">
-        <v>1</v>
+        <v>283</v>
       </c>
       <c r="C2476" s="1">
         <v>44844</v>
@@ -28091,7 +28091,7 @@
         <v>2022</v>
       </c>
       <c r="B2477">
-        <v>1</v>
+        <v>284</v>
       </c>
       <c r="C2477" s="1">
         <v>44845</v>
@@ -28102,7 +28102,7 @@
         <v>2022</v>
       </c>
       <c r="B2478">
-        <v>1</v>
+        <v>285</v>
       </c>
       <c r="C2478" s="1">
         <v>44846</v>
@@ -28113,7 +28113,7 @@
         <v>2022</v>
       </c>
       <c r="B2479">
-        <v>1</v>
+        <v>286</v>
       </c>
       <c r="C2479" s="1">
         <v>44847</v>
@@ -28124,7 +28124,7 @@
         <v>2022</v>
       </c>
       <c r="B2480">
-        <v>1</v>
+        <v>287</v>
       </c>
       <c r="C2480" s="1">
         <v>44848</v>
@@ -28135,7 +28135,7 @@
         <v>2022</v>
       </c>
       <c r="B2481">
-        <v>1</v>
+        <v>288</v>
       </c>
       <c r="C2481" s="1">
         <v>44849</v>
@@ -28146,7 +28146,7 @@
         <v>2022</v>
       </c>
       <c r="B2482">
-        <v>1</v>
+        <v>289</v>
       </c>
       <c r="C2482" s="1">
         <v>44850</v>
@@ -28157,7 +28157,7 @@
         <v>2022</v>
       </c>
       <c r="B2483">
-        <v>1</v>
+        <v>290</v>
       </c>
       <c r="C2483" s="1">
         <v>44851</v>
@@ -28168,7 +28168,7 @@
         <v>2022</v>
       </c>
       <c r="B2484">
-        <v>1</v>
+        <v>291</v>
       </c>
       <c r="C2484" s="1">
         <v>44852</v>
@@ -28179,7 +28179,7 @@
         <v>2022</v>
       </c>
       <c r="B2485">
-        <v>1</v>
+        <v>292</v>
       </c>
       <c r="C2485" s="1">
         <v>44853</v>
@@ -28190,7 +28190,7 @@
         <v>2022</v>
       </c>
       <c r="B2486">
-        <v>1</v>
+        <v>293</v>
       </c>
       <c r="C2486" s="1">
         <v>44854</v>
@@ -28201,7 +28201,7 @@
         <v>2022</v>
       </c>
       <c r="B2487">
-        <v>1</v>
+        <v>294</v>
       </c>
       <c r="C2487" s="1">
         <v>44855</v>
@@ -28212,7 +28212,7 @@
         <v>2022</v>
       </c>
       <c r="B2488">
-        <v>1</v>
+        <v>295</v>
       </c>
       <c r="C2488" s="1">
         <v>44856</v>
@@ -28223,7 +28223,7 @@
         <v>2022</v>
       </c>
       <c r="B2489">
-        <v>1</v>
+        <v>296</v>
       </c>
       <c r="C2489" s="1">
         <v>44857</v>
@@ -28234,7 +28234,7 @@
         <v>2022</v>
       </c>
       <c r="B2490">
-        <v>1</v>
+        <v>297</v>
       </c>
       <c r="C2490" s="1">
         <v>44858</v>
@@ -28245,7 +28245,7 @@
         <v>2022</v>
       </c>
       <c r="B2491">
-        <v>1</v>
+        <v>298</v>
       </c>
       <c r="C2491" s="1">
         <v>44859</v>
@@ -28256,7 +28256,7 @@
         <v>2022</v>
       </c>
       <c r="B2492">
-        <v>1</v>
+        <v>299</v>
       </c>
       <c r="C2492" s="1">
         <v>44860</v>
@@ -28267,7 +28267,7 @@
         <v>2022</v>
       </c>
       <c r="B2493">
-        <v>1</v>
+        <v>300</v>
       </c>
       <c r="C2493" s="1">
         <v>44861</v>
@@ -28278,7 +28278,7 @@
         <v>2022</v>
       </c>
       <c r="B2494">
-        <v>1</v>
+        <v>301</v>
       </c>
       <c r="C2494" s="1">
         <v>44862</v>
@@ -28289,7 +28289,7 @@
         <v>2022</v>
       </c>
       <c r="B2495">
-        <v>1</v>
+        <v>302</v>
       </c>
       <c r="C2495" s="1">
         <v>44863</v>
@@ -28300,7 +28300,7 @@
         <v>2022</v>
       </c>
       <c r="B2496">
-        <v>1</v>
+        <v>303</v>
       </c>
       <c r="C2496" s="1">
         <v>44864</v>
@@ -28311,7 +28311,7 @@
         <v>2022</v>
       </c>
       <c r="B2497">
-        <v>1</v>
+        <v>304</v>
       </c>
       <c r="C2497" s="1">
         <v>44865</v>
@@ -28322,7 +28322,7 @@
         <v>2022</v>
       </c>
       <c r="B2498">
-        <v>1</v>
+        <v>305</v>
       </c>
       <c r="C2498" s="1">
         <v>44866</v>
@@ -28333,7 +28333,7 @@
         <v>2022</v>
       </c>
       <c r="B2499">
-        <v>1</v>
+        <v>306</v>
       </c>
       <c r="C2499" s="1">
         <v>44867</v>
@@ -28344,7 +28344,7 @@
         <v>2022</v>
       </c>
       <c r="B2500">
-        <v>1</v>
+        <v>307</v>
       </c>
       <c r="C2500" s="1">
         <v>44868</v>
@@ -28355,7 +28355,7 @@
         <v>2022</v>
       </c>
       <c r="B2501">
-        <v>1</v>
+        <v>308</v>
       </c>
       <c r="C2501" s="1">
         <v>44869</v>
@@ -28366,7 +28366,7 @@
         <v>2022</v>
       </c>
       <c r="B2502">
-        <v>1</v>
+        <v>309</v>
       </c>
       <c r="C2502" s="1">
         <v>44870</v>
@@ -28377,7 +28377,7 @@
         <v>2022</v>
       </c>
       <c r="B2503">
-        <v>1</v>
+        <v>310</v>
       </c>
       <c r="C2503" s="1">
         <v>44871</v>
@@ -28388,7 +28388,7 @@
         <v>2022</v>
       </c>
       <c r="B2504">
-        <v>1</v>
+        <v>311</v>
       </c>
       <c r="C2504" s="1">
         <v>44872</v>
@@ -28399,7 +28399,7 @@
         <v>2022</v>
       </c>
       <c r="B2505">
-        <v>1</v>
+        <v>312</v>
       </c>
       <c r="C2505" s="1">
         <v>44873</v>
@@ -28410,7 +28410,7 @@
         <v>2022</v>
       </c>
       <c r="B2506">
-        <v>1</v>
+        <v>313</v>
       </c>
       <c r="C2506" s="1">
         <v>44874</v>
@@ -28421,7 +28421,7 @@
         <v>2022</v>
       </c>
       <c r="B2507">
-        <v>1</v>
+        <v>314</v>
       </c>
       <c r="C2507" s="1">
         <v>44875</v>
@@ -28432,7 +28432,7 @@
         <v>2022</v>
       </c>
       <c r="B2508">
-        <v>1</v>
+        <v>315</v>
       </c>
       <c r="C2508" s="1">
         <v>44876</v>
@@ -28443,7 +28443,7 @@
         <v>2022</v>
       </c>
       <c r="B2509">
-        <v>1</v>
+        <v>316</v>
       </c>
       <c r="C2509" s="1">
         <v>44877</v>
@@ -28454,7 +28454,7 @@
         <v>2022</v>
       </c>
       <c r="B2510">
-        <v>1</v>
+        <v>317</v>
       </c>
       <c r="C2510" s="1">
         <v>44878</v>
@@ -28465,7 +28465,7 @@
         <v>2022</v>
       </c>
       <c r="B2511">
-        <v>1</v>
+        <v>318</v>
       </c>
       <c r="C2511" s="1">
         <v>44879</v>
@@ -28476,7 +28476,7 @@
         <v>2022</v>
       </c>
       <c r="B2512">
-        <v>1</v>
+        <v>319</v>
       </c>
       <c r="C2512" s="1">
         <v>44880</v>
@@ -28487,7 +28487,7 @@
         <v>2022</v>
       </c>
       <c r="B2513">
-        <v>1</v>
+        <v>320</v>
       </c>
       <c r="C2513" s="1">
         <v>44881</v>
@@ -28498,7 +28498,7 @@
         <v>2022</v>
       </c>
       <c r="B2514">
-        <v>1</v>
+        <v>321</v>
       </c>
       <c r="C2514" s="1">
         <v>44882</v>
@@ -28509,7 +28509,7 @@
         <v>2022</v>
       </c>
       <c r="B2515">
-        <v>1</v>
+        <v>322</v>
       </c>
       <c r="C2515" s="1">
         <v>44883</v>
@@ -28520,7 +28520,7 @@
         <v>2022</v>
       </c>
       <c r="B2516">
-        <v>1</v>
+        <v>323</v>
       </c>
       <c r="C2516" s="1">
         <v>44884</v>
@@ -28531,7 +28531,7 @@
         <v>2022</v>
       </c>
       <c r="B2517">
-        <v>1</v>
+        <v>324</v>
       </c>
       <c r="C2517" s="1">
         <v>44885</v>
@@ -28542,7 +28542,7 @@
         <v>2022</v>
       </c>
       <c r="B2518">
-        <v>1</v>
+        <v>325</v>
       </c>
       <c r="C2518" s="1">
         <v>44886</v>
@@ -28553,7 +28553,7 @@
         <v>2022</v>
       </c>
       <c r="B2519">
-        <v>1</v>
+        <v>326</v>
       </c>
       <c r="C2519" s="1">
         <v>44887</v>
@@ -28564,7 +28564,7 @@
         <v>2022</v>
       </c>
       <c r="B2520">
-        <v>1</v>
+        <v>327</v>
       </c>
       <c r="C2520" s="1">
         <v>44888</v>
@@ -28575,7 +28575,7 @@
         <v>2022</v>
       </c>
       <c r="B2521">
-        <v>1</v>
+        <v>328</v>
       </c>
       <c r="C2521" s="1">
         <v>44889</v>
@@ -28586,7 +28586,7 @@
         <v>2022</v>
       </c>
       <c r="B2522">
-        <v>1</v>
+        <v>329</v>
       </c>
       <c r="C2522" s="1">
         <v>44890</v>
@@ -28597,7 +28597,7 @@
         <v>2022</v>
       </c>
       <c r="B2523">
-        <v>1</v>
+        <v>330</v>
       </c>
       <c r="C2523" s="1">
         <v>44891</v>
@@ -28608,7 +28608,7 @@
         <v>2022</v>
       </c>
       <c r="B2524">
-        <v>1</v>
+        <v>331</v>
       </c>
       <c r="C2524" s="1">
         <v>44892</v>
@@ -28619,7 +28619,7 @@
         <v>2022</v>
       </c>
       <c r="B2525">
-        <v>1</v>
+        <v>332</v>
       </c>
       <c r="C2525" s="1">
         <v>44893</v>
@@ -28630,7 +28630,7 @@
         <v>2022</v>
       </c>
       <c r="B2526">
-        <v>1</v>
+        <v>333</v>
       </c>
       <c r="C2526" s="1">
         <v>44894</v>
@@ -28641,7 +28641,7 @@
         <v>2022</v>
       </c>
       <c r="B2527">
-        <v>1</v>
+        <v>334</v>
       </c>
       <c r="C2527" s="1">
         <v>44895</v>
@@ -28652,7 +28652,7 @@
         <v>2022</v>
       </c>
       <c r="B2528">
-        <v>1</v>
+        <v>335</v>
       </c>
       <c r="C2528" s="1">
         <v>44896</v>
@@ -28663,7 +28663,7 @@
         <v>2022</v>
       </c>
       <c r="B2529">
-        <v>1</v>
+        <v>336</v>
       </c>
       <c r="C2529" s="1">
         <v>44897</v>
@@ -28674,7 +28674,7 @@
         <v>2022</v>
       </c>
       <c r="B2530">
-        <v>1</v>
+        <v>337</v>
       </c>
       <c r="C2530" s="1">
         <v>44898</v>
@@ -28685,7 +28685,7 @@
         <v>2022</v>
       </c>
       <c r="B2531">
-        <v>1</v>
+        <v>338</v>
       </c>
       <c r="C2531" s="1">
         <v>44899</v>
@@ -28696,7 +28696,7 @@
         <v>2022</v>
       </c>
       <c r="B2532">
-        <v>1</v>
+        <v>339</v>
       </c>
       <c r="C2532" s="1">
         <v>44900</v>
@@ -28707,7 +28707,7 @@
         <v>2022</v>
       </c>
       <c r="B2533">
-        <v>1</v>
+        <v>340</v>
       </c>
       <c r="C2533" s="1">
         <v>44901</v>
@@ -28718,7 +28718,7 @@
         <v>2022</v>
       </c>
       <c r="B2534">
-        <v>1</v>
+        <v>341</v>
       </c>
       <c r="C2534" s="1">
         <v>44902</v>
@@ -28729,7 +28729,7 @@
         <v>2022</v>
       </c>
       <c r="B2535">
-        <v>1</v>
+        <v>342</v>
       </c>
       <c r="C2535" s="1">
         <v>44903</v>
@@ -28740,7 +28740,7 @@
         <v>2022</v>
       </c>
       <c r="B2536">
-        <v>1</v>
+        <v>343</v>
       </c>
       <c r="C2536" s="1">
         <v>44904</v>
@@ -28751,7 +28751,7 @@
         <v>2022</v>
       </c>
       <c r="B2537">
-        <v>1</v>
+        <v>344</v>
       </c>
       <c r="C2537" s="1">
         <v>44905</v>
@@ -28762,7 +28762,7 @@
         <v>2022</v>
       </c>
       <c r="B2538">
-        <v>1</v>
+        <v>345</v>
       </c>
       <c r="C2538" s="1">
         <v>44906</v>
@@ -28773,7 +28773,7 @@
         <v>2022</v>
       </c>
       <c r="B2539">
-        <v>1</v>
+        <v>346</v>
       </c>
       <c r="C2539" s="1">
         <v>44907</v>
@@ -28784,7 +28784,7 @@
         <v>2022</v>
       </c>
       <c r="B2540">
-        <v>1</v>
+        <v>347</v>
       </c>
       <c r="C2540" s="1">
         <v>44908</v>
@@ -28795,7 +28795,7 @@
         <v>2022</v>
       </c>
       <c r="B2541">
-        <v>1</v>
+        <v>348</v>
       </c>
       <c r="C2541" s="1">
         <v>44909</v>
@@ -28806,7 +28806,7 @@
         <v>2022</v>
       </c>
       <c r="B2542">
-        <v>1</v>
+        <v>349</v>
       </c>
       <c r="C2542" s="1">
         <v>44910</v>
@@ -28817,7 +28817,7 @@
         <v>2022</v>
       </c>
       <c r="B2543">
-        <v>1</v>
+        <v>350</v>
       </c>
       <c r="C2543" s="1">
         <v>44911</v>
@@ -28828,7 +28828,7 @@
         <v>2022</v>
       </c>
       <c r="B2544">
-        <v>1</v>
+        <v>351</v>
       </c>
       <c r="C2544" s="1">
         <v>44912</v>
@@ -28839,7 +28839,7 @@
         <v>2022</v>
       </c>
       <c r="B2545">
-        <v>1</v>
+        <v>352</v>
       </c>
       <c r="C2545" s="1">
         <v>44913</v>
@@ -28850,7 +28850,7 @@
         <v>2022</v>
       </c>
       <c r="B2546">
-        <v>1</v>
+        <v>353</v>
       </c>
       <c r="C2546" s="1">
         <v>44914</v>
@@ -28861,7 +28861,7 @@
         <v>2022</v>
       </c>
       <c r="B2547">
-        <v>1</v>
+        <v>354</v>
       </c>
       <c r="C2547" s="1">
         <v>44915</v>
@@ -28872,7 +28872,7 @@
         <v>2022</v>
       </c>
       <c r="B2548">
-        <v>1</v>
+        <v>355</v>
       </c>
       <c r="C2548" s="1">
         <v>44916</v>
@@ -28883,7 +28883,7 @@
         <v>2022</v>
       </c>
       <c r="B2549">
-        <v>1</v>
+        <v>356</v>
       </c>
       <c r="C2549" s="1">
         <v>44917</v>
@@ -28894,7 +28894,7 @@
         <v>2022</v>
       </c>
       <c r="B2550">
-        <v>1</v>
+        <v>357</v>
       </c>
       <c r="C2550" s="1">
         <v>44918</v>
@@ -28905,7 +28905,7 @@
         <v>2022</v>
       </c>
       <c r="B2551">
-        <v>1</v>
+        <v>358</v>
       </c>
       <c r="C2551" s="1">
         <v>44919</v>
@@ -28916,7 +28916,7 @@
         <v>2022</v>
       </c>
       <c r="B2552">
-        <v>1</v>
+        <v>359</v>
       </c>
       <c r="C2552" s="1">
         <v>44920</v>
@@ -28927,7 +28927,7 @@
         <v>2022</v>
       </c>
       <c r="B2553">
-        <v>1</v>
+        <v>360</v>
       </c>
       <c r="C2553" s="1">
         <v>44921</v>
@@ -28938,7 +28938,7 @@
         <v>2022</v>
       </c>
       <c r="B2554">
-        <v>1</v>
+        <v>361</v>
       </c>
       <c r="C2554" s="1">
         <v>44922</v>
@@ -28949,7 +28949,7 @@
         <v>2022</v>
       </c>
       <c r="B2555">
-        <v>1</v>
+        <v>362</v>
       </c>
       <c r="C2555" s="1">
         <v>44923</v>
@@ -28960,7 +28960,7 @@
         <v>2022</v>
       </c>
       <c r="B2556">
-        <v>1</v>
+        <v>363</v>
       </c>
       <c r="C2556" s="1">
         <v>44924</v>
@@ -28971,7 +28971,7 @@
         <v>2022</v>
       </c>
       <c r="B2557">
-        <v>1</v>
+        <v>364</v>
       </c>
       <c r="C2557" s="1">
         <v>44925</v>
@@ -28982,7 +28982,7 @@
         <v>2022</v>
       </c>
       <c r="B2558">
-        <v>1</v>
+        <v>365</v>
       </c>
       <c r="C2558" s="1">
         <v>44926</v>

</xml_diff>

<commit_message>
data updated till 1/1/2023
</commit_message>
<xml_diff>
--- a/data/calendar-dates.xlsx
+++ b/data/calendar-dates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\deqhq1\WQ-Share\Harmful Algal Blooms Coordination Team\HAB_Shiny_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEF6BB3-03E4-463B-A479-B8E01D7457E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE7FB59-034A-423C-8ED3-3401572B8146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-13068" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="calendar-dates" sheetId="1" r:id="rId1"/>
@@ -839,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2558"/>
+  <dimension ref="A1:C2923"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1821" workbookViewId="0">
-      <selection activeCell="B2194" sqref="B2194:B2558"/>
+    <sheetView tabSelected="1" topLeftCell="A2913" workbookViewId="0">
+      <selection activeCell="A2559" sqref="A2559:A2923"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28988,6 +28988,4021 @@
         <v>44926</v>
       </c>
     </row>
+    <row r="2559" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2559">
+        <v>2023</v>
+      </c>
+      <c r="B2559">
+        <v>1</v>
+      </c>
+      <c r="C2559" s="1">
+        <v>44927</v>
+      </c>
+    </row>
+    <row r="2560" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2560">
+        <v>2023</v>
+      </c>
+      <c r="B2560">
+        <v>2</v>
+      </c>
+      <c r="C2560" s="1">
+        <v>44928</v>
+      </c>
+    </row>
+    <row r="2561" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2561">
+        <v>2023</v>
+      </c>
+      <c r="B2561">
+        <v>3</v>
+      </c>
+      <c r="C2561" s="1">
+        <v>44929</v>
+      </c>
+    </row>
+    <row r="2562" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2562">
+        <v>2023</v>
+      </c>
+      <c r="B2562">
+        <v>4</v>
+      </c>
+      <c r="C2562" s="1">
+        <v>44930</v>
+      </c>
+    </row>
+    <row r="2563" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2563">
+        <v>2023</v>
+      </c>
+      <c r="B2563">
+        <v>5</v>
+      </c>
+      <c r="C2563" s="1">
+        <v>44931</v>
+      </c>
+    </row>
+    <row r="2564" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2564">
+        <v>2023</v>
+      </c>
+      <c r="B2564">
+        <v>6</v>
+      </c>
+      <c r="C2564" s="1">
+        <v>44932</v>
+      </c>
+    </row>
+    <row r="2565" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2565">
+        <v>2023</v>
+      </c>
+      <c r="B2565">
+        <v>7</v>
+      </c>
+      <c r="C2565" s="1">
+        <v>44933</v>
+      </c>
+    </row>
+    <row r="2566" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2566">
+        <v>2023</v>
+      </c>
+      <c r="B2566">
+        <v>8</v>
+      </c>
+      <c r="C2566" s="1">
+        <v>44934</v>
+      </c>
+    </row>
+    <row r="2567" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2567">
+        <v>2023</v>
+      </c>
+      <c r="B2567">
+        <v>9</v>
+      </c>
+      <c r="C2567" s="1">
+        <v>44935</v>
+      </c>
+    </row>
+    <row r="2568" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2568">
+        <v>2023</v>
+      </c>
+      <c r="B2568">
+        <v>10</v>
+      </c>
+      <c r="C2568" s="1">
+        <v>44936</v>
+      </c>
+    </row>
+    <row r="2569" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2569">
+        <v>2023</v>
+      </c>
+      <c r="B2569">
+        <v>11</v>
+      </c>
+      <c r="C2569" s="1">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="2570" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2570">
+        <v>2023</v>
+      </c>
+      <c r="B2570">
+        <v>12</v>
+      </c>
+      <c r="C2570" s="1">
+        <v>44938</v>
+      </c>
+    </row>
+    <row r="2571" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2571">
+        <v>2023</v>
+      </c>
+      <c r="B2571">
+        <v>13</v>
+      </c>
+      <c r="C2571" s="1">
+        <v>44939</v>
+      </c>
+    </row>
+    <row r="2572" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2572">
+        <v>2023</v>
+      </c>
+      <c r="B2572">
+        <v>14</v>
+      </c>
+      <c r="C2572" s="1">
+        <v>44940</v>
+      </c>
+    </row>
+    <row r="2573" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2573">
+        <v>2023</v>
+      </c>
+      <c r="B2573">
+        <v>15</v>
+      </c>
+      <c r="C2573" s="1">
+        <v>44941</v>
+      </c>
+    </row>
+    <row r="2574" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2574">
+        <v>2023</v>
+      </c>
+      <c r="B2574">
+        <v>16</v>
+      </c>
+      <c r="C2574" s="1">
+        <v>44942</v>
+      </c>
+    </row>
+    <row r="2575" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2575">
+        <v>2023</v>
+      </c>
+      <c r="B2575">
+        <v>17</v>
+      </c>
+      <c r="C2575" s="1">
+        <v>44943</v>
+      </c>
+    </row>
+    <row r="2576" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2576">
+        <v>2023</v>
+      </c>
+      <c r="B2576">
+        <v>18</v>
+      </c>
+      <c r="C2576" s="1">
+        <v>44944</v>
+      </c>
+    </row>
+    <row r="2577" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2577">
+        <v>2023</v>
+      </c>
+      <c r="B2577">
+        <v>19</v>
+      </c>
+      <c r="C2577" s="1">
+        <v>44945</v>
+      </c>
+    </row>
+    <row r="2578" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2578">
+        <v>2023</v>
+      </c>
+      <c r="B2578">
+        <v>20</v>
+      </c>
+      <c r="C2578" s="1">
+        <v>44946</v>
+      </c>
+    </row>
+    <row r="2579" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2579">
+        <v>2023</v>
+      </c>
+      <c r="B2579">
+        <v>21</v>
+      </c>
+      <c r="C2579" s="1">
+        <v>44947</v>
+      </c>
+    </row>
+    <row r="2580" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2580">
+        <v>2023</v>
+      </c>
+      <c r="B2580">
+        <v>22</v>
+      </c>
+      <c r="C2580" s="1">
+        <v>44948</v>
+      </c>
+    </row>
+    <row r="2581" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2581">
+        <v>2023</v>
+      </c>
+      <c r="B2581">
+        <v>23</v>
+      </c>
+      <c r="C2581" s="1">
+        <v>44949</v>
+      </c>
+    </row>
+    <row r="2582" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2582">
+        <v>2023</v>
+      </c>
+      <c r="B2582">
+        <v>24</v>
+      </c>
+      <c r="C2582" s="1">
+        <v>44950</v>
+      </c>
+    </row>
+    <row r="2583" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2583">
+        <v>2023</v>
+      </c>
+      <c r="B2583">
+        <v>25</v>
+      </c>
+      <c r="C2583" s="1">
+        <v>44951</v>
+      </c>
+    </row>
+    <row r="2584" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2584">
+        <v>2023</v>
+      </c>
+      <c r="B2584">
+        <v>26</v>
+      </c>
+      <c r="C2584" s="1">
+        <v>44952</v>
+      </c>
+    </row>
+    <row r="2585" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2585">
+        <v>2023</v>
+      </c>
+      <c r="B2585">
+        <v>27</v>
+      </c>
+      <c r="C2585" s="1">
+        <v>44953</v>
+      </c>
+    </row>
+    <row r="2586" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2586">
+        <v>2023</v>
+      </c>
+      <c r="B2586">
+        <v>28</v>
+      </c>
+      <c r="C2586" s="1">
+        <v>44954</v>
+      </c>
+    </row>
+    <row r="2587" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2587">
+        <v>2023</v>
+      </c>
+      <c r="B2587">
+        <v>29</v>
+      </c>
+      <c r="C2587" s="1">
+        <v>44955</v>
+      </c>
+    </row>
+    <row r="2588" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2588">
+        <v>2023</v>
+      </c>
+      <c r="B2588">
+        <v>30</v>
+      </c>
+      <c r="C2588" s="1">
+        <v>44956</v>
+      </c>
+    </row>
+    <row r="2589" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2589">
+        <v>2023</v>
+      </c>
+      <c r="B2589">
+        <v>31</v>
+      </c>
+      <c r="C2589" s="1">
+        <v>44957</v>
+      </c>
+    </row>
+    <row r="2590" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2590">
+        <v>2023</v>
+      </c>
+      <c r="B2590">
+        <v>32</v>
+      </c>
+      <c r="C2590" s="1">
+        <v>44958</v>
+      </c>
+    </row>
+    <row r="2591" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2591">
+        <v>2023</v>
+      </c>
+      <c r="B2591">
+        <v>33</v>
+      </c>
+      <c r="C2591" s="1">
+        <v>44959</v>
+      </c>
+    </row>
+    <row r="2592" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2592">
+        <v>2023</v>
+      </c>
+      <c r="B2592">
+        <v>34</v>
+      </c>
+      <c r="C2592" s="1">
+        <v>44960</v>
+      </c>
+    </row>
+    <row r="2593" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2593">
+        <v>2023</v>
+      </c>
+      <c r="B2593">
+        <v>35</v>
+      </c>
+      <c r="C2593" s="1">
+        <v>44961</v>
+      </c>
+    </row>
+    <row r="2594" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2594">
+        <v>2023</v>
+      </c>
+      <c r="B2594">
+        <v>36</v>
+      </c>
+      <c r="C2594" s="1">
+        <v>44962</v>
+      </c>
+    </row>
+    <row r="2595" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2595">
+        <v>2023</v>
+      </c>
+      <c r="B2595">
+        <v>37</v>
+      </c>
+      <c r="C2595" s="1">
+        <v>44963</v>
+      </c>
+    </row>
+    <row r="2596" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2596">
+        <v>2023</v>
+      </c>
+      <c r="B2596">
+        <v>38</v>
+      </c>
+      <c r="C2596" s="1">
+        <v>44964</v>
+      </c>
+    </row>
+    <row r="2597" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2597">
+        <v>2023</v>
+      </c>
+      <c r="B2597">
+        <v>39</v>
+      </c>
+      <c r="C2597" s="1">
+        <v>44965</v>
+      </c>
+    </row>
+    <row r="2598" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2598">
+        <v>2023</v>
+      </c>
+      <c r="B2598">
+        <v>40</v>
+      </c>
+      <c r="C2598" s="1">
+        <v>44966</v>
+      </c>
+    </row>
+    <row r="2599" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2599">
+        <v>2023</v>
+      </c>
+      <c r="B2599">
+        <v>41</v>
+      </c>
+      <c r="C2599" s="1">
+        <v>44967</v>
+      </c>
+    </row>
+    <row r="2600" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2600">
+        <v>2023</v>
+      </c>
+      <c r="B2600">
+        <v>42</v>
+      </c>
+      <c r="C2600" s="1">
+        <v>44968</v>
+      </c>
+    </row>
+    <row r="2601" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2601">
+        <v>2023</v>
+      </c>
+      <c r="B2601">
+        <v>43</v>
+      </c>
+      <c r="C2601" s="1">
+        <v>44969</v>
+      </c>
+    </row>
+    <row r="2602" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2602">
+        <v>2023</v>
+      </c>
+      <c r="B2602">
+        <v>44</v>
+      </c>
+      <c r="C2602" s="1">
+        <v>44970</v>
+      </c>
+    </row>
+    <row r="2603" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2603">
+        <v>2023</v>
+      </c>
+      <c r="B2603">
+        <v>45</v>
+      </c>
+      <c r="C2603" s="1">
+        <v>44971</v>
+      </c>
+    </row>
+    <row r="2604" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2604">
+        <v>2023</v>
+      </c>
+      <c r="B2604">
+        <v>46</v>
+      </c>
+      <c r="C2604" s="1">
+        <v>44972</v>
+      </c>
+    </row>
+    <row r="2605" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2605">
+        <v>2023</v>
+      </c>
+      <c r="B2605">
+        <v>47</v>
+      </c>
+      <c r="C2605" s="1">
+        <v>44973</v>
+      </c>
+    </row>
+    <row r="2606" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2606">
+        <v>2023</v>
+      </c>
+      <c r="B2606">
+        <v>48</v>
+      </c>
+      <c r="C2606" s="1">
+        <v>44974</v>
+      </c>
+    </row>
+    <row r="2607" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2607">
+        <v>2023</v>
+      </c>
+      <c r="B2607">
+        <v>49</v>
+      </c>
+      <c r="C2607" s="1">
+        <v>44975</v>
+      </c>
+    </row>
+    <row r="2608" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2608">
+        <v>2023</v>
+      </c>
+      <c r="B2608">
+        <v>50</v>
+      </c>
+      <c r="C2608" s="1">
+        <v>44976</v>
+      </c>
+    </row>
+    <row r="2609" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2609">
+        <v>2023</v>
+      </c>
+      <c r="B2609">
+        <v>51</v>
+      </c>
+      <c r="C2609" s="1">
+        <v>44977</v>
+      </c>
+    </row>
+    <row r="2610" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2610">
+        <v>2023</v>
+      </c>
+      <c r="B2610">
+        <v>52</v>
+      </c>
+      <c r="C2610" s="1">
+        <v>44978</v>
+      </c>
+    </row>
+    <row r="2611" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2611">
+        <v>2023</v>
+      </c>
+      <c r="B2611">
+        <v>53</v>
+      </c>
+      <c r="C2611" s="1">
+        <v>44979</v>
+      </c>
+    </row>
+    <row r="2612" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2612">
+        <v>2023</v>
+      </c>
+      <c r="B2612">
+        <v>54</v>
+      </c>
+      <c r="C2612" s="1">
+        <v>44980</v>
+      </c>
+    </row>
+    <row r="2613" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2613">
+        <v>2023</v>
+      </c>
+      <c r="B2613">
+        <v>55</v>
+      </c>
+      <c r="C2613" s="1">
+        <v>44981</v>
+      </c>
+    </row>
+    <row r="2614" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2614">
+        <v>2023</v>
+      </c>
+      <c r="B2614">
+        <v>56</v>
+      </c>
+      <c r="C2614" s="1">
+        <v>44982</v>
+      </c>
+    </row>
+    <row r="2615" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2615">
+        <v>2023</v>
+      </c>
+      <c r="B2615">
+        <v>57</v>
+      </c>
+      <c r="C2615" s="1">
+        <v>44983</v>
+      </c>
+    </row>
+    <row r="2616" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2616">
+        <v>2023</v>
+      </c>
+      <c r="B2616">
+        <v>58</v>
+      </c>
+      <c r="C2616" s="1">
+        <v>44984</v>
+      </c>
+    </row>
+    <row r="2617" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2617">
+        <v>2023</v>
+      </c>
+      <c r="B2617">
+        <v>59</v>
+      </c>
+      <c r="C2617" s="1">
+        <v>44985</v>
+      </c>
+    </row>
+    <row r="2618" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2618">
+        <v>2023</v>
+      </c>
+      <c r="B2618">
+        <v>60</v>
+      </c>
+      <c r="C2618" s="1">
+        <v>44986</v>
+      </c>
+    </row>
+    <row r="2619" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2619">
+        <v>2023</v>
+      </c>
+      <c r="B2619">
+        <v>61</v>
+      </c>
+      <c r="C2619" s="1">
+        <v>44987</v>
+      </c>
+    </row>
+    <row r="2620" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2620">
+        <v>2023</v>
+      </c>
+      <c r="B2620">
+        <v>62</v>
+      </c>
+      <c r="C2620" s="1">
+        <v>44988</v>
+      </c>
+    </row>
+    <row r="2621" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2621">
+        <v>2023</v>
+      </c>
+      <c r="B2621">
+        <v>63</v>
+      </c>
+      <c r="C2621" s="1">
+        <v>44989</v>
+      </c>
+    </row>
+    <row r="2622" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2622">
+        <v>2023</v>
+      </c>
+      <c r="B2622">
+        <v>64</v>
+      </c>
+      <c r="C2622" s="1">
+        <v>44990</v>
+      </c>
+    </row>
+    <row r="2623" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2623">
+        <v>2023</v>
+      </c>
+      <c r="B2623">
+        <v>65</v>
+      </c>
+      <c r="C2623" s="1">
+        <v>44991</v>
+      </c>
+    </row>
+    <row r="2624" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2624">
+        <v>2023</v>
+      </c>
+      <c r="B2624">
+        <v>66</v>
+      </c>
+      <c r="C2624" s="1">
+        <v>44992</v>
+      </c>
+    </row>
+    <row r="2625" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2625">
+        <v>2023</v>
+      </c>
+      <c r="B2625">
+        <v>67</v>
+      </c>
+      <c r="C2625" s="1">
+        <v>44993</v>
+      </c>
+    </row>
+    <row r="2626" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2626">
+        <v>2023</v>
+      </c>
+      <c r="B2626">
+        <v>68</v>
+      </c>
+      <c r="C2626" s="1">
+        <v>44994</v>
+      </c>
+    </row>
+    <row r="2627" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2627">
+        <v>2023</v>
+      </c>
+      <c r="B2627">
+        <v>69</v>
+      </c>
+      <c r="C2627" s="1">
+        <v>44995</v>
+      </c>
+    </row>
+    <row r="2628" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2628">
+        <v>2023</v>
+      </c>
+      <c r="B2628">
+        <v>70</v>
+      </c>
+      <c r="C2628" s="1">
+        <v>44996</v>
+      </c>
+    </row>
+    <row r="2629" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2629">
+        <v>2023</v>
+      </c>
+      <c r="B2629">
+        <v>71</v>
+      </c>
+      <c r="C2629" s="1">
+        <v>44997</v>
+      </c>
+    </row>
+    <row r="2630" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2630">
+        <v>2023</v>
+      </c>
+      <c r="B2630">
+        <v>72</v>
+      </c>
+      <c r="C2630" s="1">
+        <v>44998</v>
+      </c>
+    </row>
+    <row r="2631" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2631">
+        <v>2023</v>
+      </c>
+      <c r="B2631">
+        <v>73</v>
+      </c>
+      <c r="C2631" s="1">
+        <v>44999</v>
+      </c>
+    </row>
+    <row r="2632" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2632">
+        <v>2023</v>
+      </c>
+      <c r="B2632">
+        <v>74</v>
+      </c>
+      <c r="C2632" s="1">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="2633" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2633">
+        <v>2023</v>
+      </c>
+      <c r="B2633">
+        <v>75</v>
+      </c>
+      <c r="C2633" s="1">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="2634" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2634">
+        <v>2023</v>
+      </c>
+      <c r="B2634">
+        <v>76</v>
+      </c>
+      <c r="C2634" s="1">
+        <v>45002</v>
+      </c>
+    </row>
+    <row r="2635" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2635">
+        <v>2023</v>
+      </c>
+      <c r="B2635">
+        <v>77</v>
+      </c>
+      <c r="C2635" s="1">
+        <v>45003</v>
+      </c>
+    </row>
+    <row r="2636" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2636">
+        <v>2023</v>
+      </c>
+      <c r="B2636">
+        <v>78</v>
+      </c>
+      <c r="C2636" s="1">
+        <v>45004</v>
+      </c>
+    </row>
+    <row r="2637" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2637">
+        <v>2023</v>
+      </c>
+      <c r="B2637">
+        <v>79</v>
+      </c>
+      <c r="C2637" s="1">
+        <v>45005</v>
+      </c>
+    </row>
+    <row r="2638" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2638">
+        <v>2023</v>
+      </c>
+      <c r="B2638">
+        <v>80</v>
+      </c>
+      <c r="C2638" s="1">
+        <v>45006</v>
+      </c>
+    </row>
+    <row r="2639" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2639">
+        <v>2023</v>
+      </c>
+      <c r="B2639">
+        <v>81</v>
+      </c>
+      <c r="C2639" s="1">
+        <v>45007</v>
+      </c>
+    </row>
+    <row r="2640" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2640">
+        <v>2023</v>
+      </c>
+      <c r="B2640">
+        <v>82</v>
+      </c>
+      <c r="C2640" s="1">
+        <v>45008</v>
+      </c>
+    </row>
+    <row r="2641" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2641">
+        <v>2023</v>
+      </c>
+      <c r="B2641">
+        <v>83</v>
+      </c>
+      <c r="C2641" s="1">
+        <v>45009</v>
+      </c>
+    </row>
+    <row r="2642" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2642">
+        <v>2023</v>
+      </c>
+      <c r="B2642">
+        <v>84</v>
+      </c>
+      <c r="C2642" s="1">
+        <v>45010</v>
+      </c>
+    </row>
+    <row r="2643" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2643">
+        <v>2023</v>
+      </c>
+      <c r="B2643">
+        <v>85</v>
+      </c>
+      <c r="C2643" s="1">
+        <v>45011</v>
+      </c>
+    </row>
+    <row r="2644" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2644">
+        <v>2023</v>
+      </c>
+      <c r="B2644">
+        <v>86</v>
+      </c>
+      <c r="C2644" s="1">
+        <v>45012</v>
+      </c>
+    </row>
+    <row r="2645" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2645">
+        <v>2023</v>
+      </c>
+      <c r="B2645">
+        <v>87</v>
+      </c>
+      <c r="C2645" s="1">
+        <v>45013</v>
+      </c>
+    </row>
+    <row r="2646" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2646">
+        <v>2023</v>
+      </c>
+      <c r="B2646">
+        <v>88</v>
+      </c>
+      <c r="C2646" s="1">
+        <v>45014</v>
+      </c>
+    </row>
+    <row r="2647" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2647">
+        <v>2023</v>
+      </c>
+      <c r="B2647">
+        <v>89</v>
+      </c>
+      <c r="C2647" s="1">
+        <v>45015</v>
+      </c>
+    </row>
+    <row r="2648" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2648">
+        <v>2023</v>
+      </c>
+      <c r="B2648">
+        <v>90</v>
+      </c>
+      <c r="C2648" s="1">
+        <v>45016</v>
+      </c>
+    </row>
+    <row r="2649" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2649">
+        <v>2023</v>
+      </c>
+      <c r="B2649">
+        <v>91</v>
+      </c>
+      <c r="C2649" s="1">
+        <v>45017</v>
+      </c>
+    </row>
+    <row r="2650" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2650">
+        <v>2023</v>
+      </c>
+      <c r="B2650">
+        <v>92</v>
+      </c>
+      <c r="C2650" s="1">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="2651" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2651">
+        <v>2023</v>
+      </c>
+      <c r="B2651">
+        <v>93</v>
+      </c>
+      <c r="C2651" s="1">
+        <v>45019</v>
+      </c>
+    </row>
+    <row r="2652" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2652">
+        <v>2023</v>
+      </c>
+      <c r="B2652">
+        <v>94</v>
+      </c>
+      <c r="C2652" s="1">
+        <v>45020</v>
+      </c>
+    </row>
+    <row r="2653" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2653">
+        <v>2023</v>
+      </c>
+      <c r="B2653">
+        <v>95</v>
+      </c>
+      <c r="C2653" s="1">
+        <v>45021</v>
+      </c>
+    </row>
+    <row r="2654" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2654">
+        <v>2023</v>
+      </c>
+      <c r="B2654">
+        <v>96</v>
+      </c>
+      <c r="C2654" s="1">
+        <v>45022</v>
+      </c>
+    </row>
+    <row r="2655" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2655">
+        <v>2023</v>
+      </c>
+      <c r="B2655">
+        <v>97</v>
+      </c>
+      <c r="C2655" s="1">
+        <v>45023</v>
+      </c>
+    </row>
+    <row r="2656" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2656">
+        <v>2023</v>
+      </c>
+      <c r="B2656">
+        <v>98</v>
+      </c>
+      <c r="C2656" s="1">
+        <v>45024</v>
+      </c>
+    </row>
+    <row r="2657" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2657">
+        <v>2023</v>
+      </c>
+      <c r="B2657">
+        <v>99</v>
+      </c>
+      <c r="C2657" s="1">
+        <v>45025</v>
+      </c>
+    </row>
+    <row r="2658" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2658">
+        <v>2023</v>
+      </c>
+      <c r="B2658">
+        <v>100</v>
+      </c>
+      <c r="C2658" s="1">
+        <v>45026</v>
+      </c>
+    </row>
+    <row r="2659" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2659">
+        <v>2023</v>
+      </c>
+      <c r="B2659">
+        <v>101</v>
+      </c>
+      <c r="C2659" s="1">
+        <v>45027</v>
+      </c>
+    </row>
+    <row r="2660" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2660">
+        <v>2023</v>
+      </c>
+      <c r="B2660">
+        <v>102</v>
+      </c>
+      <c r="C2660" s="1">
+        <v>45028</v>
+      </c>
+    </row>
+    <row r="2661" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2661">
+        <v>2023</v>
+      </c>
+      <c r="B2661">
+        <v>103</v>
+      </c>
+      <c r="C2661" s="1">
+        <v>45029</v>
+      </c>
+    </row>
+    <row r="2662" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2662">
+        <v>2023</v>
+      </c>
+      <c r="B2662">
+        <v>104</v>
+      </c>
+      <c r="C2662" s="1">
+        <v>45030</v>
+      </c>
+    </row>
+    <row r="2663" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2663">
+        <v>2023</v>
+      </c>
+      <c r="B2663">
+        <v>105</v>
+      </c>
+      <c r="C2663" s="1">
+        <v>45031</v>
+      </c>
+    </row>
+    <row r="2664" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2664">
+        <v>2023</v>
+      </c>
+      <c r="B2664">
+        <v>106</v>
+      </c>
+      <c r="C2664" s="1">
+        <v>45032</v>
+      </c>
+    </row>
+    <row r="2665" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2665">
+        <v>2023</v>
+      </c>
+      <c r="B2665">
+        <v>107</v>
+      </c>
+      <c r="C2665" s="1">
+        <v>45033</v>
+      </c>
+    </row>
+    <row r="2666" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2666">
+        <v>2023</v>
+      </c>
+      <c r="B2666">
+        <v>108</v>
+      </c>
+      <c r="C2666" s="1">
+        <v>45034</v>
+      </c>
+    </row>
+    <row r="2667" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2667">
+        <v>2023</v>
+      </c>
+      <c r="B2667">
+        <v>109</v>
+      </c>
+      <c r="C2667" s="1">
+        <v>45035</v>
+      </c>
+    </row>
+    <row r="2668" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2668">
+        <v>2023</v>
+      </c>
+      <c r="B2668">
+        <v>110</v>
+      </c>
+      <c r="C2668" s="1">
+        <v>45036</v>
+      </c>
+    </row>
+    <row r="2669" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2669">
+        <v>2023</v>
+      </c>
+      <c r="B2669">
+        <v>111</v>
+      </c>
+      <c r="C2669" s="1">
+        <v>45037</v>
+      </c>
+    </row>
+    <row r="2670" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2670">
+        <v>2023</v>
+      </c>
+      <c r="B2670">
+        <v>112</v>
+      </c>
+      <c r="C2670" s="1">
+        <v>45038</v>
+      </c>
+    </row>
+    <row r="2671" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2671">
+        <v>2023</v>
+      </c>
+      <c r="B2671">
+        <v>113</v>
+      </c>
+      <c r="C2671" s="1">
+        <v>45039</v>
+      </c>
+    </row>
+    <row r="2672" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2672">
+        <v>2023</v>
+      </c>
+      <c r="B2672">
+        <v>114</v>
+      </c>
+      <c r="C2672" s="1">
+        <v>45040</v>
+      </c>
+    </row>
+    <row r="2673" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2673">
+        <v>2023</v>
+      </c>
+      <c r="B2673">
+        <v>115</v>
+      </c>
+      <c r="C2673" s="1">
+        <v>45041</v>
+      </c>
+    </row>
+    <row r="2674" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2674">
+        <v>2023</v>
+      </c>
+      <c r="B2674">
+        <v>116</v>
+      </c>
+      <c r="C2674" s="1">
+        <v>45042</v>
+      </c>
+    </row>
+    <row r="2675" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2675">
+        <v>2023</v>
+      </c>
+      <c r="B2675">
+        <v>117</v>
+      </c>
+      <c r="C2675" s="1">
+        <v>45043</v>
+      </c>
+    </row>
+    <row r="2676" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2676">
+        <v>2023</v>
+      </c>
+      <c r="B2676">
+        <v>118</v>
+      </c>
+      <c r="C2676" s="1">
+        <v>45044</v>
+      </c>
+    </row>
+    <row r="2677" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2677">
+        <v>2023</v>
+      </c>
+      <c r="B2677">
+        <v>119</v>
+      </c>
+      <c r="C2677" s="1">
+        <v>45045</v>
+      </c>
+    </row>
+    <row r="2678" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2678">
+        <v>2023</v>
+      </c>
+      <c r="B2678">
+        <v>120</v>
+      </c>
+      <c r="C2678" s="1">
+        <v>45046</v>
+      </c>
+    </row>
+    <row r="2679" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2679">
+        <v>2023</v>
+      </c>
+      <c r="B2679">
+        <v>121</v>
+      </c>
+      <c r="C2679" s="1">
+        <v>45047</v>
+      </c>
+    </row>
+    <row r="2680" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2680">
+        <v>2023</v>
+      </c>
+      <c r="B2680">
+        <v>122</v>
+      </c>
+      <c r="C2680" s="1">
+        <v>45048</v>
+      </c>
+    </row>
+    <row r="2681" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2681">
+        <v>2023</v>
+      </c>
+      <c r="B2681">
+        <v>123</v>
+      </c>
+      <c r="C2681" s="1">
+        <v>45049</v>
+      </c>
+    </row>
+    <row r="2682" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2682">
+        <v>2023</v>
+      </c>
+      <c r="B2682">
+        <v>124</v>
+      </c>
+      <c r="C2682" s="1">
+        <v>45050</v>
+      </c>
+    </row>
+    <row r="2683" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2683">
+        <v>2023</v>
+      </c>
+      <c r="B2683">
+        <v>125</v>
+      </c>
+      <c r="C2683" s="1">
+        <v>45051</v>
+      </c>
+    </row>
+    <row r="2684" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2684">
+        <v>2023</v>
+      </c>
+      <c r="B2684">
+        <v>126</v>
+      </c>
+      <c r="C2684" s="1">
+        <v>45052</v>
+      </c>
+    </row>
+    <row r="2685" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2685">
+        <v>2023</v>
+      </c>
+      <c r="B2685">
+        <v>127</v>
+      </c>
+      <c r="C2685" s="1">
+        <v>45053</v>
+      </c>
+    </row>
+    <row r="2686" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2686">
+        <v>2023</v>
+      </c>
+      <c r="B2686">
+        <v>128</v>
+      </c>
+      <c r="C2686" s="1">
+        <v>45054</v>
+      </c>
+    </row>
+    <row r="2687" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2687">
+        <v>2023</v>
+      </c>
+      <c r="B2687">
+        <v>129</v>
+      </c>
+      <c r="C2687" s="1">
+        <v>45055</v>
+      </c>
+    </row>
+    <row r="2688" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2688">
+        <v>2023</v>
+      </c>
+      <c r="B2688">
+        <v>130</v>
+      </c>
+      <c r="C2688" s="1">
+        <v>45056</v>
+      </c>
+    </row>
+    <row r="2689" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2689">
+        <v>2023</v>
+      </c>
+      <c r="B2689">
+        <v>131</v>
+      </c>
+      <c r="C2689" s="1">
+        <v>45057</v>
+      </c>
+    </row>
+    <row r="2690" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2690">
+        <v>2023</v>
+      </c>
+      <c r="B2690">
+        <v>132</v>
+      </c>
+      <c r="C2690" s="1">
+        <v>45058</v>
+      </c>
+    </row>
+    <row r="2691" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2691">
+        <v>2023</v>
+      </c>
+      <c r="B2691">
+        <v>133</v>
+      </c>
+      <c r="C2691" s="1">
+        <v>45059</v>
+      </c>
+    </row>
+    <row r="2692" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2692">
+        <v>2023</v>
+      </c>
+      <c r="B2692">
+        <v>134</v>
+      </c>
+      <c r="C2692" s="1">
+        <v>45060</v>
+      </c>
+    </row>
+    <row r="2693" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2693">
+        <v>2023</v>
+      </c>
+      <c r="B2693">
+        <v>135</v>
+      </c>
+      <c r="C2693" s="1">
+        <v>45061</v>
+      </c>
+    </row>
+    <row r="2694" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2694">
+        <v>2023</v>
+      </c>
+      <c r="B2694">
+        <v>136</v>
+      </c>
+      <c r="C2694" s="1">
+        <v>45062</v>
+      </c>
+    </row>
+    <row r="2695" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2695">
+        <v>2023</v>
+      </c>
+      <c r="B2695">
+        <v>137</v>
+      </c>
+      <c r="C2695" s="1">
+        <v>45063</v>
+      </c>
+    </row>
+    <row r="2696" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2696">
+        <v>2023</v>
+      </c>
+      <c r="B2696">
+        <v>138</v>
+      </c>
+      <c r="C2696" s="1">
+        <v>45064</v>
+      </c>
+    </row>
+    <row r="2697" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2697">
+        <v>2023</v>
+      </c>
+      <c r="B2697">
+        <v>139</v>
+      </c>
+      <c r="C2697" s="1">
+        <v>45065</v>
+      </c>
+    </row>
+    <row r="2698" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2698">
+        <v>2023</v>
+      </c>
+      <c r="B2698">
+        <v>140</v>
+      </c>
+      <c r="C2698" s="1">
+        <v>45066</v>
+      </c>
+    </row>
+    <row r="2699" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2699">
+        <v>2023</v>
+      </c>
+      <c r="B2699">
+        <v>141</v>
+      </c>
+      <c r="C2699" s="1">
+        <v>45067</v>
+      </c>
+    </row>
+    <row r="2700" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2700">
+        <v>2023</v>
+      </c>
+      <c r="B2700">
+        <v>142</v>
+      </c>
+      <c r="C2700" s="1">
+        <v>45068</v>
+      </c>
+    </row>
+    <row r="2701" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2701">
+        <v>2023</v>
+      </c>
+      <c r="B2701">
+        <v>143</v>
+      </c>
+      <c r="C2701" s="1">
+        <v>45069</v>
+      </c>
+    </row>
+    <row r="2702" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2702">
+        <v>2023</v>
+      </c>
+      <c r="B2702">
+        <v>144</v>
+      </c>
+      <c r="C2702" s="1">
+        <v>45070</v>
+      </c>
+    </row>
+    <row r="2703" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2703">
+        <v>2023</v>
+      </c>
+      <c r="B2703">
+        <v>145</v>
+      </c>
+      <c r="C2703" s="1">
+        <v>45071</v>
+      </c>
+    </row>
+    <row r="2704" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2704">
+        <v>2023</v>
+      </c>
+      <c r="B2704">
+        <v>146</v>
+      </c>
+      <c r="C2704" s="1">
+        <v>45072</v>
+      </c>
+    </row>
+    <row r="2705" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2705">
+        <v>2023</v>
+      </c>
+      <c r="B2705">
+        <v>147</v>
+      </c>
+      <c r="C2705" s="1">
+        <v>45073</v>
+      </c>
+    </row>
+    <row r="2706" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2706">
+        <v>2023</v>
+      </c>
+      <c r="B2706">
+        <v>148</v>
+      </c>
+      <c r="C2706" s="1">
+        <v>45074</v>
+      </c>
+    </row>
+    <row r="2707" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2707">
+        <v>2023</v>
+      </c>
+      <c r="B2707">
+        <v>149</v>
+      </c>
+      <c r="C2707" s="1">
+        <v>45075</v>
+      </c>
+    </row>
+    <row r="2708" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2708">
+        <v>2023</v>
+      </c>
+      <c r="B2708">
+        <v>150</v>
+      </c>
+      <c r="C2708" s="1">
+        <v>45076</v>
+      </c>
+    </row>
+    <row r="2709" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2709">
+        <v>2023</v>
+      </c>
+      <c r="B2709">
+        <v>151</v>
+      </c>
+      <c r="C2709" s="1">
+        <v>45077</v>
+      </c>
+    </row>
+    <row r="2710" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2710">
+        <v>2023</v>
+      </c>
+      <c r="B2710">
+        <v>152</v>
+      </c>
+      <c r="C2710" s="1">
+        <v>45078</v>
+      </c>
+    </row>
+    <row r="2711" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2711">
+        <v>2023</v>
+      </c>
+      <c r="B2711">
+        <v>153</v>
+      </c>
+      <c r="C2711" s="1">
+        <v>45079</v>
+      </c>
+    </row>
+    <row r="2712" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2712">
+        <v>2023</v>
+      </c>
+      <c r="B2712">
+        <v>154</v>
+      </c>
+      <c r="C2712" s="1">
+        <v>45080</v>
+      </c>
+    </row>
+    <row r="2713" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2713">
+        <v>2023</v>
+      </c>
+      <c r="B2713">
+        <v>155</v>
+      </c>
+      <c r="C2713" s="1">
+        <v>45081</v>
+      </c>
+    </row>
+    <row r="2714" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2714">
+        <v>2023</v>
+      </c>
+      <c r="B2714">
+        <v>156</v>
+      </c>
+      <c r="C2714" s="1">
+        <v>45082</v>
+      </c>
+    </row>
+    <row r="2715" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2715">
+        <v>2023</v>
+      </c>
+      <c r="B2715">
+        <v>157</v>
+      </c>
+      <c r="C2715" s="1">
+        <v>45083</v>
+      </c>
+    </row>
+    <row r="2716" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2716">
+        <v>2023</v>
+      </c>
+      <c r="B2716">
+        <v>158</v>
+      </c>
+      <c r="C2716" s="1">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="2717" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2717">
+        <v>2023</v>
+      </c>
+      <c r="B2717">
+        <v>159</v>
+      </c>
+      <c r="C2717" s="1">
+        <v>45085</v>
+      </c>
+    </row>
+    <row r="2718" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2718">
+        <v>2023</v>
+      </c>
+      <c r="B2718">
+        <v>160</v>
+      </c>
+      <c r="C2718" s="1">
+        <v>45086</v>
+      </c>
+    </row>
+    <row r="2719" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2719">
+        <v>2023</v>
+      </c>
+      <c r="B2719">
+        <v>161</v>
+      </c>
+      <c r="C2719" s="1">
+        <v>45087</v>
+      </c>
+    </row>
+    <row r="2720" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2720">
+        <v>2023</v>
+      </c>
+      <c r="B2720">
+        <v>162</v>
+      </c>
+      <c r="C2720" s="1">
+        <v>45088</v>
+      </c>
+    </row>
+    <row r="2721" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2721">
+        <v>2023</v>
+      </c>
+      <c r="B2721">
+        <v>163</v>
+      </c>
+      <c r="C2721" s="1">
+        <v>45089</v>
+      </c>
+    </row>
+    <row r="2722" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2722">
+        <v>2023</v>
+      </c>
+      <c r="B2722">
+        <v>164</v>
+      </c>
+      <c r="C2722" s="1">
+        <v>45090</v>
+      </c>
+    </row>
+    <row r="2723" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2723">
+        <v>2023</v>
+      </c>
+      <c r="B2723">
+        <v>165</v>
+      </c>
+      <c r="C2723" s="1">
+        <v>45091</v>
+      </c>
+    </row>
+    <row r="2724" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2724">
+        <v>2023</v>
+      </c>
+      <c r="B2724">
+        <v>166</v>
+      </c>
+      <c r="C2724" s="1">
+        <v>45092</v>
+      </c>
+    </row>
+    <row r="2725" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2725">
+        <v>2023</v>
+      </c>
+      <c r="B2725">
+        <v>167</v>
+      </c>
+      <c r="C2725" s="1">
+        <v>45093</v>
+      </c>
+    </row>
+    <row r="2726" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2726">
+        <v>2023</v>
+      </c>
+      <c r="B2726">
+        <v>168</v>
+      </c>
+      <c r="C2726" s="1">
+        <v>45094</v>
+      </c>
+    </row>
+    <row r="2727" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2727">
+        <v>2023</v>
+      </c>
+      <c r="B2727">
+        <v>169</v>
+      </c>
+      <c r="C2727" s="1">
+        <v>45095</v>
+      </c>
+    </row>
+    <row r="2728" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2728">
+        <v>2023</v>
+      </c>
+      <c r="B2728">
+        <v>170</v>
+      </c>
+      <c r="C2728" s="1">
+        <v>45096</v>
+      </c>
+    </row>
+    <row r="2729" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2729">
+        <v>2023</v>
+      </c>
+      <c r="B2729">
+        <v>171</v>
+      </c>
+      <c r="C2729" s="1">
+        <v>45097</v>
+      </c>
+    </row>
+    <row r="2730" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2730">
+        <v>2023</v>
+      </c>
+      <c r="B2730">
+        <v>172</v>
+      </c>
+      <c r="C2730" s="1">
+        <v>45098</v>
+      </c>
+    </row>
+    <row r="2731" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2731">
+        <v>2023</v>
+      </c>
+      <c r="B2731">
+        <v>173</v>
+      </c>
+      <c r="C2731" s="1">
+        <v>45099</v>
+      </c>
+    </row>
+    <row r="2732" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2732">
+        <v>2023</v>
+      </c>
+      <c r="B2732">
+        <v>174</v>
+      </c>
+      <c r="C2732" s="1">
+        <v>45100</v>
+      </c>
+    </row>
+    <row r="2733" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2733">
+        <v>2023</v>
+      </c>
+      <c r="B2733">
+        <v>175</v>
+      </c>
+      <c r="C2733" s="1">
+        <v>45101</v>
+      </c>
+    </row>
+    <row r="2734" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2734">
+        <v>2023</v>
+      </c>
+      <c r="B2734">
+        <v>176</v>
+      </c>
+      <c r="C2734" s="1">
+        <v>45102</v>
+      </c>
+    </row>
+    <row r="2735" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2735">
+        <v>2023</v>
+      </c>
+      <c r="B2735">
+        <v>177</v>
+      </c>
+      <c r="C2735" s="1">
+        <v>45103</v>
+      </c>
+    </row>
+    <row r="2736" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2736">
+        <v>2023</v>
+      </c>
+      <c r="B2736">
+        <v>178</v>
+      </c>
+      <c r="C2736" s="1">
+        <v>45104</v>
+      </c>
+    </row>
+    <row r="2737" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2737">
+        <v>2023</v>
+      </c>
+      <c r="B2737">
+        <v>179</v>
+      </c>
+      <c r="C2737" s="1">
+        <v>45105</v>
+      </c>
+    </row>
+    <row r="2738" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2738">
+        <v>2023</v>
+      </c>
+      <c r="B2738">
+        <v>180</v>
+      </c>
+      <c r="C2738" s="1">
+        <v>45106</v>
+      </c>
+    </row>
+    <row r="2739" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2739">
+        <v>2023</v>
+      </c>
+      <c r="B2739">
+        <v>181</v>
+      </c>
+      <c r="C2739" s="1">
+        <v>45107</v>
+      </c>
+    </row>
+    <row r="2740" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2740">
+        <v>2023</v>
+      </c>
+      <c r="B2740">
+        <v>182</v>
+      </c>
+      <c r="C2740" s="1">
+        <v>45108</v>
+      </c>
+    </row>
+    <row r="2741" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2741">
+        <v>2023</v>
+      </c>
+      <c r="B2741">
+        <v>183</v>
+      </c>
+      <c r="C2741" s="1">
+        <v>45109</v>
+      </c>
+    </row>
+    <row r="2742" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2742">
+        <v>2023</v>
+      </c>
+      <c r="B2742">
+        <v>184</v>
+      </c>
+      <c r="C2742" s="1">
+        <v>45110</v>
+      </c>
+    </row>
+    <row r="2743" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2743">
+        <v>2023</v>
+      </c>
+      <c r="B2743">
+        <v>185</v>
+      </c>
+      <c r="C2743" s="1">
+        <v>45111</v>
+      </c>
+    </row>
+    <row r="2744" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2744">
+        <v>2023</v>
+      </c>
+      <c r="B2744">
+        <v>186</v>
+      </c>
+      <c r="C2744" s="1">
+        <v>45112</v>
+      </c>
+    </row>
+    <row r="2745" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2745">
+        <v>2023</v>
+      </c>
+      <c r="B2745">
+        <v>187</v>
+      </c>
+      <c r="C2745" s="1">
+        <v>45113</v>
+      </c>
+    </row>
+    <row r="2746" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2746">
+        <v>2023</v>
+      </c>
+      <c r="B2746">
+        <v>188</v>
+      </c>
+      <c r="C2746" s="1">
+        <v>45114</v>
+      </c>
+    </row>
+    <row r="2747" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2747">
+        <v>2023</v>
+      </c>
+      <c r="B2747">
+        <v>189</v>
+      </c>
+      <c r="C2747" s="1">
+        <v>45115</v>
+      </c>
+    </row>
+    <row r="2748" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2748">
+        <v>2023</v>
+      </c>
+      <c r="B2748">
+        <v>190</v>
+      </c>
+      <c r="C2748" s="1">
+        <v>45116</v>
+      </c>
+    </row>
+    <row r="2749" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2749">
+        <v>2023</v>
+      </c>
+      <c r="B2749">
+        <v>191</v>
+      </c>
+      <c r="C2749" s="1">
+        <v>45117</v>
+      </c>
+    </row>
+    <row r="2750" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2750">
+        <v>2023</v>
+      </c>
+      <c r="B2750">
+        <v>192</v>
+      </c>
+      <c r="C2750" s="1">
+        <v>45118</v>
+      </c>
+    </row>
+    <row r="2751" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2751">
+        <v>2023</v>
+      </c>
+      <c r="B2751">
+        <v>193</v>
+      </c>
+      <c r="C2751" s="1">
+        <v>45119</v>
+      </c>
+    </row>
+    <row r="2752" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2752">
+        <v>2023</v>
+      </c>
+      <c r="B2752">
+        <v>194</v>
+      </c>
+      <c r="C2752" s="1">
+        <v>45120</v>
+      </c>
+    </row>
+    <row r="2753" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2753">
+        <v>2023</v>
+      </c>
+      <c r="B2753">
+        <v>195</v>
+      </c>
+      <c r="C2753" s="1">
+        <v>45121</v>
+      </c>
+    </row>
+    <row r="2754" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2754">
+        <v>2023</v>
+      </c>
+      <c r="B2754">
+        <v>196</v>
+      </c>
+      <c r="C2754" s="1">
+        <v>45122</v>
+      </c>
+    </row>
+    <row r="2755" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2755">
+        <v>2023</v>
+      </c>
+      <c r="B2755">
+        <v>197</v>
+      </c>
+      <c r="C2755" s="1">
+        <v>45123</v>
+      </c>
+    </row>
+    <row r="2756" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2756">
+        <v>2023</v>
+      </c>
+      <c r="B2756">
+        <v>198</v>
+      </c>
+      <c r="C2756" s="1">
+        <v>45124</v>
+      </c>
+    </row>
+    <row r="2757" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2757">
+        <v>2023</v>
+      </c>
+      <c r="B2757">
+        <v>199</v>
+      </c>
+      <c r="C2757" s="1">
+        <v>45125</v>
+      </c>
+    </row>
+    <row r="2758" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2758">
+        <v>2023</v>
+      </c>
+      <c r="B2758">
+        <v>200</v>
+      </c>
+      <c r="C2758" s="1">
+        <v>45126</v>
+      </c>
+    </row>
+    <row r="2759" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2759">
+        <v>2023</v>
+      </c>
+      <c r="B2759">
+        <v>201</v>
+      </c>
+      <c r="C2759" s="1">
+        <v>45127</v>
+      </c>
+    </row>
+    <row r="2760" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2760">
+        <v>2023</v>
+      </c>
+      <c r="B2760">
+        <v>202</v>
+      </c>
+      <c r="C2760" s="1">
+        <v>45128</v>
+      </c>
+    </row>
+    <row r="2761" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2761">
+        <v>2023</v>
+      </c>
+      <c r="B2761">
+        <v>203</v>
+      </c>
+      <c r="C2761" s="1">
+        <v>45129</v>
+      </c>
+    </row>
+    <row r="2762" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2762">
+        <v>2023</v>
+      </c>
+      <c r="B2762">
+        <v>204</v>
+      </c>
+      <c r="C2762" s="1">
+        <v>45130</v>
+      </c>
+    </row>
+    <row r="2763" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2763">
+        <v>2023</v>
+      </c>
+      <c r="B2763">
+        <v>205</v>
+      </c>
+      <c r="C2763" s="1">
+        <v>45131</v>
+      </c>
+    </row>
+    <row r="2764" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2764">
+        <v>2023</v>
+      </c>
+      <c r="B2764">
+        <v>206</v>
+      </c>
+      <c r="C2764" s="1">
+        <v>45132</v>
+      </c>
+    </row>
+    <row r="2765" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2765">
+        <v>2023</v>
+      </c>
+      <c r="B2765">
+        <v>207</v>
+      </c>
+      <c r="C2765" s="1">
+        <v>45133</v>
+      </c>
+    </row>
+    <row r="2766" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2766">
+        <v>2023</v>
+      </c>
+      <c r="B2766">
+        <v>208</v>
+      </c>
+      <c r="C2766" s="1">
+        <v>45134</v>
+      </c>
+    </row>
+    <row r="2767" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2767">
+        <v>2023</v>
+      </c>
+      <c r="B2767">
+        <v>209</v>
+      </c>
+      <c r="C2767" s="1">
+        <v>45135</v>
+      </c>
+    </row>
+    <row r="2768" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2768">
+        <v>2023</v>
+      </c>
+      <c r="B2768">
+        <v>210</v>
+      </c>
+      <c r="C2768" s="1">
+        <v>45136</v>
+      </c>
+    </row>
+    <row r="2769" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2769">
+        <v>2023</v>
+      </c>
+      <c r="B2769">
+        <v>211</v>
+      </c>
+      <c r="C2769" s="1">
+        <v>45137</v>
+      </c>
+    </row>
+    <row r="2770" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2770">
+        <v>2023</v>
+      </c>
+      <c r="B2770">
+        <v>212</v>
+      </c>
+      <c r="C2770" s="1">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="2771" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2771">
+        <v>2023</v>
+      </c>
+      <c r="B2771">
+        <v>213</v>
+      </c>
+      <c r="C2771" s="1">
+        <v>45139</v>
+      </c>
+    </row>
+    <row r="2772" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2772">
+        <v>2023</v>
+      </c>
+      <c r="B2772">
+        <v>214</v>
+      </c>
+      <c r="C2772" s="1">
+        <v>45140</v>
+      </c>
+    </row>
+    <row r="2773" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2773">
+        <v>2023</v>
+      </c>
+      <c r="B2773">
+        <v>215</v>
+      </c>
+      <c r="C2773" s="1">
+        <v>45141</v>
+      </c>
+    </row>
+    <row r="2774" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2774">
+        <v>2023</v>
+      </c>
+      <c r="B2774">
+        <v>216</v>
+      </c>
+      <c r="C2774" s="1">
+        <v>45142</v>
+      </c>
+    </row>
+    <row r="2775" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2775">
+        <v>2023</v>
+      </c>
+      <c r="B2775">
+        <v>217</v>
+      </c>
+      <c r="C2775" s="1">
+        <v>45143</v>
+      </c>
+    </row>
+    <row r="2776" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2776">
+        <v>2023</v>
+      </c>
+      <c r="B2776">
+        <v>218</v>
+      </c>
+      <c r="C2776" s="1">
+        <v>45144</v>
+      </c>
+    </row>
+    <row r="2777" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2777">
+        <v>2023</v>
+      </c>
+      <c r="B2777">
+        <v>219</v>
+      </c>
+      <c r="C2777" s="1">
+        <v>45145</v>
+      </c>
+    </row>
+    <row r="2778" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2778">
+        <v>2023</v>
+      </c>
+      <c r="B2778">
+        <v>220</v>
+      </c>
+      <c r="C2778" s="1">
+        <v>45146</v>
+      </c>
+    </row>
+    <row r="2779" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2779">
+        <v>2023</v>
+      </c>
+      <c r="B2779">
+        <v>221</v>
+      </c>
+      <c r="C2779" s="1">
+        <v>45147</v>
+      </c>
+    </row>
+    <row r="2780" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2780">
+        <v>2023</v>
+      </c>
+      <c r="B2780">
+        <v>222</v>
+      </c>
+      <c r="C2780" s="1">
+        <v>45148</v>
+      </c>
+    </row>
+    <row r="2781" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2781">
+        <v>2023</v>
+      </c>
+      <c r="B2781">
+        <v>223</v>
+      </c>
+      <c r="C2781" s="1">
+        <v>45149</v>
+      </c>
+    </row>
+    <row r="2782" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2782">
+        <v>2023</v>
+      </c>
+      <c r="B2782">
+        <v>224</v>
+      </c>
+      <c r="C2782" s="1">
+        <v>45150</v>
+      </c>
+    </row>
+    <row r="2783" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2783">
+        <v>2023</v>
+      </c>
+      <c r="B2783">
+        <v>225</v>
+      </c>
+      <c r="C2783" s="1">
+        <v>45151</v>
+      </c>
+    </row>
+    <row r="2784" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2784">
+        <v>2023</v>
+      </c>
+      <c r="B2784">
+        <v>226</v>
+      </c>
+      <c r="C2784" s="1">
+        <v>45152</v>
+      </c>
+    </row>
+    <row r="2785" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2785">
+        <v>2023</v>
+      </c>
+      <c r="B2785">
+        <v>227</v>
+      </c>
+      <c r="C2785" s="1">
+        <v>45153</v>
+      </c>
+    </row>
+    <row r="2786" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2786">
+        <v>2023</v>
+      </c>
+      <c r="B2786">
+        <v>228</v>
+      </c>
+      <c r="C2786" s="1">
+        <v>45154</v>
+      </c>
+    </row>
+    <row r="2787" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2787">
+        <v>2023</v>
+      </c>
+      <c r="B2787">
+        <v>229</v>
+      </c>
+      <c r="C2787" s="1">
+        <v>45155</v>
+      </c>
+    </row>
+    <row r="2788" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2788">
+        <v>2023</v>
+      </c>
+      <c r="B2788">
+        <v>230</v>
+      </c>
+      <c r="C2788" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="2789" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2789">
+        <v>2023</v>
+      </c>
+      <c r="B2789">
+        <v>231</v>
+      </c>
+      <c r="C2789" s="1">
+        <v>45157</v>
+      </c>
+    </row>
+    <row r="2790" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2790">
+        <v>2023</v>
+      </c>
+      <c r="B2790">
+        <v>232</v>
+      </c>
+      <c r="C2790" s="1">
+        <v>45158</v>
+      </c>
+    </row>
+    <row r="2791" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2791">
+        <v>2023</v>
+      </c>
+      <c r="B2791">
+        <v>233</v>
+      </c>
+      <c r="C2791" s="1">
+        <v>45159</v>
+      </c>
+    </row>
+    <row r="2792" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2792">
+        <v>2023</v>
+      </c>
+      <c r="B2792">
+        <v>234</v>
+      </c>
+      <c r="C2792" s="1">
+        <v>45160</v>
+      </c>
+    </row>
+    <row r="2793" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2793">
+        <v>2023</v>
+      </c>
+      <c r="B2793">
+        <v>235</v>
+      </c>
+      <c r="C2793" s="1">
+        <v>45161</v>
+      </c>
+    </row>
+    <row r="2794" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2794">
+        <v>2023</v>
+      </c>
+      <c r="B2794">
+        <v>236</v>
+      </c>
+      <c r="C2794" s="1">
+        <v>45162</v>
+      </c>
+    </row>
+    <row r="2795" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2795">
+        <v>2023</v>
+      </c>
+      <c r="B2795">
+        <v>237</v>
+      </c>
+      <c r="C2795" s="1">
+        <v>45163</v>
+      </c>
+    </row>
+    <row r="2796" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2796">
+        <v>2023</v>
+      </c>
+      <c r="B2796">
+        <v>238</v>
+      </c>
+      <c r="C2796" s="1">
+        <v>45164</v>
+      </c>
+    </row>
+    <row r="2797" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2797">
+        <v>2023</v>
+      </c>
+      <c r="B2797">
+        <v>239</v>
+      </c>
+      <c r="C2797" s="1">
+        <v>45165</v>
+      </c>
+    </row>
+    <row r="2798" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2798">
+        <v>2023</v>
+      </c>
+      <c r="B2798">
+        <v>240</v>
+      </c>
+      <c r="C2798" s="1">
+        <v>45166</v>
+      </c>
+    </row>
+    <row r="2799" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2799">
+        <v>2023</v>
+      </c>
+      <c r="B2799">
+        <v>241</v>
+      </c>
+      <c r="C2799" s="1">
+        <v>45167</v>
+      </c>
+    </row>
+    <row r="2800" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2800">
+        <v>2023</v>
+      </c>
+      <c r="B2800">
+        <v>242</v>
+      </c>
+      <c r="C2800" s="1">
+        <v>45168</v>
+      </c>
+    </row>
+    <row r="2801" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2801">
+        <v>2023</v>
+      </c>
+      <c r="B2801">
+        <v>243</v>
+      </c>
+      <c r="C2801" s="1">
+        <v>45169</v>
+      </c>
+    </row>
+    <row r="2802" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2802">
+        <v>2023</v>
+      </c>
+      <c r="B2802">
+        <v>244</v>
+      </c>
+      <c r="C2802" s="1">
+        <v>45170</v>
+      </c>
+    </row>
+    <row r="2803" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2803">
+        <v>2023</v>
+      </c>
+      <c r="B2803">
+        <v>245</v>
+      </c>
+      <c r="C2803" s="1">
+        <v>45171</v>
+      </c>
+    </row>
+    <row r="2804" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2804">
+        <v>2023</v>
+      </c>
+      <c r="B2804">
+        <v>246</v>
+      </c>
+      <c r="C2804" s="1">
+        <v>45172</v>
+      </c>
+    </row>
+    <row r="2805" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2805">
+        <v>2023</v>
+      </c>
+      <c r="B2805">
+        <v>247</v>
+      </c>
+      <c r="C2805" s="1">
+        <v>45173</v>
+      </c>
+    </row>
+    <row r="2806" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2806">
+        <v>2023</v>
+      </c>
+      <c r="B2806">
+        <v>248</v>
+      </c>
+      <c r="C2806" s="1">
+        <v>45174</v>
+      </c>
+    </row>
+    <row r="2807" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2807">
+        <v>2023</v>
+      </c>
+      <c r="B2807">
+        <v>249</v>
+      </c>
+      <c r="C2807" s="1">
+        <v>45175</v>
+      </c>
+    </row>
+    <row r="2808" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2808">
+        <v>2023</v>
+      </c>
+      <c r="B2808">
+        <v>250</v>
+      </c>
+      <c r="C2808" s="1">
+        <v>45176</v>
+      </c>
+    </row>
+    <row r="2809" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2809">
+        <v>2023</v>
+      </c>
+      <c r="B2809">
+        <v>251</v>
+      </c>
+      <c r="C2809" s="1">
+        <v>45177</v>
+      </c>
+    </row>
+    <row r="2810" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2810">
+        <v>2023</v>
+      </c>
+      <c r="B2810">
+        <v>252</v>
+      </c>
+      <c r="C2810" s="1">
+        <v>45178</v>
+      </c>
+    </row>
+    <row r="2811" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2811">
+        <v>2023</v>
+      </c>
+      <c r="B2811">
+        <v>253</v>
+      </c>
+      <c r="C2811" s="1">
+        <v>45179</v>
+      </c>
+    </row>
+    <row r="2812" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2812">
+        <v>2023</v>
+      </c>
+      <c r="B2812">
+        <v>254</v>
+      </c>
+      <c r="C2812" s="1">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="2813" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2813">
+        <v>2023</v>
+      </c>
+      <c r="B2813">
+        <v>255</v>
+      </c>
+      <c r="C2813" s="1">
+        <v>45181</v>
+      </c>
+    </row>
+    <row r="2814" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2814">
+        <v>2023</v>
+      </c>
+      <c r="B2814">
+        <v>256</v>
+      </c>
+      <c r="C2814" s="1">
+        <v>45182</v>
+      </c>
+    </row>
+    <row r="2815" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2815">
+        <v>2023</v>
+      </c>
+      <c r="B2815">
+        <v>257</v>
+      </c>
+      <c r="C2815" s="1">
+        <v>45183</v>
+      </c>
+    </row>
+    <row r="2816" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2816">
+        <v>2023</v>
+      </c>
+      <c r="B2816">
+        <v>258</v>
+      </c>
+      <c r="C2816" s="1">
+        <v>45184</v>
+      </c>
+    </row>
+    <row r="2817" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2817">
+        <v>2023</v>
+      </c>
+      <c r="B2817">
+        <v>259</v>
+      </c>
+      <c r="C2817" s="1">
+        <v>45185</v>
+      </c>
+    </row>
+    <row r="2818" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2818">
+        <v>2023</v>
+      </c>
+      <c r="B2818">
+        <v>260</v>
+      </c>
+      <c r="C2818" s="1">
+        <v>45186</v>
+      </c>
+    </row>
+    <row r="2819" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2819">
+        <v>2023</v>
+      </c>
+      <c r="B2819">
+        <v>261</v>
+      </c>
+      <c r="C2819" s="1">
+        <v>45187</v>
+      </c>
+    </row>
+    <row r="2820" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2820">
+        <v>2023</v>
+      </c>
+      <c r="B2820">
+        <v>262</v>
+      </c>
+      <c r="C2820" s="1">
+        <v>45188</v>
+      </c>
+    </row>
+    <row r="2821" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2821">
+        <v>2023</v>
+      </c>
+      <c r="B2821">
+        <v>263</v>
+      </c>
+      <c r="C2821" s="1">
+        <v>45189</v>
+      </c>
+    </row>
+    <row r="2822" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2822">
+        <v>2023</v>
+      </c>
+      <c r="B2822">
+        <v>264</v>
+      </c>
+      <c r="C2822" s="1">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="2823" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2823">
+        <v>2023</v>
+      </c>
+      <c r="B2823">
+        <v>265</v>
+      </c>
+      <c r="C2823" s="1">
+        <v>45191</v>
+      </c>
+    </row>
+    <row r="2824" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2824">
+        <v>2023</v>
+      </c>
+      <c r="B2824">
+        <v>266</v>
+      </c>
+      <c r="C2824" s="1">
+        <v>45192</v>
+      </c>
+    </row>
+    <row r="2825" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2825">
+        <v>2023</v>
+      </c>
+      <c r="B2825">
+        <v>267</v>
+      </c>
+      <c r="C2825" s="1">
+        <v>45193</v>
+      </c>
+    </row>
+    <row r="2826" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2826">
+        <v>2023</v>
+      </c>
+      <c r="B2826">
+        <v>268</v>
+      </c>
+      <c r="C2826" s="1">
+        <v>45194</v>
+      </c>
+    </row>
+    <row r="2827" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2827">
+        <v>2023</v>
+      </c>
+      <c r="B2827">
+        <v>269</v>
+      </c>
+      <c r="C2827" s="1">
+        <v>45195</v>
+      </c>
+    </row>
+    <row r="2828" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2828">
+        <v>2023</v>
+      </c>
+      <c r="B2828">
+        <v>270</v>
+      </c>
+      <c r="C2828" s="1">
+        <v>45196</v>
+      </c>
+    </row>
+    <row r="2829" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2829">
+        <v>2023</v>
+      </c>
+      <c r="B2829">
+        <v>271</v>
+      </c>
+      <c r="C2829" s="1">
+        <v>45197</v>
+      </c>
+    </row>
+    <row r="2830" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2830">
+        <v>2023</v>
+      </c>
+      <c r="B2830">
+        <v>272</v>
+      </c>
+      <c r="C2830" s="1">
+        <v>45198</v>
+      </c>
+    </row>
+    <row r="2831" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2831">
+        <v>2023</v>
+      </c>
+      <c r="B2831">
+        <v>273</v>
+      </c>
+      <c r="C2831" s="1">
+        <v>45199</v>
+      </c>
+    </row>
+    <row r="2832" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2832">
+        <v>2023</v>
+      </c>
+      <c r="B2832">
+        <v>274</v>
+      </c>
+      <c r="C2832" s="1">
+        <v>45200</v>
+      </c>
+    </row>
+    <row r="2833" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2833">
+        <v>2023</v>
+      </c>
+      <c r="B2833">
+        <v>275</v>
+      </c>
+      <c r="C2833" s="1">
+        <v>45201</v>
+      </c>
+    </row>
+    <row r="2834" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2834">
+        <v>2023</v>
+      </c>
+      <c r="B2834">
+        <v>276</v>
+      </c>
+      <c r="C2834" s="1">
+        <v>45202</v>
+      </c>
+    </row>
+    <row r="2835" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2835">
+        <v>2023</v>
+      </c>
+      <c r="B2835">
+        <v>277</v>
+      </c>
+      <c r="C2835" s="1">
+        <v>45203</v>
+      </c>
+    </row>
+    <row r="2836" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2836">
+        <v>2023</v>
+      </c>
+      <c r="B2836">
+        <v>278</v>
+      </c>
+      <c r="C2836" s="1">
+        <v>45204</v>
+      </c>
+    </row>
+    <row r="2837" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2837">
+        <v>2023</v>
+      </c>
+      <c r="B2837">
+        <v>279</v>
+      </c>
+      <c r="C2837" s="1">
+        <v>45205</v>
+      </c>
+    </row>
+    <row r="2838" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2838">
+        <v>2023</v>
+      </c>
+      <c r="B2838">
+        <v>280</v>
+      </c>
+      <c r="C2838" s="1">
+        <v>45206</v>
+      </c>
+    </row>
+    <row r="2839" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2839">
+        <v>2023</v>
+      </c>
+      <c r="B2839">
+        <v>281</v>
+      </c>
+      <c r="C2839" s="1">
+        <v>45207</v>
+      </c>
+    </row>
+    <row r="2840" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2840">
+        <v>2023</v>
+      </c>
+      <c r="B2840">
+        <v>282</v>
+      </c>
+      <c r="C2840" s="1">
+        <v>45208</v>
+      </c>
+    </row>
+    <row r="2841" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2841">
+        <v>2023</v>
+      </c>
+      <c r="B2841">
+        <v>283</v>
+      </c>
+      <c r="C2841" s="1">
+        <v>45209</v>
+      </c>
+    </row>
+    <row r="2842" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2842">
+        <v>2023</v>
+      </c>
+      <c r="B2842">
+        <v>284</v>
+      </c>
+      <c r="C2842" s="1">
+        <v>45210</v>
+      </c>
+    </row>
+    <row r="2843" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2843">
+        <v>2023</v>
+      </c>
+      <c r="B2843">
+        <v>285</v>
+      </c>
+      <c r="C2843" s="1">
+        <v>45211</v>
+      </c>
+    </row>
+    <row r="2844" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2844">
+        <v>2023</v>
+      </c>
+      <c r="B2844">
+        <v>286</v>
+      </c>
+      <c r="C2844" s="1">
+        <v>45212</v>
+      </c>
+    </row>
+    <row r="2845" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2845">
+        <v>2023</v>
+      </c>
+      <c r="B2845">
+        <v>287</v>
+      </c>
+      <c r="C2845" s="1">
+        <v>45213</v>
+      </c>
+    </row>
+    <row r="2846" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2846">
+        <v>2023</v>
+      </c>
+      <c r="B2846">
+        <v>288</v>
+      </c>
+      <c r="C2846" s="1">
+        <v>45214</v>
+      </c>
+    </row>
+    <row r="2847" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2847">
+        <v>2023</v>
+      </c>
+      <c r="B2847">
+        <v>289</v>
+      </c>
+      <c r="C2847" s="1">
+        <v>45215</v>
+      </c>
+    </row>
+    <row r="2848" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2848">
+        <v>2023</v>
+      </c>
+      <c r="B2848">
+        <v>290</v>
+      </c>
+      <c r="C2848" s="1">
+        <v>45216</v>
+      </c>
+    </row>
+    <row r="2849" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2849">
+        <v>2023</v>
+      </c>
+      <c r="B2849">
+        <v>291</v>
+      </c>
+      <c r="C2849" s="1">
+        <v>45217</v>
+      </c>
+    </row>
+    <row r="2850" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2850">
+        <v>2023</v>
+      </c>
+      <c r="B2850">
+        <v>292</v>
+      </c>
+      <c r="C2850" s="1">
+        <v>45218</v>
+      </c>
+    </row>
+    <row r="2851" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2851">
+        <v>2023</v>
+      </c>
+      <c r="B2851">
+        <v>293</v>
+      </c>
+      <c r="C2851" s="1">
+        <v>45219</v>
+      </c>
+    </row>
+    <row r="2852" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2852">
+        <v>2023</v>
+      </c>
+      <c r="B2852">
+        <v>294</v>
+      </c>
+      <c r="C2852" s="1">
+        <v>45220</v>
+      </c>
+    </row>
+    <row r="2853" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2853">
+        <v>2023</v>
+      </c>
+      <c r="B2853">
+        <v>295</v>
+      </c>
+      <c r="C2853" s="1">
+        <v>45221</v>
+      </c>
+    </row>
+    <row r="2854" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2854">
+        <v>2023</v>
+      </c>
+      <c r="B2854">
+        <v>296</v>
+      </c>
+      <c r="C2854" s="1">
+        <v>45222</v>
+      </c>
+    </row>
+    <row r="2855" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2855">
+        <v>2023</v>
+      </c>
+      <c r="B2855">
+        <v>297</v>
+      </c>
+      <c r="C2855" s="1">
+        <v>45223</v>
+      </c>
+    </row>
+    <row r="2856" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2856">
+        <v>2023</v>
+      </c>
+      <c r="B2856">
+        <v>298</v>
+      </c>
+      <c r="C2856" s="1">
+        <v>45224</v>
+      </c>
+    </row>
+    <row r="2857" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2857">
+        <v>2023</v>
+      </c>
+      <c r="B2857">
+        <v>299</v>
+      </c>
+      <c r="C2857" s="1">
+        <v>45225</v>
+      </c>
+    </row>
+    <row r="2858" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2858">
+        <v>2023</v>
+      </c>
+      <c r="B2858">
+        <v>300</v>
+      </c>
+      <c r="C2858" s="1">
+        <v>45226</v>
+      </c>
+    </row>
+    <row r="2859" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2859">
+        <v>2023</v>
+      </c>
+      <c r="B2859">
+        <v>301</v>
+      </c>
+      <c r="C2859" s="1">
+        <v>45227</v>
+      </c>
+    </row>
+    <row r="2860" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2860">
+        <v>2023</v>
+      </c>
+      <c r="B2860">
+        <v>302</v>
+      </c>
+      <c r="C2860" s="1">
+        <v>45228</v>
+      </c>
+    </row>
+    <row r="2861" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2861">
+        <v>2023</v>
+      </c>
+      <c r="B2861">
+        <v>303</v>
+      </c>
+      <c r="C2861" s="1">
+        <v>45229</v>
+      </c>
+    </row>
+    <row r="2862" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2862">
+        <v>2023</v>
+      </c>
+      <c r="B2862">
+        <v>304</v>
+      </c>
+      <c r="C2862" s="1">
+        <v>45230</v>
+      </c>
+    </row>
+    <row r="2863" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2863">
+        <v>2023</v>
+      </c>
+      <c r="B2863">
+        <v>305</v>
+      </c>
+      <c r="C2863" s="1">
+        <v>45231</v>
+      </c>
+    </row>
+    <row r="2864" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2864">
+        <v>2023</v>
+      </c>
+      <c r="B2864">
+        <v>306</v>
+      </c>
+      <c r="C2864" s="1">
+        <v>45232</v>
+      </c>
+    </row>
+    <row r="2865" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2865">
+        <v>2023</v>
+      </c>
+      <c r="B2865">
+        <v>307</v>
+      </c>
+      <c r="C2865" s="1">
+        <v>45233</v>
+      </c>
+    </row>
+    <row r="2866" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2866">
+        <v>2023</v>
+      </c>
+      <c r="B2866">
+        <v>308</v>
+      </c>
+      <c r="C2866" s="1">
+        <v>45234</v>
+      </c>
+    </row>
+    <row r="2867" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2867">
+        <v>2023</v>
+      </c>
+      <c r="B2867">
+        <v>309</v>
+      </c>
+      <c r="C2867" s="1">
+        <v>45235</v>
+      </c>
+    </row>
+    <row r="2868" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2868">
+        <v>2023</v>
+      </c>
+      <c r="B2868">
+        <v>310</v>
+      </c>
+      <c r="C2868" s="1">
+        <v>45236</v>
+      </c>
+    </row>
+    <row r="2869" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2869">
+        <v>2023</v>
+      </c>
+      <c r="B2869">
+        <v>311</v>
+      </c>
+      <c r="C2869" s="1">
+        <v>45237</v>
+      </c>
+    </row>
+    <row r="2870" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2870">
+        <v>2023</v>
+      </c>
+      <c r="B2870">
+        <v>312</v>
+      </c>
+      <c r="C2870" s="1">
+        <v>45238</v>
+      </c>
+    </row>
+    <row r="2871" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2871">
+        <v>2023</v>
+      </c>
+      <c r="B2871">
+        <v>313</v>
+      </c>
+      <c r="C2871" s="1">
+        <v>45239</v>
+      </c>
+    </row>
+    <row r="2872" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2872">
+        <v>2023</v>
+      </c>
+      <c r="B2872">
+        <v>314</v>
+      </c>
+      <c r="C2872" s="1">
+        <v>45240</v>
+      </c>
+    </row>
+    <row r="2873" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2873">
+        <v>2023</v>
+      </c>
+      <c r="B2873">
+        <v>315</v>
+      </c>
+      <c r="C2873" s="1">
+        <v>45241</v>
+      </c>
+    </row>
+    <row r="2874" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2874">
+        <v>2023</v>
+      </c>
+      <c r="B2874">
+        <v>316</v>
+      </c>
+      <c r="C2874" s="1">
+        <v>45242</v>
+      </c>
+    </row>
+    <row r="2875" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2875">
+        <v>2023</v>
+      </c>
+      <c r="B2875">
+        <v>317</v>
+      </c>
+      <c r="C2875" s="1">
+        <v>45243</v>
+      </c>
+    </row>
+    <row r="2876" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2876">
+        <v>2023</v>
+      </c>
+      <c r="B2876">
+        <v>318</v>
+      </c>
+      <c r="C2876" s="1">
+        <v>45244</v>
+      </c>
+    </row>
+    <row r="2877" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2877">
+        <v>2023</v>
+      </c>
+      <c r="B2877">
+        <v>319</v>
+      </c>
+      <c r="C2877" s="1">
+        <v>45245</v>
+      </c>
+    </row>
+    <row r="2878" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2878">
+        <v>2023</v>
+      </c>
+      <c r="B2878">
+        <v>320</v>
+      </c>
+      <c r="C2878" s="1">
+        <v>45246</v>
+      </c>
+    </row>
+    <row r="2879" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2879">
+        <v>2023</v>
+      </c>
+      <c r="B2879">
+        <v>321</v>
+      </c>
+      <c r="C2879" s="1">
+        <v>45247</v>
+      </c>
+    </row>
+    <row r="2880" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2880">
+        <v>2023</v>
+      </c>
+      <c r="B2880">
+        <v>322</v>
+      </c>
+      <c r="C2880" s="1">
+        <v>45248</v>
+      </c>
+    </row>
+    <row r="2881" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2881">
+        <v>2023</v>
+      </c>
+      <c r="B2881">
+        <v>323</v>
+      </c>
+      <c r="C2881" s="1">
+        <v>45249</v>
+      </c>
+    </row>
+    <row r="2882" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2882">
+        <v>2023</v>
+      </c>
+      <c r="B2882">
+        <v>324</v>
+      </c>
+      <c r="C2882" s="1">
+        <v>45250</v>
+      </c>
+    </row>
+    <row r="2883" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2883">
+        <v>2023</v>
+      </c>
+      <c r="B2883">
+        <v>325</v>
+      </c>
+      <c r="C2883" s="1">
+        <v>45251</v>
+      </c>
+    </row>
+    <row r="2884" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2884">
+        <v>2023</v>
+      </c>
+      <c r="B2884">
+        <v>326</v>
+      </c>
+      <c r="C2884" s="1">
+        <v>45252</v>
+      </c>
+    </row>
+    <row r="2885" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2885">
+        <v>2023</v>
+      </c>
+      <c r="B2885">
+        <v>327</v>
+      </c>
+      <c r="C2885" s="1">
+        <v>45253</v>
+      </c>
+    </row>
+    <row r="2886" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2886">
+        <v>2023</v>
+      </c>
+      <c r="B2886">
+        <v>328</v>
+      </c>
+      <c r="C2886" s="1">
+        <v>45254</v>
+      </c>
+    </row>
+    <row r="2887" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2887">
+        <v>2023</v>
+      </c>
+      <c r="B2887">
+        <v>329</v>
+      </c>
+      <c r="C2887" s="1">
+        <v>45255</v>
+      </c>
+    </row>
+    <row r="2888" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2888">
+        <v>2023</v>
+      </c>
+      <c r="B2888">
+        <v>330</v>
+      </c>
+      <c r="C2888" s="1">
+        <v>45256</v>
+      </c>
+    </row>
+    <row r="2889" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2889">
+        <v>2023</v>
+      </c>
+      <c r="B2889">
+        <v>331</v>
+      </c>
+      <c r="C2889" s="1">
+        <v>45257</v>
+      </c>
+    </row>
+    <row r="2890" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2890">
+        <v>2023</v>
+      </c>
+      <c r="B2890">
+        <v>332</v>
+      </c>
+      <c r="C2890" s="1">
+        <v>45258</v>
+      </c>
+    </row>
+    <row r="2891" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2891">
+        <v>2023</v>
+      </c>
+      <c r="B2891">
+        <v>333</v>
+      </c>
+      <c r="C2891" s="1">
+        <v>45259</v>
+      </c>
+    </row>
+    <row r="2892" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2892">
+        <v>2023</v>
+      </c>
+      <c r="B2892">
+        <v>334</v>
+      </c>
+      <c r="C2892" s="1">
+        <v>45260</v>
+      </c>
+    </row>
+    <row r="2893" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2893">
+        <v>2023</v>
+      </c>
+      <c r="B2893">
+        <v>335</v>
+      </c>
+      <c r="C2893" s="1">
+        <v>45261</v>
+      </c>
+    </row>
+    <row r="2894" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2894">
+        <v>2023</v>
+      </c>
+      <c r="B2894">
+        <v>336</v>
+      </c>
+      <c r="C2894" s="1">
+        <v>45262</v>
+      </c>
+    </row>
+    <row r="2895" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2895">
+        <v>2023</v>
+      </c>
+      <c r="B2895">
+        <v>337</v>
+      </c>
+      <c r="C2895" s="1">
+        <v>45263</v>
+      </c>
+    </row>
+    <row r="2896" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2896">
+        <v>2023</v>
+      </c>
+      <c r="B2896">
+        <v>338</v>
+      </c>
+      <c r="C2896" s="1">
+        <v>45264</v>
+      </c>
+    </row>
+    <row r="2897" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2897">
+        <v>2023</v>
+      </c>
+      <c r="B2897">
+        <v>339</v>
+      </c>
+      <c r="C2897" s="1">
+        <v>45265</v>
+      </c>
+    </row>
+    <row r="2898" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2898">
+        <v>2023</v>
+      </c>
+      <c r="B2898">
+        <v>340</v>
+      </c>
+      <c r="C2898" s="1">
+        <v>45266</v>
+      </c>
+    </row>
+    <row r="2899" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2899">
+        <v>2023</v>
+      </c>
+      <c r="B2899">
+        <v>341</v>
+      </c>
+      <c r="C2899" s="1">
+        <v>45267</v>
+      </c>
+    </row>
+    <row r="2900" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2900">
+        <v>2023</v>
+      </c>
+      <c r="B2900">
+        <v>342</v>
+      </c>
+      <c r="C2900" s="1">
+        <v>45268</v>
+      </c>
+    </row>
+    <row r="2901" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2901">
+        <v>2023</v>
+      </c>
+      <c r="B2901">
+        <v>343</v>
+      </c>
+      <c r="C2901" s="1">
+        <v>45269</v>
+      </c>
+    </row>
+    <row r="2902" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2902">
+        <v>2023</v>
+      </c>
+      <c r="B2902">
+        <v>344</v>
+      </c>
+      <c r="C2902" s="1">
+        <v>45270</v>
+      </c>
+    </row>
+    <row r="2903" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2903">
+        <v>2023</v>
+      </c>
+      <c r="B2903">
+        <v>345</v>
+      </c>
+      <c r="C2903" s="1">
+        <v>45271</v>
+      </c>
+    </row>
+    <row r="2904" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2904">
+        <v>2023</v>
+      </c>
+      <c r="B2904">
+        <v>346</v>
+      </c>
+      <c r="C2904" s="1">
+        <v>45272</v>
+      </c>
+    </row>
+    <row r="2905" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2905">
+        <v>2023</v>
+      </c>
+      <c r="B2905">
+        <v>347</v>
+      </c>
+      <c r="C2905" s="1">
+        <v>45273</v>
+      </c>
+    </row>
+    <row r="2906" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2906">
+        <v>2023</v>
+      </c>
+      <c r="B2906">
+        <v>348</v>
+      </c>
+      <c r="C2906" s="1">
+        <v>45274</v>
+      </c>
+    </row>
+    <row r="2907" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2907">
+        <v>2023</v>
+      </c>
+      <c r="B2907">
+        <v>349</v>
+      </c>
+      <c r="C2907" s="1">
+        <v>45275</v>
+      </c>
+    </row>
+    <row r="2908" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2908">
+        <v>2023</v>
+      </c>
+      <c r="B2908">
+        <v>350</v>
+      </c>
+      <c r="C2908" s="1">
+        <v>45276</v>
+      </c>
+    </row>
+    <row r="2909" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2909">
+        <v>2023</v>
+      </c>
+      <c r="B2909">
+        <v>351</v>
+      </c>
+      <c r="C2909" s="1">
+        <v>45277</v>
+      </c>
+    </row>
+    <row r="2910" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2910">
+        <v>2023</v>
+      </c>
+      <c r="B2910">
+        <v>352</v>
+      </c>
+      <c r="C2910" s="1">
+        <v>45278</v>
+      </c>
+    </row>
+    <row r="2911" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2911">
+        <v>2023</v>
+      </c>
+      <c r="B2911">
+        <v>353</v>
+      </c>
+      <c r="C2911" s="1">
+        <v>45279</v>
+      </c>
+    </row>
+    <row r="2912" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2912">
+        <v>2023</v>
+      </c>
+      <c r="B2912">
+        <v>354</v>
+      </c>
+      <c r="C2912" s="1">
+        <v>45280</v>
+      </c>
+    </row>
+    <row r="2913" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2913">
+        <v>2023</v>
+      </c>
+      <c r="B2913">
+        <v>355</v>
+      </c>
+      <c r="C2913" s="1">
+        <v>45281</v>
+      </c>
+    </row>
+    <row r="2914" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2914">
+        <v>2023</v>
+      </c>
+      <c r="B2914">
+        <v>356</v>
+      </c>
+      <c r="C2914" s="1">
+        <v>45282</v>
+      </c>
+    </row>
+    <row r="2915" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2915">
+        <v>2023</v>
+      </c>
+      <c r="B2915">
+        <v>357</v>
+      </c>
+      <c r="C2915" s="1">
+        <v>45283</v>
+      </c>
+    </row>
+    <row r="2916" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2916">
+        <v>2023</v>
+      </c>
+      <c r="B2916">
+        <v>358</v>
+      </c>
+      <c r="C2916" s="1">
+        <v>45284</v>
+      </c>
+    </row>
+    <row r="2917" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2917">
+        <v>2023</v>
+      </c>
+      <c r="B2917">
+        <v>359</v>
+      </c>
+      <c r="C2917" s="1">
+        <v>45285</v>
+      </c>
+    </row>
+    <row r="2918" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2918">
+        <v>2023</v>
+      </c>
+      <c r="B2918">
+        <v>360</v>
+      </c>
+      <c r="C2918" s="1">
+        <v>45286</v>
+      </c>
+    </row>
+    <row r="2919" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2919">
+        <v>2023</v>
+      </c>
+      <c r="B2919">
+        <v>361</v>
+      </c>
+      <c r="C2919" s="1">
+        <v>45287</v>
+      </c>
+    </row>
+    <row r="2920" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2920">
+        <v>2023</v>
+      </c>
+      <c r="B2920">
+        <v>362</v>
+      </c>
+      <c r="C2920" s="1">
+        <v>45288</v>
+      </c>
+    </row>
+    <row r="2921" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2921">
+        <v>2023</v>
+      </c>
+      <c r="B2921">
+        <v>363</v>
+      </c>
+      <c r="C2921" s="1">
+        <v>45289</v>
+      </c>
+    </row>
+    <row r="2922" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2922">
+        <v>2023</v>
+      </c>
+      <c r="B2922">
+        <v>364</v>
+      </c>
+      <c r="C2922" s="1">
+        <v>45290</v>
+      </c>
+    </row>
+    <row r="2923" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2923">
+        <v>2023</v>
+      </c>
+      <c r="B2923">
+        <v>365</v>
+      </c>
+      <c r="C2923" s="1">
+        <v>45291</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>